<commit_message>
antes de codigo omar
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10995" tabRatio="789" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10995" tabRatio="789" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="NOMINA TOTAL" sheetId="27" r:id="rId1"/>
@@ -18,21 +18,23 @@
     <sheet name="DETALLE" sheetId="28" r:id="rId4"/>
     <sheet name="Hoja1" sheetId="31" r:id="rId5"/>
     <sheet name="FACT" sheetId="30" r:id="rId6"/>
+    <sheet name="PENSION ALIMENTICIA" sheetId="32" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="__TC1">[1]FOR!$B$9</definedName>
     <definedName name="__TC2">[1]FOR!$B$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'OPERADORA ABORDO'!$A$3:$W$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'OPERADORA DESCANSO'!$A$3:$W$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'PENSION ALIMENTICIA'!$B$1:$G$1</definedName>
     <definedName name="_TC1">[2]FOR!$B$9</definedName>
     <definedName name="_TC2">[2]FOR!$B$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">DETALLE!$A$1:$K$54</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'OPERADORA ABORDO'!$A$1:$AO$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'OPERADORA ABORDO'!$A$1:$AP$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'OPERADORA DESCANSO'!$A$1:$AN$19</definedName>
     <definedName name="LICS">[3]FOR!$F$59:$F$71</definedName>
     <definedName name="LIIMP">[3]FOR!$F$36:$F$40</definedName>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="122">
   <si>
     <t>SUBTOTAL</t>
   </si>
@@ -409,6 +411,27 @@
   <si>
     <t>SUBSEA 88</t>
   </si>
+  <si>
+    <t>FONACOT</t>
+  </si>
+  <si>
+    <t>NOMBRE TRABAJADOR</t>
+  </si>
+  <si>
+    <t>NOMBRE BENFICIARIO</t>
+  </si>
+  <si>
+    <t>PORCENTAJE</t>
+  </si>
+  <si>
+    <t>MONTO ABORDO</t>
+  </si>
+  <si>
+    <t>MONTO DESCANSO</t>
+  </si>
+  <si>
+    <t>SUBSEA88</t>
+  </si>
 </sst>
 </file>
 
@@ -421,7 +444,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;???_-;_-@_-"/>
   </numFmts>
-  <fonts count="41" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -680,6 +703,13 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -2408,7 +2438,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2674,32 +2704,12 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1113" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1113" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1113" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1113" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1113" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="34" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="17" fontId="27" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2788,7 +2798,35 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1488" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1490" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="43" fontId="41" fillId="0" borderId="0" xfId="1490" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="43" fontId="41" fillId="0" borderId="0" xfId="1488" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="1" xfId="1318" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="33" fillId="0" borderId="0" xfId="1488" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1113" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1113" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1113" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1113" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1113" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="17" fontId="27" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4310,8 +4348,8 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>87842</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>151342</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>27517</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5083,11 +5121,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:BE12"/>
+  <dimension ref="B1:BG12"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="Q1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P13" sqref="P13"/>
+      <selection pane="bottomLeft" activeCell="Q10" sqref="A1:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5107,21 +5145,21 @@
     <col min="13" max="13" width="13.5703125" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.28515625" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" customWidth="1"/>
-    <col min="18" max="18" width="17" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="1.85546875" customWidth="1"/>
-    <col min="22" max="22" width="15.42578125" customWidth="1"/>
-    <col min="23" max="23" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="18.28515625" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" customWidth="1"/>
+    <col min="20" max="20" width="17" customWidth="1"/>
+    <col min="21" max="21" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="1.85546875" customWidth="1"/>
+    <col min="24" max="24" width="15.42578125" customWidth="1"/>
+    <col min="25" max="25" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.140625" customWidth="1"/>
+    <col min="27" max="27" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:57" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:59" s="1" customFormat="1" ht="13.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -5138,18 +5176,17 @@
       <c r="O1" s="4"/>
       <c r="P1" s="13"/>
       <c r="Q1" s="13"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
       <c r="V1" s="7"/>
       <c r="W1" s="7"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
       <c r="Z1" s="3"/>
-      <c r="AB1" s="50"/>
-      <c r="AC1" s="50"/>
-      <c r="AD1" s="50"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
       <c r="AE1" s="50"/>
       <c r="AF1" s="50"/>
       <c r="AG1" s="50"/>
@@ -5177,8 +5214,10 @@
       <c r="BC1" s="50"/>
       <c r="BD1" s="50"/>
       <c r="BE1" s="50"/>
-    </row>
-    <row r="2" spans="2:57" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="BF1" s="50"/>
+      <c r="BG1" s="50"/>
+    </row>
+    <row r="2" spans="2:59" s="1" customFormat="1" ht="13.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
@@ -5204,12 +5243,12 @@
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
       <c r="AA2" s="6"/>
-      <c r="AB2" s="50"/>
-      <c r="AC2" s="50"/>
-      <c r="AD2" s="50"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
       <c r="AE2" s="50"/>
       <c r="AF2" s="50"/>
       <c r="AG2" s="50"/>
@@ -5237,8 +5276,10 @@
       <c r="BC2" s="50"/>
       <c r="BD2" s="50"/>
       <c r="BE2" s="50"/>
-    </row>
-    <row r="3" spans="2:57" s="43" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="BF2" s="50"/>
+      <c r="BG2" s="50"/>
+    </row>
+    <row r="3" spans="2:59" s="43" customFormat="1" ht="13.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
       <c r="D3" s="41"/>
@@ -5262,12 +5303,12 @@
       <c r="V3" s="42"/>
       <c r="W3" s="42"/>
       <c r="X3" s="42"/>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="41"/>
+      <c r="Y3" s="42"/>
+      <c r="Z3" s="42"/>
       <c r="AA3" s="41"/>
-      <c r="AB3" s="50"/>
-      <c r="AC3" s="50"/>
-      <c r="AD3" s="50"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="41"/>
+      <c r="AD3" s="41"/>
       <c r="AE3" s="50"/>
       <c r="AF3" s="50"/>
       <c r="AG3" s="50"/>
@@ -5295,8 +5336,10 @@
       <c r="BC3" s="50"/>
       <c r="BD3" s="50"/>
       <c r="BE3" s="50"/>
-    </row>
-    <row r="4" spans="2:57" s="43" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="BF3" s="50"/>
+      <c r="BG3" s="50"/>
+    </row>
+    <row r="4" spans="2:59" s="43" customFormat="1" ht="13.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
       <c r="D4" s="41"/>
@@ -5312,20 +5355,20 @@
       <c r="N4" s="42"/>
       <c r="O4" s="42"/>
       <c r="P4" s="42"/>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="60"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="42"/>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="42"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
       <c r="U4" s="42"/>
       <c r="V4" s="42"/>
       <c r="W4" s="42"/>
       <c r="X4" s="42"/>
-      <c r="Y4" s="41"/>
-      <c r="Z4" s="41"/>
+      <c r="Y4" s="42"/>
+      <c r="Z4" s="42"/>
       <c r="AA4" s="41"/>
-      <c r="AB4" s="50"/>
-      <c r="AC4" s="50"/>
-      <c r="AD4" s="50"/>
+      <c r="AB4" s="41"/>
+      <c r="AC4" s="41"/>
+      <c r="AD4" s="41"/>
       <c r="AE4" s="50"/>
       <c r="AF4" s="50"/>
       <c r="AG4" s="50"/>
@@ -5353,8 +5396,10 @@
       <c r="BC4" s="50"/>
       <c r="BD4" s="50"/>
       <c r="BE4" s="50"/>
-    </row>
-    <row r="5" spans="2:57" s="43" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="BF4" s="50"/>
+      <c r="BG4" s="50"/>
+    </row>
+    <row r="5" spans="2:59" s="43" customFormat="1" ht="13.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
       <c r="D5" s="41"/>
@@ -5370,20 +5415,20 @@
       <c r="N5" s="42"/>
       <c r="O5" s="42"/>
       <c r="P5" s="42"/>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
       <c r="U5" s="42"/>
       <c r="V5" s="42"/>
       <c r="W5" s="42"/>
       <c r="X5" s="42"/>
-      <c r="Y5" s="41"/>
-      <c r="Z5" s="41"/>
+      <c r="Y5" s="42"/>
+      <c r="Z5" s="42"/>
       <c r="AA5" s="41"/>
-      <c r="AB5" s="50"/>
-      <c r="AC5" s="50"/>
-      <c r="AD5" s="50"/>
+      <c r="AB5" s="41"/>
+      <c r="AC5" s="41"/>
+      <c r="AD5" s="41"/>
       <c r="AE5" s="50"/>
       <c r="AF5" s="50"/>
       <c r="AG5" s="50"/>
@@ -5411,8 +5456,10 @@
       <c r="BC5" s="50"/>
       <c r="BD5" s="50"/>
       <c r="BE5" s="50"/>
-    </row>
-    <row r="6" spans="2:57" s="43" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="BF5" s="50"/>
+      <c r="BG5" s="50"/>
+    </row>
+    <row r="6" spans="2:59" s="43" customFormat="1" ht="13.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
@@ -5430,18 +5477,18 @@
       <c r="P6" s="60"/>
       <c r="Q6" s="60"/>
       <c r="R6" s="60"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
+      <c r="S6" s="60"/>
+      <c r="T6" s="60"/>
       <c r="U6" s="42"/>
       <c r="V6" s="42"/>
       <c r="W6" s="42"/>
       <c r="X6" s="42"/>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="41"/>
+      <c r="Y6" s="42"/>
+      <c r="Z6" s="42"/>
       <c r="AA6" s="41"/>
-      <c r="AB6" s="50"/>
-      <c r="AC6" s="50"/>
-      <c r="AD6" s="50"/>
+      <c r="AB6" s="41"/>
+      <c r="AC6" s="41"/>
+      <c r="AD6" s="41"/>
       <c r="AE6" s="50"/>
       <c r="AF6" s="50"/>
       <c r="AG6" s="50"/>
@@ -5469,8 +5516,10 @@
       <c r="BC6" s="50"/>
       <c r="BD6" s="50"/>
       <c r="BE6" s="50"/>
-    </row>
-    <row r="7" spans="2:57" s="43" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="BF6" s="50"/>
+      <c r="BG6" s="50"/>
+    </row>
+    <row r="7" spans="2:59" s="43" customFormat="1" ht="13.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="41"/>
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
@@ -5488,18 +5537,18 @@
       <c r="P7" s="61"/>
       <c r="Q7" s="61"/>
       <c r="R7" s="61"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
+      <c r="S7" s="61"/>
+      <c r="T7" s="61"/>
       <c r="U7" s="42"/>
       <c r="V7" s="42"/>
       <c r="W7" s="42"/>
       <c r="X7" s="42"/>
-      <c r="Y7" s="41"/>
-      <c r="Z7" s="41"/>
+      <c r="Y7" s="42"/>
+      <c r="Z7" s="42"/>
       <c r="AA7" s="41"/>
-      <c r="AB7" s="50"/>
-      <c r="AC7" s="50"/>
-      <c r="AD7" s="50"/>
+      <c r="AB7" s="41"/>
+      <c r="AC7" s="41"/>
+      <c r="AD7" s="41"/>
       <c r="AE7" s="50"/>
       <c r="AF7" s="50"/>
       <c r="AG7" s="50"/>
@@ -5527,8 +5576,10 @@
       <c r="BC7" s="50"/>
       <c r="BD7" s="50"/>
       <c r="BE7" s="50"/>
-    </row>
-    <row r="8" spans="2:57" s="43" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="BF7" s="50"/>
+      <c r="BG7" s="50"/>
+    </row>
+    <row r="8" spans="2:59" s="43" customFormat="1" ht="13.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
       <c r="D8" s="41"/>
@@ -5544,20 +5595,20 @@
       <c r="N8" s="60"/>
       <c r="O8" s="61"/>
       <c r="P8" s="105"/>
-      <c r="Q8" s="61"/>
-      <c r="R8" s="60"/>
-      <c r="S8" s="60"/>
+      <c r="Q8" s="105"/>
+      <c r="R8" s="105"/>
+      <c r="S8" s="61"/>
       <c r="T8" s="60"/>
       <c r="U8" s="60"/>
       <c r="V8" s="60"/>
       <c r="W8" s="60"/>
       <c r="X8" s="60"/>
-      <c r="Y8" s="111"/>
-      <c r="Z8" s="111"/>
+      <c r="Y8" s="60"/>
+      <c r="Z8" s="60"/>
       <c r="AA8" s="111"/>
-      <c r="AB8" s="50"/>
-      <c r="AC8" s="50"/>
-      <c r="AD8" s="50"/>
+      <c r="AB8" s="111"/>
+      <c r="AC8" s="111"/>
+      <c r="AD8" s="111"/>
       <c r="AE8" s="50"/>
       <c r="AF8" s="50"/>
       <c r="AG8" s="50"/>
@@ -5585,8 +5636,10 @@
       <c r="BC8" s="50"/>
       <c r="BD8" s="50"/>
       <c r="BE8" s="50"/>
-    </row>
-    <row r="9" spans="2:57" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="BF8" s="50"/>
+      <c r="BG8" s="50"/>
+    </row>
+    <row r="9" spans="2:59" s="1" customFormat="1" ht="13.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -5602,9 +5655,9 @@
       <c r="N9" s="4"/>
       <c r="O9" s="62"/>
       <c r="P9" s="62"/>
-      <c r="Q9" s="112"/>
-      <c r="R9" s="44"/>
-      <c r="S9" s="44"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="112"/>
       <c r="T9" s="44"/>
       <c r="U9" s="44"/>
       <c r="V9" s="44"/>
@@ -5613,9 +5666,9 @@
       <c r="Y9" s="44"/>
       <c r="Z9" s="44"/>
       <c r="AA9" s="44"/>
-      <c r="AB9" s="50"/>
-      <c r="AC9" s="50"/>
-      <c r="AD9" s="50"/>
+      <c r="AB9" s="44"/>
+      <c r="AC9" s="44"/>
+      <c r="AD9" s="44"/>
       <c r="AE9" s="50"/>
       <c r="AF9" s="50"/>
       <c r="AG9" s="50"/>
@@ -5643,8 +5696,10 @@
       <c r="BC9" s="50"/>
       <c r="BD9" s="50"/>
       <c r="BE9" s="50"/>
-    </row>
-    <row r="10" spans="2:57" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="BF9" s="50"/>
+      <c r="BG9" s="50"/>
+    </row>
+    <row r="10" spans="2:59" s="1" customFormat="1" ht="13.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="114"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -5660,9 +5715,9 @@
       <c r="N10" s="4"/>
       <c r="O10" s="62"/>
       <c r="P10" s="62"/>
-      <c r="Q10" s="112"/>
-      <c r="R10" s="44"/>
-      <c r="S10" s="44"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="112"/>
       <c r="T10" s="44"/>
       <c r="U10" s="44"/>
       <c r="V10" s="44"/>
@@ -5671,9 +5726,9 @@
       <c r="Y10" s="44"/>
       <c r="Z10" s="44"/>
       <c r="AA10" s="44"/>
-      <c r="AB10" s="50"/>
-      <c r="AC10" s="50"/>
-      <c r="AD10" s="50"/>
+      <c r="AB10" s="44"/>
+      <c r="AC10" s="44"/>
+      <c r="AD10" s="44"/>
       <c r="AE10" s="50"/>
       <c r="AF10" s="50"/>
       <c r="AG10" s="50"/>
@@ -5701,85 +5756,87 @@
       <c r="BC10" s="50"/>
       <c r="BD10" s="50"/>
       <c r="BE10" s="50"/>
-    </row>
-    <row r="11" spans="2:57" s="85" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="132" t="s">
+      <c r="BF10" s="50"/>
+      <c r="BG10" s="50"/>
+    </row>
+    <row r="11" spans="2:59" s="85" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="132" t="s">
+      <c r="C11" s="179" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="132" t="s">
+      <c r="D11" s="179" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="132" t="s">
+      <c r="E11" s="179" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="132" t="s">
+      <c r="F11" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="132" t="s">
+      <c r="G11" s="179" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="132" t="s">
+      <c r="H11" s="179" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="132" t="s">
+      <c r="I11" s="179" t="s">
         <v>71</v>
       </c>
-      <c r="J11" s="132" t="s">
+      <c r="J11" s="179" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="132" t="s">
+      <c r="K11" s="179" t="s">
         <v>59</v>
       </c>
-      <c r="L11" s="132" t="s">
+      <c r="L11" s="179" t="s">
         <v>4</v>
       </c>
-      <c r="M11" s="132" t="s">
+      <c r="M11" s="179" t="s">
         <v>62</v>
       </c>
-      <c r="N11" s="132" t="s">
+      <c r="N11" s="179" t="s">
         <v>72</v>
       </c>
       <c r="O11" s="129"/>
-      <c r="P11" s="132" t="s">
+      <c r="P11" s="179" t="s">
         <v>52</v>
       </c>
-      <c r="Q11" s="132" t="s">
+      <c r="Q11" s="132"/>
+      <c r="R11" s="132"/>
+      <c r="S11" s="179" t="s">
         <v>58</v>
       </c>
-      <c r="R11" s="132" t="s">
+      <c r="T11" s="179" t="s">
         <v>17</v>
       </c>
-      <c r="S11" s="132" t="s">
+      <c r="U11" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="T11" s="132" t="s">
+      <c r="V11" s="179" t="s">
         <v>73</v>
       </c>
-      <c r="U11" s="86"/>
-      <c r="V11" s="132" t="s">
+      <c r="W11" s="86"/>
+      <c r="X11" s="179" t="s">
         <v>74</v>
       </c>
-      <c r="W11" s="132" t="s">
+      <c r="Y11" s="179" t="s">
         <v>75</v>
       </c>
-      <c r="X11" s="132" t="s">
+      <c r="Z11" s="179" t="s">
         <v>5</v>
       </c>
-      <c r="Y11" s="132" t="s">
+      <c r="AA11" s="179" t="s">
         <v>0</v>
       </c>
-      <c r="Z11" s="133" t="s">
+      <c r="AB11" s="180" t="s">
         <v>20</v>
       </c>
-      <c r="AA11" s="132" t="s">
+      <c r="AC11" s="179" t="s">
         <v>1</v>
       </c>
-      <c r="AB11" s="132"/>
-      <c r="AD11" s="84"/>
-      <c r="AE11" s="84"/>
+      <c r="AD11" s="179"/>
       <c r="AF11" s="84"/>
       <c r="AG11" s="84"/>
       <c r="AH11" s="84"/>
@@ -5805,42 +5862,48 @@
       <c r="BB11" s="84"/>
       <c r="BC11" s="84"/>
       <c r="BD11" s="84"/>
-    </row>
-    <row r="12" spans="2:57" s="87" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="132"/>
-      <c r="C12" s="132"/>
-      <c r="D12" s="132"/>
-      <c r="E12" s="132"/>
-      <c r="F12" s="132"/>
-      <c r="G12" s="132"/>
-      <c r="H12" s="132"/>
-      <c r="I12" s="132"/>
-      <c r="J12" s="132"/>
-      <c r="K12" s="132"/>
-      <c r="L12" s="132"/>
-      <c r="M12" s="132"/>
-      <c r="N12" s="132"/>
+      <c r="BE11" s="84"/>
+      <c r="BF11" s="84"/>
+    </row>
+    <row r="12" spans="2:59" s="87" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="179"/>
+      <c r="C12" s="179"/>
+      <c r="D12" s="179"/>
+      <c r="E12" s="179"/>
+      <c r="F12" s="179"/>
+      <c r="G12" s="179"/>
+      <c r="H12" s="179"/>
+      <c r="I12" s="179"/>
+      <c r="J12" s="179"/>
+      <c r="K12" s="179"/>
+      <c r="L12" s="179"/>
+      <c r="M12" s="179"/>
+      <c r="N12" s="179"/>
       <c r="O12" s="129" t="s">
         <v>76</v>
       </c>
-      <c r="P12" s="132" t="s">
+      <c r="P12" s="179" t="s">
         <v>63</v>
       </c>
-      <c r="Q12" s="132"/>
-      <c r="R12" s="132"/>
-      <c r="S12" s="132"/>
-      <c r="T12" s="132"/>
-      <c r="U12" s="86"/>
-      <c r="V12" s="132"/>
-      <c r="W12" s="132"/>
-      <c r="X12" s="132"/>
-      <c r="Y12" s="132"/>
-      <c r="Z12" s="133"/>
-      <c r="AA12" s="132"/>
-      <c r="AB12" s="132"/>
-      <c r="AC12" s="88"/>
-      <c r="AD12" s="89"/>
-      <c r="AE12" s="89"/>
+      <c r="Q12" s="132" t="s">
+        <v>66</v>
+      </c>
+      <c r="R12" s="132" t="s">
+        <v>115</v>
+      </c>
+      <c r="S12" s="179"/>
+      <c r="T12" s="179"/>
+      <c r="U12" s="179"/>
+      <c r="V12" s="179"/>
+      <c r="W12" s="86"/>
+      <c r="X12" s="179"/>
+      <c r="Y12" s="179"/>
+      <c r="Z12" s="179"/>
+      <c r="AA12" s="179"/>
+      <c r="AB12" s="180"/>
+      <c r="AC12" s="179"/>
+      <c r="AD12" s="179"/>
+      <c r="AE12" s="88"/>
       <c r="AF12" s="89"/>
       <c r="AG12" s="89"/>
       <c r="AH12" s="89"/>
@@ -5866,34 +5929,36 @@
       <c r="BB12" s="89"/>
       <c r="BC12" s="89"/>
       <c r="BD12" s="89"/>
+      <c r="BE12" s="89"/>
+      <c r="BF12" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="AB11:AB12"/>
-    <mergeCell ref="AA11:AA12"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="Z11:Z12"/>
+    <mergeCell ref="Y11:Y12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="AD11:AD12"/>
+    <mergeCell ref="AC11:AC12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="M11:M12"/>
-    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="V11:V12"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="N11:N12"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="AA11:AA12"/>
+    <mergeCell ref="AB11:AB12"/>
+    <mergeCell ref="P11:P12"/>
     <mergeCell ref="S11:S12"/>
-    <mergeCell ref="Y11:Y12"/>
-    <mergeCell ref="Z11:Z12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="V11:V12"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5902,10 +5967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:KA47"/>
+  <dimension ref="A1:KB47"/>
   <sheetViews>
-    <sheetView topLeftCell="AS1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AV1" sqref="AV1:AX1048576"/>
+    <sheetView topLeftCell="AM1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AQ8" sqref="AQ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5940,23 +6005,23 @@
     <col min="35" max="37" width="14.140625" customWidth="1"/>
     <col min="38" max="38" width="15.85546875" customWidth="1"/>
     <col min="39" max="39" width="12" customWidth="1"/>
-    <col min="40" max="40" width="13.42578125" customWidth="1"/>
-    <col min="41" max="46" width="14.28515625" customWidth="1"/>
-    <col min="47" max="47" width="12.28515625" customWidth="1"/>
-    <col min="48" max="50" width="0" style="10" hidden="1" customWidth="1"/>
-    <col min="51" max="55" width="11.42578125" style="10" customWidth="1"/>
-    <col min="56" max="56" width="16.85546875" customWidth="1"/>
+    <col min="40" max="41" width="13.42578125" customWidth="1"/>
+    <col min="42" max="47" width="14.28515625" customWidth="1"/>
+    <col min="48" max="48" width="12.28515625" customWidth="1"/>
+    <col min="49" max="51" width="0" style="10" hidden="1" customWidth="1"/>
+    <col min="52" max="56" width="11.42578125" style="10" customWidth="1"/>
+    <col min="57" max="57" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:287" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:288" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="27"/>
-      <c r="B1" s="134" t="s">
+      <c r="B1" s="181" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
       <c r="G1" s="65"/>
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
@@ -5997,9 +6062,10 @@
       <c r="AR1" s="24"/>
       <c r="AS1" s="24"/>
       <c r="AT1" s="24"/>
-      <c r="BC1"/>
-    </row>
-    <row r="2" spans="1:287" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU1" s="24"/>
+      <c r="BD1"/>
+    </row>
+    <row r="2" spans="1:288" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="51" t="s">
         <v>23</v>
@@ -6048,17 +6114,18 @@
       <c r="AR2" s="24"/>
       <c r="AS2" s="24"/>
       <c r="AT2" s="24"/>
-      <c r="BC2"/>
-    </row>
-    <row r="3" spans="1:287" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU2" s="24"/>
+      <c r="BD2"/>
+    </row>
+    <row r="3" spans="1:288" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
-      <c r="B3" s="136" t="s">
+      <c r="B3" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
       <c r="G3" s="67"/>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
@@ -6099,23 +6166,24 @@
       <c r="AR3" s="24"/>
       <c r="AS3" s="24"/>
       <c r="AT3" s="24"/>
-      <c r="AV3" s="110"/>
+      <c r="AU3" s="24"/>
       <c r="AW3" s="110"/>
       <c r="AX3" s="110"/>
       <c r="AY3" s="110"/>
       <c r="AZ3" s="110"/>
       <c r="BA3" s="110"/>
       <c r="BB3" s="110"/>
-    </row>
-    <row r="4" spans="1:287" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="BC3" s="110"/>
+    </row>
+    <row r="4" spans="1:288" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
-      <c r="B4" s="137" t="s">
+      <c r="B4" s="184" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="138"/>
-      <c r="D4" s="138"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="138"/>
+      <c r="C4" s="185"/>
+      <c r="D4" s="185"/>
+      <c r="E4" s="185"/>
+      <c r="F4" s="185"/>
       <c r="G4" s="67"/>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
@@ -6156,8 +6224,9 @@
       <c r="AR4" s="24"/>
       <c r="AS4" s="24"/>
       <c r="AT4" s="24"/>
-    </row>
-    <row r="5" spans="1:287" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AU4" s="24"/>
+    </row>
+    <row r="5" spans="1:288" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="29" t="s">
         <v>21</v>
@@ -6206,8 +6275,9 @@
       <c r="AR5" s="24"/>
       <c r="AS5" s="24"/>
       <c r="AT5" s="24"/>
-    </row>
-    <row r="6" spans="1:287" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AU5" s="24"/>
+    </row>
+    <row r="6" spans="1:288" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="29" t="s">
         <v>22</v>
@@ -6256,8 +6326,8 @@
       <c r="AR6" s="24"/>
       <c r="AS6" s="24"/>
       <c r="AT6" s="24"/>
-      <c r="AU6"/>
-      <c r="BC6"/>
+      <c r="AU6" s="24"/>
+      <c r="AV6"/>
       <c r="BD6"/>
       <c r="BE6"/>
       <c r="BF6"/>
@@ -6316,8 +6386,9 @@
       <c r="DG6"/>
       <c r="DH6"/>
       <c r="DI6"/>
-    </row>
-    <row r="7" spans="1:287" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="DJ6"/>
+    </row>
+    <row r="7" spans="1:288" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="68"/>
@@ -6345,7 +6416,6 @@
       <c r="Y7" s="16"/>
       <c r="Z7" s="16"/>
       <c r="AA7" s="18"/>
-      <c r="AU7" s="110"/>
       <c r="AV7" s="110"/>
       <c r="AW7" s="110"/>
       <c r="AX7" s="110"/>
@@ -6412,8 +6482,9 @@
       <c r="DG7" s="110"/>
       <c r="DH7" s="110"/>
       <c r="DI7" s="110"/>
-    </row>
-    <row r="8" spans="1:287" s="45" customFormat="1" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DJ7" s="110"/>
+    </row>
+    <row r="8" spans="1:288" s="45" customFormat="1" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
         <v>16</v>
       </c>
@@ -6534,37 +6605,39 @@
       <c r="AN8" s="128" t="s">
         <v>66</v>
       </c>
-      <c r="AO8" s="127" t="s">
+      <c r="AO8" s="128" t="s">
+        <v>115</v>
+      </c>
+      <c r="AP8" s="127" t="s">
         <v>53</v>
       </c>
-      <c r="AP8" s="130" t="s">
+      <c r="AQ8" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="AQ8" s="130" t="s">
+      <c r="AR8" s="130" t="s">
         <v>67</v>
       </c>
-      <c r="AR8" s="130" t="s">
+      <c r="AS8" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="AS8" s="130" t="s">
+      <c r="AT8" s="130" t="s">
         <v>68</v>
       </c>
-      <c r="AT8" s="131" t="s">
+      <c r="AU8" s="131" t="s">
         <v>69</v>
       </c>
-      <c r="AU8" s="130" t="s">
+      <c r="AV8" s="130" t="s">
         <v>70</v>
       </c>
-      <c r="AV8" s="128" t="s">
+      <c r="AW8" s="128" t="s">
         <v>99</v>
       </c>
-      <c r="AW8" s="128" t="s">
+      <c r="AX8" s="128" t="s">
         <v>100</v>
       </c>
-      <c r="AX8" s="128" t="s">
+      <c r="AY8" s="128" t="s">
         <v>101</v>
       </c>
-      <c r="AY8" s="10"/>
       <c r="AZ8" s="10"/>
       <c r="BA8" s="10"/>
       <c r="BB8" s="10"/>
@@ -6627,7 +6700,7 @@
       <c r="DG8" s="10"/>
       <c r="DH8" s="10"/>
       <c r="DI8" s="10"/>
-      <c r="DJ8" s="126"/>
+      <c r="DJ8" s="10"/>
       <c r="DK8" s="126"/>
       <c r="DL8" s="126"/>
       <c r="DM8" s="126"/>
@@ -6638,8 +6711,8 @@
       <c r="DR8" s="126"/>
       <c r="DS8" s="126"/>
       <c r="DT8" s="126"/>
-      <c r="DU8" s="125"/>
-      <c r="DV8" s="124"/>
+      <c r="DU8" s="126"/>
+      <c r="DV8" s="125"/>
       <c r="DW8" s="124"/>
       <c r="DX8" s="124"/>
       <c r="DY8" s="124"/>
@@ -6801,8 +6874,9 @@
       <c r="JY8" s="124"/>
       <c r="JZ8" s="124"/>
       <c r="KA8" s="124"/>
-    </row>
-    <row r="9" spans="1:287" s="79" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="KB8" s="124"/>
+    </row>
+    <row r="9" spans="1:288" s="79" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="49"/>
       <c r="B9" s="5"/>
       <c r="C9" s="74"/>
@@ -6833,15 +6907,15 @@
       <c r="AI9" s="83"/>
       <c r="AJ9" s="83"/>
       <c r="AK9" s="83"/>
-      <c r="AO9" s="83"/>
       <c r="AP9" s="83"/>
       <c r="AQ9" s="83"/>
       <c r="AR9" s="83"/>
       <c r="AS9" s="83"/>
       <c r="AT9" s="83"/>
       <c r="AU9" s="83"/>
-    </row>
-    <row r="10" spans="1:287" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV9" s="83"/>
+    </row>
+    <row r="10" spans="1:288" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="115"/>
       <c r="B10" s="116"/>
       <c r="C10" s="117"/>
@@ -6883,17 +6957,18 @@
       <c r="AM10" s="119"/>
       <c r="AN10" s="119"/>
       <c r="AO10" s="119"/>
-      <c r="AP10" s="48"/>
+      <c r="AP10" s="119"/>
       <c r="AQ10" s="48"/>
       <c r="AR10" s="48"/>
       <c r="AS10" s="48"/>
       <c r="AT10" s="48"/>
-      <c r="AU10" s="54"/>
-      <c r="AV10" s="79"/>
+      <c r="AU10" s="48"/>
+      <c r="AV10" s="54"/>
       <c r="AW10" s="79"/>
       <c r="AX10" s="79"/>
-    </row>
-    <row r="11" spans="1:287" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AY10" s="79"/>
+    </row>
+    <row r="11" spans="1:288" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="49"/>
       <c r="B11" s="5"/>
       <c r="C11" s="74"/>
@@ -6928,15 +7003,16 @@
       <c r="AL11" s="102"/>
       <c r="AM11" s="102"/>
       <c r="AN11" s="102"/>
-      <c r="AO11" s="103"/>
+      <c r="AO11" s="102"/>
       <c r="AP11" s="103"/>
       <c r="AQ11" s="103"/>
       <c r="AR11" s="103"/>
       <c r="AS11" s="103"/>
       <c r="AT11" s="103"/>
-      <c r="AU11" s="83"/>
-    </row>
-    <row r="12" spans="1:287" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AU11" s="103"/>
+      <c r="AV11" s="83"/>
+    </row>
+    <row r="12" spans="1:288" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="46"/>
       <c r="B12" s="38"/>
       <c r="C12" s="69"/>
@@ -6983,12 +7059,13 @@
       <c r="AR12" s="48"/>
       <c r="AS12" s="48"/>
       <c r="AT12" s="48"/>
-      <c r="AU12" s="54"/>
-      <c r="AV12" s="79"/>
+      <c r="AU12" s="48"/>
+      <c r="AV12" s="54"/>
       <c r="AW12" s="79"/>
       <c r="AX12" s="79"/>
-    </row>
-    <row r="13" spans="1:287" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AY12" s="79"/>
+    </row>
+    <row r="13" spans="1:288" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="46"/>
       <c r="B13" s="38"/>
       <c r="C13" s="69"/>
@@ -7035,11 +7112,12 @@
       <c r="AR13" s="48"/>
       <c r="AS13" s="48"/>
       <c r="AT13" s="48"/>
-      <c r="AV13" s="79"/>
+      <c r="AU13" s="48"/>
       <c r="AW13" s="79"/>
       <c r="AX13" s="79"/>
-    </row>
-    <row r="14" spans="1:287" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AY13" s="79"/>
+    </row>
+    <row r="14" spans="1:288" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="46"/>
       <c r="B14" s="38"/>
       <c r="C14" s="69"/>
@@ -7086,11 +7164,12 @@
       <c r="AR14" s="48"/>
       <c r="AS14" s="48"/>
       <c r="AT14" s="48"/>
-      <c r="AV14" s="79"/>
+      <c r="AU14" s="48"/>
       <c r="AW14" s="79"/>
       <c r="AX14" s="79"/>
-    </row>
-    <row r="15" spans="1:287" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AY14" s="79"/>
+    </row>
+    <row r="15" spans="1:288" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="46"/>
       <c r="B15" s="38"/>
       <c r="C15" s="69"/>
@@ -7137,11 +7216,12 @@
       <c r="AR15" s="48"/>
       <c r="AS15" s="48"/>
       <c r="AT15" s="48"/>
-      <c r="AV15" s="79"/>
+      <c r="AU15" s="48"/>
       <c r="AW15" s="79"/>
       <c r="AX15" s="79"/>
-    </row>
-    <row r="16" spans="1:287" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AY15" s="79"/>
+    </row>
+    <row r="16" spans="1:288" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="46"/>
       <c r="B16" s="38"/>
       <c r="C16" s="69"/>
@@ -7188,11 +7268,12 @@
       <c r="AR16" s="48"/>
       <c r="AS16" s="48"/>
       <c r="AT16" s="48"/>
-      <c r="AV16" s="79"/>
+      <c r="AU16" s="48"/>
       <c r="AW16" s="79"/>
       <c r="AX16" s="79"/>
-    </row>
-    <row r="17" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AY16" s="79"/>
+    </row>
+    <row r="17" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="46"/>
       <c r="B17" s="38"/>
       <c r="C17" s="69"/>
@@ -7239,11 +7320,12 @@
       <c r="AR17" s="48"/>
       <c r="AS17" s="48"/>
       <c r="AT17" s="48"/>
-      <c r="AV17" s="79"/>
+      <c r="AU17" s="48"/>
       <c r="AW17" s="79"/>
       <c r="AX17" s="79"/>
-    </row>
-    <row r="18" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AY17" s="79"/>
+    </row>
+    <row r="18" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="46"/>
       <c r="B18" s="38"/>
       <c r="C18" s="69"/>
@@ -7290,11 +7372,12 @@
       <c r="AR18" s="48"/>
       <c r="AS18" s="48"/>
       <c r="AT18" s="48"/>
-      <c r="AV18" s="79"/>
+      <c r="AU18" s="48"/>
       <c r="AW18" s="79"/>
       <c r="AX18" s="79"/>
-    </row>
-    <row r="19" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AY18" s="79"/>
+    </row>
+    <row r="19" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="39"/>
       <c r="B19" s="38"/>
       <c r="C19" s="69"/>
@@ -7341,11 +7424,12 @@
       <c r="AR19" s="48"/>
       <c r="AS19" s="48"/>
       <c r="AT19" s="48"/>
-      <c r="AV19" s="79"/>
+      <c r="AU19" s="48"/>
       <c r="AW19" s="79"/>
       <c r="AX19" s="79"/>
-    </row>
-    <row r="20" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AY19" s="79"/>
+    </row>
+    <row r="20" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="26"/>
       <c r="B20" s="25"/>
       <c r="C20" s="69"/>
@@ -7392,8 +7476,9 @@
       <c r="AR20" s="48"/>
       <c r="AS20" s="48"/>
       <c r="AT20" s="48"/>
-    </row>
-    <row r="21" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AU20" s="48"/>
+    </row>
+    <row r="21" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="26"/>
       <c r="B21" s="25"/>
       <c r="C21" s="69"/>
@@ -7440,8 +7525,9 @@
       <c r="AR21" s="48"/>
       <c r="AS21" s="48"/>
       <c r="AT21" s="48"/>
-    </row>
-    <row r="22" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AU21" s="48"/>
+    </row>
+    <row r="22" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="26"/>
       <c r="B22" s="25"/>
       <c r="C22" s="69"/>
@@ -7488,8 +7574,9 @@
       <c r="AR22" s="48"/>
       <c r="AS22" s="48"/>
       <c r="AT22" s="48"/>
-    </row>
-    <row r="23" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AU22" s="48"/>
+    </row>
+    <row r="23" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="35"/>
       <c r="B23" s="30"/>
       <c r="C23" s="67"/>
@@ -7536,8 +7623,9 @@
       <c r="AR23" s="48"/>
       <c r="AS23" s="48"/>
       <c r="AT23" s="48"/>
-    </row>
-    <row r="24" spans="1:50" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AU23" s="48"/>
+    </row>
+    <row r="24" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
       <c r="B24" s="24"/>
       <c r="C24" s="70"/>
@@ -7584,8 +7672,9 @@
       <c r="AR24" s="48"/>
       <c r="AS24" s="48"/>
       <c r="AT24" s="48"/>
-    </row>
-    <row r="25" spans="1:50" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AU24" s="48"/>
+    </row>
+    <row r="25" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="19"/>
       <c r="C25" s="71"/>
@@ -7632,8 +7721,9 @@
       <c r="AR25" s="19"/>
       <c r="AS25" s="19"/>
       <c r="AT25" s="19"/>
-    </row>
-    <row r="26" spans="1:50" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AU25" s="19"/>
+    </row>
+    <row r="26" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="31"/>
       <c r="B26" s="24"/>
       <c r="C26" s="65"/>
@@ -7680,8 +7770,9 @@
       <c r="AR26" s="24"/>
       <c r="AS26" s="24"/>
       <c r="AT26" s="24"/>
-    </row>
-    <row r="27" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AU26" s="24"/>
+    </row>
+    <row r="27" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="26"/>
       <c r="B27" s="25"/>
       <c r="C27" s="69"/>
@@ -7722,14 +7813,15 @@
       <c r="AL27" s="32"/>
       <c r="AM27" s="40"/>
       <c r="AN27" s="40"/>
-      <c r="AO27" s="32"/>
-      <c r="AP27" s="40"/>
+      <c r="AO27" s="40"/>
+      <c r="AP27" s="32"/>
       <c r="AQ27" s="40"/>
       <c r="AR27" s="40"/>
       <c r="AS27" s="40"/>
       <c r="AT27" s="40"/>
-    </row>
-    <row r="28" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AU27" s="40"/>
+    </row>
+    <row r="28" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="26"/>
       <c r="B28" s="25"/>
       <c r="C28" s="69"/>
@@ -7770,14 +7862,15 @@
       <c r="AL28" s="32"/>
       <c r="AM28" s="40"/>
       <c r="AN28" s="40"/>
-      <c r="AO28" s="32"/>
-      <c r="AP28" s="40"/>
+      <c r="AO28" s="40"/>
+      <c r="AP28" s="32"/>
       <c r="AQ28" s="40"/>
       <c r="AR28" s="40"/>
       <c r="AS28" s="40"/>
       <c r="AT28" s="40"/>
-    </row>
-    <row r="29" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AU28" s="40"/>
+    </row>
+    <row r="29" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="35"/>
       <c r="B29" s="30"/>
       <c r="C29" s="67"/>
@@ -7824,8 +7917,9 @@
       <c r="AR29" s="30"/>
       <c r="AS29" s="30"/>
       <c r="AT29" s="30"/>
-    </row>
-    <row r="30" spans="1:50" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AU29" s="30"/>
+    </row>
+    <row r="30" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" s="24"/>
       <c r="C30" s="70"/>
@@ -7872,8 +7966,9 @@
       <c r="AR30" s="36"/>
       <c r="AS30" s="36"/>
       <c r="AT30" s="36"/>
-    </row>
-    <row r="31" spans="1:50" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AU30" s="36"/>
+    </row>
+    <row r="31" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="72"/>
@@ -7920,8 +8015,9 @@
       <c r="AR31" s="22"/>
       <c r="AS31" s="22"/>
       <c r="AT31" s="22"/>
-    </row>
-    <row r="32" spans="1:50" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AU31" s="22"/>
+    </row>
+    <row r="32" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
       <c r="B32" s="24"/>
       <c r="C32" s="65"/>
@@ -7968,8 +8064,9 @@
       <c r="AR32" s="24"/>
       <c r="AS32" s="24"/>
       <c r="AT32" s="24"/>
-    </row>
-    <row r="33" spans="1:46" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AU32" s="24"/>
+    </row>
+    <row r="33" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="26"/>
       <c r="B33" s="25"/>
       <c r="C33" s="69"/>
@@ -8010,14 +8107,15 @@
       <c r="AL33" s="32"/>
       <c r="AM33" s="40"/>
       <c r="AN33" s="40"/>
-      <c r="AO33" s="32"/>
-      <c r="AP33" s="40"/>
+      <c r="AO33" s="40"/>
+      <c r="AP33" s="32"/>
       <c r="AQ33" s="40"/>
       <c r="AR33" s="40"/>
       <c r="AS33" s="40"/>
       <c r="AT33" s="40"/>
-    </row>
-    <row r="34" spans="1:46" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AU33" s="40"/>
+    </row>
+    <row r="34" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="26"/>
       <c r="B34" s="25"/>
       <c r="C34" s="69"/>
@@ -8058,14 +8156,15 @@
       <c r="AL34" s="32"/>
       <c r="AM34" s="40"/>
       <c r="AN34" s="40"/>
-      <c r="AO34" s="32"/>
-      <c r="AP34" s="40"/>
+      <c r="AO34" s="40"/>
+      <c r="AP34" s="32"/>
       <c r="AQ34" s="40"/>
       <c r="AR34" s="40"/>
       <c r="AS34" s="40"/>
       <c r="AT34" s="40"/>
-    </row>
-    <row r="35" spans="1:46" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AU34" s="40"/>
+    </row>
+    <row r="35" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="35"/>
       <c r="B35" s="30"/>
       <c r="C35" s="67"/>
@@ -8112,8 +8211,9 @@
       <c r="AR35" s="30"/>
       <c r="AS35" s="30"/>
       <c r="AT35" s="30"/>
-    </row>
-    <row r="36" spans="1:46" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AU35" s="30"/>
+    </row>
+    <row r="36" spans="1:47" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
       <c r="B36" s="24"/>
       <c r="C36" s="70"/>
@@ -8160,8 +8260,9 @@
       <c r="AR36" s="36"/>
       <c r="AS36" s="36"/>
       <c r="AT36" s="36"/>
-    </row>
-    <row r="37" spans="1:46" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AU36" s="36"/>
+    </row>
+    <row r="37" spans="1:47" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="72"/>
@@ -8208,8 +8309,9 @@
       <c r="AR37" s="22"/>
       <c r="AS37" s="22"/>
       <c r="AT37" s="22"/>
-    </row>
-    <row r="38" spans="1:46" ht="15" x14ac:dyDescent="0.25">
+      <c r="AU37" s="22"/>
+    </row>
+    <row r="38" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
       <c r="B38" s="24"/>
       <c r="C38" s="65"/>
@@ -8256,8 +8358,9 @@
       <c r="AR38" s="24"/>
       <c r="AS38" s="24"/>
       <c r="AT38" s="24"/>
-    </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="AU38" s="24"/>
+    </row>
+    <row r="39" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A39" s="26"/>
       <c r="B39" s="25"/>
       <c r="C39" s="69"/>
@@ -8298,14 +8401,15 @@
       <c r="AL39" s="32"/>
       <c r="AM39" s="40"/>
       <c r="AN39" s="40"/>
-      <c r="AO39" s="32"/>
-      <c r="AP39" s="40"/>
+      <c r="AO39" s="40"/>
+      <c r="AP39" s="32"/>
       <c r="AQ39" s="40"/>
       <c r="AR39" s="40"/>
       <c r="AS39" s="40"/>
       <c r="AT39" s="40"/>
-    </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="AU39" s="40"/>
+    </row>
+    <row r="40" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A40" s="26"/>
       <c r="B40" s="25"/>
       <c r="C40" s="69"/>
@@ -8346,14 +8450,15 @@
       <c r="AL40" s="32"/>
       <c r="AM40" s="40"/>
       <c r="AN40" s="40"/>
-      <c r="AO40" s="32"/>
-      <c r="AP40" s="40"/>
+      <c r="AO40" s="40"/>
+      <c r="AP40" s="32"/>
       <c r="AQ40" s="40"/>
       <c r="AR40" s="40"/>
       <c r="AS40" s="40"/>
       <c r="AT40" s="40"/>
-    </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="AU40" s="40"/>
+    </row>
+    <row r="41" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A41" s="35"/>
       <c r="B41" s="30"/>
       <c r="C41" s="67"/>
@@ -8400,8 +8505,9 @@
       <c r="AR41" s="30"/>
       <c r="AS41" s="30"/>
       <c r="AT41" s="30"/>
-    </row>
-    <row r="42" spans="1:46" ht="15" x14ac:dyDescent="0.25">
+      <c r="AU41" s="30"/>
+    </row>
+    <row r="42" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="24"/>
       <c r="C42" s="70"/>
@@ -8448,8 +8554,9 @@
       <c r="AR42" s="36"/>
       <c r="AS42" s="36"/>
       <c r="AT42" s="36"/>
-    </row>
-    <row r="43" spans="1:46" ht="15" x14ac:dyDescent="0.25">
+      <c r="AU42" s="36"/>
+    </row>
+    <row r="43" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
       <c r="B43" s="21"/>
       <c r="C43" s="72"/>
@@ -8496,8 +8603,9 @@
       <c r="AR43" s="22"/>
       <c r="AS43" s="22"/>
       <c r="AT43" s="22"/>
-    </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="AU43" s="22"/>
+    </row>
+    <row r="44" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A44" s="34"/>
       <c r="B44" s="30"/>
       <c r="C44" s="67"/>
@@ -8544,8 +8652,9 @@
       <c r="AR44" s="30"/>
       <c r="AS44" s="30"/>
       <c r="AT44" s="30"/>
-    </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="AU44" s="30"/>
+    </row>
+    <row r="45" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A45" s="35"/>
       <c r="B45" s="25"/>
       <c r="C45" s="70"/>
@@ -8592,8 +8701,9 @@
       <c r="AR45" s="36"/>
       <c r="AS45" s="36"/>
       <c r="AT45" s="36"/>
-    </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="AU45" s="36"/>
+    </row>
+    <row r="47" spans="1:47" x14ac:dyDescent="0.2">
       <c r="X47" s="8"/>
       <c r="AE47" s="8"/>
       <c r="AF47" s="8"/>
@@ -8612,10 +8722,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CP59"/>
+  <dimension ref="A1:CQ59"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AO1" sqref="AO1"/>
+    <sheetView topLeftCell="Y1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8650,20 +8760,21 @@
     <col min="36" max="37" width="14.140625" customWidth="1"/>
     <col min="38" max="39" width="11.42578125" customWidth="1"/>
     <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.42578125" style="10"/>
-    <col min="42" max="44" width="0" style="10" hidden="1" customWidth="1"/>
-    <col min="45" max="51" width="11.42578125" style="10"/>
+    <col min="41" max="41" width="13.42578125" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" style="10"/>
+    <col min="43" max="45" width="0" style="10" hidden="1" customWidth="1"/>
+    <col min="46" max="52" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:95" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="27"/>
-      <c r="B1" s="134" t="s">
+      <c r="B1" s="181" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
       <c r="G1" s="24"/>
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
@@ -8698,8 +8809,9 @@
       <c r="AL1" s="24"/>
       <c r="AM1" s="24"/>
       <c r="AN1" s="24"/>
-    </row>
-    <row r="2" spans="1:94" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AO1" s="24"/>
+    </row>
+    <row r="2" spans="1:95" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="51" t="s">
         <v>23</v>
@@ -8742,16 +8854,17 @@
       <c r="AL2" s="24"/>
       <c r="AM2" s="24"/>
       <c r="AN2" s="24"/>
-    </row>
-    <row r="3" spans="1:94" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AO2" s="24"/>
+    </row>
+    <row r="3" spans="1:95" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
-      <c r="B3" s="136" t="s">
+      <c r="B3" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
       <c r="G3" s="30"/>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
@@ -8786,7 +8899,7 @@
       <c r="AL3" s="24"/>
       <c r="AM3" s="24"/>
       <c r="AN3" s="24"/>
-      <c r="AO3" s="110"/>
+      <c r="AO3" s="24"/>
       <c r="AP3" s="110"/>
       <c r="AQ3" s="110"/>
       <c r="AR3" s="110"/>
@@ -8797,16 +8910,17 @@
       <c r="AW3" s="110"/>
       <c r="AX3" s="110"/>
       <c r="AY3" s="110"/>
-    </row>
-    <row r="4" spans="1:94" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AZ3" s="110"/>
+    </row>
+    <row r="4" spans="1:95" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
-      <c r="B4" s="137" t="s">
+      <c r="B4" s="184" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="138"/>
-      <c r="D4" s="138"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="138"/>
+      <c r="C4" s="185"/>
+      <c r="D4" s="185"/>
+      <c r="E4" s="185"/>
+      <c r="F4" s="185"/>
       <c r="G4" s="67"/>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
@@ -8841,8 +8955,9 @@
       <c r="AL4" s="24"/>
       <c r="AM4" s="24"/>
       <c r="AN4" s="24"/>
-    </row>
-    <row r="5" spans="1:94" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO4" s="24"/>
+    </row>
+    <row r="5" spans="1:95" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="29" t="s">
         <v>21</v>
@@ -8885,8 +9000,9 @@
       <c r="AL5" s="24"/>
       <c r="AM5" s="24"/>
       <c r="AN5" s="24"/>
-    </row>
-    <row r="6" spans="1:94" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO5" s="24"/>
+    </row>
+    <row r="6" spans="1:95" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="29" t="s">
         <v>22</v>
@@ -8929,7 +9045,7 @@
       <c r="AL6" s="24"/>
       <c r="AM6" s="24"/>
       <c r="AN6" s="24"/>
-      <c r="AZ6"/>
+      <c r="AO6" s="24"/>
       <c r="BA6"/>
       <c r="BB6"/>
       <c r="BC6"/>
@@ -8972,8 +9088,9 @@
       <c r="CN6"/>
       <c r="CO6"/>
       <c r="CP6"/>
-    </row>
-    <row r="7" spans="1:94" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="CQ6"/>
+    </row>
+    <row r="7" spans="1:95" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
@@ -9001,7 +9118,6 @@
       <c r="Y7" s="16"/>
       <c r="Z7" s="16"/>
       <c r="AA7" s="18"/>
-      <c r="AO7" s="110"/>
       <c r="AP7" s="110"/>
       <c r="AQ7" s="110"/>
       <c r="AR7" s="110"/>
@@ -9012,7 +9128,7 @@
       <c r="AW7" s="110"/>
       <c r="AX7" s="110"/>
       <c r="AY7" s="110"/>
-      <c r="AZ7" s="9"/>
+      <c r="AZ7" s="110"/>
       <c r="BA7" s="9"/>
       <c r="BB7" s="9"/>
       <c r="BC7" s="9"/>
@@ -9055,8 +9171,9 @@
       <c r="CN7" s="9"/>
       <c r="CO7" s="9"/>
       <c r="CP7" s="9"/>
-    </row>
-    <row r="8" spans="1:94" s="45" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="CQ7" s="9"/>
+    </row>
+    <row r="8" spans="1:95" s="45" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
         <v>16</v>
       </c>
@@ -9177,19 +9294,21 @@
       <c r="AN8" s="128" t="s">
         <v>66</v>
       </c>
-      <c r="AO8" s="127" t="s">
+      <c r="AO8" s="128" t="s">
+        <v>115</v>
+      </c>
+      <c r="AP8" s="127" t="s">
         <v>53</v>
       </c>
-      <c r="AP8" s="128" t="s">
+      <c r="AQ8" s="128" t="s">
         <v>99</v>
       </c>
-      <c r="AQ8" s="128" t="s">
+      <c r="AR8" s="128" t="s">
         <v>100</v>
       </c>
-      <c r="AR8" s="128" t="s">
+      <c r="AS8" s="128" t="s">
         <v>101</v>
       </c>
-      <c r="AS8" s="10"/>
       <c r="AT8" s="10"/>
       <c r="AU8" s="10"/>
       <c r="AV8" s="10"/>
@@ -9239,8 +9358,9 @@
       <c r="CN8" s="10"/>
       <c r="CO8" s="10"/>
       <c r="CP8" s="10"/>
-    </row>
-    <row r="9" spans="1:94" s="79" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="CQ8" s="10"/>
+    </row>
+    <row r="9" spans="1:95" s="79" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="49"/>
       <c r="B9" s="5"/>
       <c r="C9" s="63"/>
@@ -9278,7 +9398,7 @@
       <c r="AM9" s="102"/>
       <c r="AN9" s="103"/>
     </row>
-    <row r="10" spans="1:94" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:95" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="49"/>
       <c r="B10" s="5"/>
       <c r="C10" s="63"/>
@@ -9315,8 +9435,9 @@
       <c r="AL10" s="102"/>
       <c r="AM10" s="102"/>
       <c r="AN10" s="103"/>
-    </row>
-    <row r="11" spans="1:94" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO10" s="119"/>
+    </row>
+    <row r="11" spans="1:95" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="49"/>
       <c r="B11" s="5"/>
       <c r="C11" s="63"/>
@@ -9353,8 +9474,9 @@
       <c r="AL11" s="102"/>
       <c r="AM11" s="102"/>
       <c r="AN11" s="103"/>
-    </row>
-    <row r="12" spans="1:94" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO11" s="102"/>
+    </row>
+    <row r="12" spans="1:95" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
       <c r="B12" s="5"/>
       <c r="C12" s="63"/>
@@ -9391,8 +9513,9 @@
       <c r="AL12" s="102"/>
       <c r="AM12" s="102"/>
       <c r="AN12" s="103"/>
-    </row>
-    <row r="13" spans="1:94" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO12" s="48"/>
+    </row>
+    <row r="13" spans="1:95" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="5"/>
       <c r="C13" s="63"/>
@@ -9429,8 +9552,9 @@
       <c r="AL13" s="102"/>
       <c r="AM13" s="102"/>
       <c r="AN13" s="103"/>
-    </row>
-    <row r="14" spans="1:94" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO13" s="48"/>
+    </row>
+    <row r="14" spans="1:95" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="49"/>
       <c r="B14" s="5"/>
       <c r="C14" s="63"/>
@@ -9467,8 +9591,9 @@
       <c r="AL14" s="102"/>
       <c r="AM14" s="102"/>
       <c r="AN14" s="103"/>
-    </row>
-    <row r="15" spans="1:94" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO14" s="48"/>
+    </row>
+    <row r="15" spans="1:95" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="49"/>
       <c r="B15" s="5"/>
       <c r="C15" s="63"/>
@@ -9505,8 +9630,9 @@
       <c r="AL15" s="102"/>
       <c r="AM15" s="102"/>
       <c r="AN15" s="103"/>
-    </row>
-    <row r="16" spans="1:94" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO15" s="48"/>
+    </row>
+    <row r="16" spans="1:95" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="49"/>
       <c r="B16" s="5"/>
       <c r="C16" s="63"/>
@@ -9543,8 +9669,9 @@
       <c r="AL16" s="102"/>
       <c r="AM16" s="102"/>
       <c r="AN16" s="103"/>
-    </row>
-    <row r="17" spans="1:40" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO16" s="48"/>
+    </row>
+    <row r="17" spans="1:41" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="49"/>
       <c r="B17" s="5"/>
       <c r="C17" s="63"/>
@@ -9581,8 +9708,9 @@
       <c r="AL17" s="102"/>
       <c r="AM17" s="102"/>
       <c r="AN17" s="103"/>
-    </row>
-    <row r="18" spans="1:40" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO17" s="48"/>
+    </row>
+    <row r="18" spans="1:41" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="49"/>
       <c r="B18" s="5"/>
       <c r="C18" s="63"/>
@@ -9618,8 +9746,9 @@
       <c r="AL18" s="102"/>
       <c r="AM18" s="102"/>
       <c r="AN18" s="103"/>
-    </row>
-    <row r="19" spans="1:40" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO18" s="48"/>
+    </row>
+    <row r="19" spans="1:41" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="49"/>
       <c r="B19" s="5"/>
       <c r="C19" s="63"/>
@@ -9654,8 +9783,9 @@
       <c r="AL19" s="102"/>
       <c r="AM19" s="102"/>
       <c r="AN19" s="103"/>
-    </row>
-    <row r="20" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO19" s="48"/>
+    </row>
+    <row r="20" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="46"/>
       <c r="B20" s="38"/>
       <c r="C20" s="40"/>
@@ -9696,8 +9826,9 @@
       <c r="AL20" s="54"/>
       <c r="AM20" s="54"/>
       <c r="AN20" s="54"/>
-    </row>
-    <row r="21" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO20" s="48"/>
+    </row>
+    <row r="21" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="46"/>
       <c r="B21" s="38"/>
       <c r="C21" s="40"/>
@@ -9738,8 +9869,9 @@
       <c r="AL21" s="48"/>
       <c r="AM21" s="48"/>
       <c r="AN21" s="48"/>
-    </row>
-    <row r="22" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO21" s="48"/>
+    </row>
+    <row r="22" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="46"/>
       <c r="B22" s="38"/>
       <c r="C22" s="40"/>
@@ -9780,8 +9912,9 @@
       <c r="AL22" s="48"/>
       <c r="AM22" s="48"/>
       <c r="AN22" s="48"/>
-    </row>
-    <row r="23" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO22" s="48"/>
+    </row>
+    <row r="23" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="46"/>
       <c r="B23" s="38"/>
       <c r="C23" s="40"/>
@@ -9822,8 +9955,9 @@
       <c r="AL23" s="48"/>
       <c r="AM23" s="48"/>
       <c r="AN23" s="48"/>
-    </row>
-    <row r="24" spans="1:40" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO23" s="48"/>
+    </row>
+    <row r="24" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="46"/>
       <c r="B24" s="38"/>
       <c r="C24" s="40"/>
@@ -9864,8 +9998,9 @@
       <c r="AL24" s="48"/>
       <c r="AM24" s="48"/>
       <c r="AN24" s="48"/>
-    </row>
-    <row r="25" spans="1:40" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO24" s="48"/>
+    </row>
+    <row r="25" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
       <c r="B25" s="38"/>
       <c r="C25" s="40"/>
@@ -9906,8 +10041,9 @@
       <c r="AL25" s="48"/>
       <c r="AM25" s="48"/>
       <c r="AN25" s="48"/>
-    </row>
-    <row r="26" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO25" s="19"/>
+    </row>
+    <row r="26" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="46"/>
       <c r="B26" s="38"/>
       <c r="C26" s="40"/>
@@ -9948,8 +10084,9 @@
       <c r="AL26" s="48"/>
       <c r="AM26" s="48"/>
       <c r="AN26" s="48"/>
-    </row>
-    <row r="27" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO26" s="24"/>
+    </row>
+    <row r="27" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="46"/>
       <c r="B27" s="38"/>
       <c r="C27" s="40"/>
@@ -9990,8 +10127,9 @@
       <c r="AL27" s="48"/>
       <c r="AM27" s="48"/>
       <c r="AN27" s="48"/>
-    </row>
-    <row r="28" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO27" s="40"/>
+    </row>
+    <row r="28" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="46"/>
       <c r="B28" s="38"/>
       <c r="C28" s="40"/>
@@ -10032,8 +10170,9 @@
       <c r="AL28" s="48"/>
       <c r="AM28" s="48"/>
       <c r="AN28" s="48"/>
-    </row>
-    <row r="29" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO28" s="40"/>
+    </row>
+    <row r="29" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="46"/>
       <c r="B29" s="38"/>
       <c r="C29" s="40"/>
@@ -10074,8 +10213,9 @@
       <c r="AL29" s="48"/>
       <c r="AM29" s="48"/>
       <c r="AN29" s="48"/>
-    </row>
-    <row r="30" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO29" s="30"/>
+    </row>
+    <row r="30" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="46"/>
       <c r="B30" s="38"/>
       <c r="C30" s="40"/>
@@ -10116,8 +10256,9 @@
       <c r="AL30" s="48"/>
       <c r="AM30" s="48"/>
       <c r="AN30" s="48"/>
-    </row>
-    <row r="31" spans="1:40" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO30" s="36"/>
+    </row>
+    <row r="31" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="39"/>
       <c r="B31" s="38"/>
       <c r="C31" s="40"/>
@@ -10158,8 +10299,9 @@
       <c r="AL31" s="48"/>
       <c r="AM31" s="48"/>
       <c r="AN31" s="48"/>
-    </row>
-    <row r="32" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO31" s="22"/>
+    </row>
+    <row r="32" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="39"/>
       <c r="B32" s="38"/>
       <c r="C32" s="40"/>
@@ -10200,8 +10342,9 @@
       <c r="AL32" s="48"/>
       <c r="AM32" s="48"/>
       <c r="AN32" s="48"/>
-    </row>
-    <row r="33" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO32" s="24"/>
+    </row>
+    <row r="33" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="39"/>
       <c r="B33" s="38"/>
       <c r="C33" s="40"/>
@@ -10242,8 +10385,9 @@
       <c r="AL33" s="48"/>
       <c r="AM33" s="48"/>
       <c r="AN33" s="48"/>
-    </row>
-    <row r="34" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO33" s="40"/>
+    </row>
+    <row r="34" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="39"/>
       <c r="B34" s="38"/>
       <c r="C34" s="40"/>
@@ -10284,8 +10428,9 @@
       <c r="AL34" s="48"/>
       <c r="AM34" s="48"/>
       <c r="AN34" s="48"/>
-    </row>
-    <row r="35" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO34" s="40"/>
+    </row>
+    <row r="35" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="35"/>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
@@ -10326,8 +10471,9 @@
       <c r="AL35" s="48"/>
       <c r="AM35" s="48"/>
       <c r="AN35" s="48"/>
-    </row>
-    <row r="36" spans="1:40" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO35" s="30"/>
+    </row>
+    <row r="36" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
       <c r="B36" s="24"/>
       <c r="C36" s="36"/>
@@ -10368,8 +10514,9 @@
       <c r="AL36" s="48"/>
       <c r="AM36" s="48"/>
       <c r="AN36" s="48"/>
-    </row>
-    <row r="37" spans="1:40" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO36" s="36"/>
+    </row>
+    <row r="37" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
@@ -10410,8 +10557,9 @@
       <c r="AL37" s="19"/>
       <c r="AM37" s="19"/>
       <c r="AN37" s="19"/>
-    </row>
-    <row r="38" spans="1:40" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO37" s="22"/>
+    </row>
+    <row r="38" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
       <c r="B38" s="24"/>
       <c r="C38" s="24"/>
@@ -10452,8 +10600,9 @@
       <c r="AL38" s="24"/>
       <c r="AM38" s="24"/>
       <c r="AN38" s="24"/>
-    </row>
-    <row r="39" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO38" s="24"/>
+    </row>
+    <row r="39" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="39"/>
       <c r="B39" s="38"/>
       <c r="C39" s="40"/>
@@ -10494,8 +10643,9 @@
       <c r="AL39" s="40"/>
       <c r="AM39" s="40"/>
       <c r="AN39" s="40"/>
-    </row>
-    <row r="40" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO39" s="40"/>
+    </row>
+    <row r="40" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="39"/>
       <c r="B40" s="38"/>
       <c r="C40" s="40"/>
@@ -10536,8 +10686,9 @@
       <c r="AL40" s="40"/>
       <c r="AM40" s="40"/>
       <c r="AN40" s="40"/>
-    </row>
-    <row r="41" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO40" s="40"/>
+    </row>
+    <row r="41" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="35"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
@@ -10578,8 +10729,9 @@
       <c r="AL41" s="30"/>
       <c r="AM41" s="30"/>
       <c r="AN41" s="30"/>
-    </row>
-    <row r="42" spans="1:40" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO41" s="30"/>
+    </row>
+    <row r="42" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="24"/>
       <c r="C42" s="36"/>
@@ -10620,8 +10772,9 @@
       <c r="AL42" s="36"/>
       <c r="AM42" s="36"/>
       <c r="AN42" s="36"/>
-    </row>
-    <row r="43" spans="1:40" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO42" s="36"/>
+    </row>
+    <row r="43" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
       <c r="B43" s="21"/>
       <c r="C43" s="22"/>
@@ -10662,8 +10815,9 @@
       <c r="AL43" s="22"/>
       <c r="AM43" s="22"/>
       <c r="AN43" s="22"/>
-    </row>
-    <row r="44" spans="1:40" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO43" s="22"/>
+    </row>
+    <row r="44" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="31"/>
       <c r="B44" s="24"/>
       <c r="C44" s="24"/>
@@ -10704,8 +10858,9 @@
       <c r="AL44" s="24"/>
       <c r="AM44" s="24"/>
       <c r="AN44" s="24"/>
-    </row>
-    <row r="45" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO44" s="30"/>
+    </row>
+    <row r="45" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="39"/>
       <c r="B45" s="38"/>
       <c r="C45" s="40"/>
@@ -10746,8 +10901,9 @@
       <c r="AL45" s="40"/>
       <c r="AM45" s="40"/>
       <c r="AN45" s="40"/>
-    </row>
-    <row r="46" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO45" s="36"/>
+    </row>
+    <row r="46" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="39"/>
       <c r="B46" s="38"/>
       <c r="C46" s="40"/>
@@ -10788,8 +10944,9 @@
       <c r="AL46" s="40"/>
       <c r="AM46" s="40"/>
       <c r="AN46" s="40"/>
-    </row>
-    <row r="47" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO46"/>
+    </row>
+    <row r="47" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="35"/>
       <c r="B47" s="30"/>
       <c r="C47" s="30"/>
@@ -10830,8 +10987,9 @@
       <c r="AL47" s="30"/>
       <c r="AM47" s="30"/>
       <c r="AN47" s="30"/>
-    </row>
-    <row r="48" spans="1:40" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO47"/>
+    </row>
+    <row r="48" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="24"/>
       <c r="B48" s="24"/>
       <c r="C48" s="36"/>
@@ -10872,8 +11030,9 @@
       <c r="AL48" s="36"/>
       <c r="AM48" s="36"/>
       <c r="AN48" s="36"/>
-    </row>
-    <row r="49" spans="1:40" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO48"/>
+    </row>
+    <row r="49" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="21"/>
       <c r="B49" s="21"/>
       <c r="C49" s="22"/>
@@ -10914,8 +11073,9 @@
       <c r="AL49" s="22"/>
       <c r="AM49" s="22"/>
       <c r="AN49" s="22"/>
-    </row>
-    <row r="50" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO49"/>
+    </row>
+    <row r="50" spans="1:41" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="31"/>
       <c r="B50" s="24"/>
       <c r="C50" s="24"/>
@@ -10955,7 +11115,7 @@
       <c r="AM50" s="24"/>
       <c r="AN50" s="24"/>
     </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A51" s="39"/>
       <c r="B51" s="38"/>
       <c r="C51" s="40"/>
@@ -10995,7 +11155,7 @@
       <c r="AM51" s="40"/>
       <c r="AN51" s="40"/>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A52" s="39"/>
       <c r="B52" s="38"/>
       <c r="C52" s="40"/>
@@ -11035,7 +11195,7 @@
       <c r="AM52" s="40"/>
       <c r="AN52" s="40"/>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A53" s="35"/>
       <c r="B53" s="30"/>
       <c r="C53" s="30"/>
@@ -11075,7 +11235,7 @@
       <c r="AM53" s="30"/>
       <c r="AN53" s="30"/>
     </row>
-    <row r="54" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:41" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="24"/>
       <c r="B54" s="24"/>
       <c r="C54" s="36"/>
@@ -11115,7 +11275,7 @@
       <c r="AM54" s="36"/>
       <c r="AN54" s="36"/>
     </row>
-    <row r="55" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:41" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="22"/>
@@ -11155,7 +11315,7 @@
       <c r="AM55" s="22"/>
       <c r="AN55" s="22"/>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A56" s="34"/>
       <c r="B56" s="30"/>
       <c r="C56" s="30"/>
@@ -11195,7 +11355,7 @@
       <c r="AM56" s="30"/>
       <c r="AN56" s="30"/>
     </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A57" s="35"/>
       <c r="B57" s="38"/>
       <c r="C57" s="36"/>
@@ -11235,7 +11395,7 @@
       <c r="AM57" s="36"/>
       <c r="AN57" s="36"/>
     </row>
-    <row r="59" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.2">
       <c r="X59" s="8"/>
       <c r="AE59" s="8"/>
       <c r="AF59" s="8"/>
@@ -11897,875 +12057,931 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="139"/>
-      <c r="B1" s="139"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="141"/>
-      <c r="F1" s="141"/>
-      <c r="G1" s="141"/>
-      <c r="H1" s="141"/>
-      <c r="I1" s="141"/>
-      <c r="J1" s="141"/>
+      <c r="A1" s="133"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
     </row>
     <row r="2" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="139"/>
-      <c r="B2" s="139"/>
-      <c r="C2" s="140"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="140"/>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
-      <c r="J2" s="141"/>
+      <c r="A2" s="133"/>
+      <c r="B2" s="133"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="139"/>
-      <c r="B3" s="142" t="s">
+      <c r="A3" s="133"/>
+      <c r="B3" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="143">
+      <c r="C3" s="186">
         <v>43374</v>
       </c>
-      <c r="D3" s="144"/>
-      <c r="E3" s="145"/>
-      <c r="F3" s="142" t="s">
+      <c r="D3" s="187"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="146"/>
-      <c r="H3" s="143"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="141"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="186"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="135"/>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="139"/>
-      <c r="B4" s="147" t="s">
+      <c r="A4" s="133"/>
+      <c r="B4" s="139" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="148" t="s">
+      <c r="C4" s="140" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="148" t="s">
+      <c r="D4" s="140" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="149"/>
-      <c r="F4" s="147" t="s">
+      <c r="E4" s="141"/>
+      <c r="F4" s="139" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="150" t="s">
+      <c r="G4" s="142" t="s">
         <v>102</v>
       </c>
-      <c r="H4" s="148" t="s">
+      <c r="H4" s="140" t="s">
         <v>79</v>
       </c>
-      <c r="I4" s="148" t="s">
+      <c r="I4" s="140" t="s">
         <v>80</v>
       </c>
-      <c r="J4" s="141"/>
+      <c r="J4" s="135"/>
     </row>
     <row r="5" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="139"/>
-      <c r="B5" s="151" t="s">
+      <c r="A5" s="133"/>
+      <c r="B5" s="143" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="152"/>
-      <c r="D5" s="152"/>
-      <c r="E5" s="140"/>
-      <c r="F5" s="151" t="s">
+      <c r="C5" s="144"/>
+      <c r="D5" s="144"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="143" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="151"/>
-      <c r="H5" s="152"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="141"/>
+      <c r="G5" s="143"/>
+      <c r="H5" s="144"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="135"/>
     </row>
     <row r="6" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="139"/>
-      <c r="B6" s="154" t="s">
+      <c r="A6" s="133"/>
+      <c r="B6" s="146" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="155"/>
-      <c r="D6" s="155"/>
-      <c r="E6" s="140"/>
-      <c r="F6" s="156" t="s">
+      <c r="C6" s="147"/>
+      <c r="D6" s="147"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="148" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="157"/>
-      <c r="H6" s="155"/>
-      <c r="I6" s="153"/>
-      <c r="J6" s="141"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="147"/>
+      <c r="I6" s="145"/>
+      <c r="J6" s="135"/>
     </row>
     <row r="7" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="139"/>
-      <c r="B7" s="154" t="s">
+      <c r="A7" s="133"/>
+      <c r="B7" s="146" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="155"/>
-      <c r="D7" s="155"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="156" t="s">
+      <c r="C7" s="147"/>
+      <c r="D7" s="147"/>
+      <c r="E7" s="150"/>
+      <c r="F7" s="148" t="s">
         <v>103</v>
       </c>
-      <c r="G7" s="157"/>
-      <c r="H7" s="155"/>
-      <c r="I7" s="153"/>
-      <c r="J7" s="141"/>
+      <c r="G7" s="149"/>
+      <c r="H7" s="147"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="135"/>
     </row>
     <row r="8" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="139"/>
-      <c r="B8" s="154" t="s">
+      <c r="A8" s="133"/>
+      <c r="B8" s="146" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="155"/>
-      <c r="D8" s="155"/>
-      <c r="E8" s="159"/>
-      <c r="F8" s="156" t="s">
+      <c r="C8" s="147"/>
+      <c r="D8" s="147"/>
+      <c r="E8" s="151"/>
+      <c r="F8" s="148" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="157"/>
-      <c r="H8" s="155"/>
-      <c r="I8" s="153"/>
-      <c r="J8" s="141"/>
+      <c r="G8" s="149"/>
+      <c r="H8" s="147"/>
+      <c r="I8" s="145"/>
+      <c r="J8" s="135"/>
     </row>
     <row r="9" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="139"/>
-      <c r="B9" s="154" t="s">
+      <c r="A9" s="133"/>
+      <c r="B9" s="146" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="155"/>
-      <c r="D9" s="155"/>
-      <c r="E9" s="160"/>
-      <c r="F9" s="156" t="s">
+      <c r="C9" s="147"/>
+      <c r="D9" s="147"/>
+      <c r="E9" s="152"/>
+      <c r="F9" s="148" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="157"/>
-      <c r="H9" s="155"/>
-      <c r="I9" s="153"/>
-      <c r="J9" s="141"/>
+      <c r="G9" s="149"/>
+      <c r="H9" s="147"/>
+      <c r="I9" s="145"/>
+      <c r="J9" s="135"/>
     </row>
     <row r="10" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="139"/>
-      <c r="B10" s="154" t="s">
+      <c r="A10" s="133"/>
+      <c r="B10" s="146" t="s">
         <v>106</v>
       </c>
-      <c r="C10" s="155"/>
-      <c r="D10" s="155"/>
-      <c r="E10" s="158"/>
-      <c r="F10" s="156" t="s">
+      <c r="C10" s="147"/>
+      <c r="D10" s="147"/>
+      <c r="E10" s="150"/>
+      <c r="F10" s="148" t="s">
         <v>105</v>
       </c>
-      <c r="G10" s="157"/>
-      <c r="H10" s="155"/>
-      <c r="I10" s="153"/>
-      <c r="J10" s="141"/>
+      <c r="G10" s="149"/>
+      <c r="H10" s="147"/>
+      <c r="I10" s="145"/>
+      <c r="J10" s="135"/>
     </row>
     <row r="11" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="139"/>
-      <c r="B11" s="154" t="s">
+      <c r="A11" s="133"/>
+      <c r="B11" s="146" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="155"/>
-      <c r="D11" s="155"/>
-      <c r="E11" s="158"/>
-      <c r="F11" s="156" t="s">
+      <c r="C11" s="147"/>
+      <c r="D11" s="147"/>
+      <c r="E11" s="150"/>
+      <c r="F11" s="148" t="s">
         <v>107</v>
       </c>
-      <c r="G11" s="157"/>
-      <c r="H11" s="155"/>
-      <c r="I11" s="153"/>
-      <c r="J11" s="141"/>
+      <c r="G11" s="149"/>
+      <c r="H11" s="147"/>
+      <c r="I11" s="145"/>
+      <c r="J11" s="135"/>
     </row>
     <row r="12" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="139"/>
-      <c r="B12" s="154" t="s">
+      <c r="A12" s="133"/>
+      <c r="B12" s="146" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="155"/>
-      <c r="D12" s="155"/>
-      <c r="E12" s="159"/>
-      <c r="F12" s="156" t="s">
+      <c r="C12" s="147"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="151"/>
+      <c r="F12" s="148" t="s">
         <v>93</v>
       </c>
-      <c r="G12" s="157"/>
-      <c r="H12" s="155"/>
-      <c r="I12" s="155"/>
-      <c r="J12" s="141"/>
+      <c r="G12" s="149"/>
+      <c r="H12" s="147"/>
+      <c r="I12" s="147"/>
+      <c r="J12" s="135"/>
     </row>
     <row r="13" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="139"/>
-      <c r="B13" s="154" t="s">
+      <c r="A13" s="133"/>
+      <c r="B13" s="146" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="155"/>
-      <c r="E13" s="159"/>
-      <c r="F13" s="156" t="s">
+      <c r="C13" s="147"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="151"/>
+      <c r="F13" s="148" t="s">
         <v>108</v>
       </c>
-      <c r="G13" s="157"/>
-      <c r="H13" s="155"/>
-      <c r="I13" s="155"/>
-      <c r="J13" s="141"/>
+      <c r="G13" s="149"/>
+      <c r="H13" s="147"/>
+      <c r="I13" s="147"/>
+      <c r="J13" s="135"/>
     </row>
     <row r="14" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="139"/>
-      <c r="B14" s="154" t="s">
+      <c r="A14" s="133"/>
+      <c r="B14" s="146" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="159"/>
-      <c r="D14" s="155"/>
-      <c r="E14" s="160"/>
-      <c r="F14" s="156" t="s">
+      <c r="C14" s="151"/>
+      <c r="D14" s="147"/>
+      <c r="E14" s="152"/>
+      <c r="F14" s="148" t="s">
         <v>109</v>
       </c>
-      <c r="G14" s="157"/>
-      <c r="H14" s="155"/>
-      <c r="I14" s="155"/>
-      <c r="J14" s="141"/>
+      <c r="G14" s="149"/>
+      <c r="H14" s="147"/>
+      <c r="I14" s="147"/>
+      <c r="J14" s="135"/>
     </row>
     <row r="15" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="139"/>
-      <c r="B15" s="161" t="s">
+      <c r="A15" s="133"/>
+      <c r="B15" s="153" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="155"/>
-      <c r="D15" s="155"/>
-      <c r="E15" s="162"/>
-      <c r="F15" s="156" t="s">
+      <c r="C15" s="147"/>
+      <c r="D15" s="147"/>
+      <c r="E15" s="154"/>
+      <c r="F15" s="148" t="s">
         <v>96</v>
       </c>
-      <c r="G15" s="157"/>
-      <c r="H15" s="155"/>
-      <c r="I15" s="155"/>
-      <c r="J15" s="141"/>
+      <c r="G15" s="149"/>
+      <c r="H15" s="147"/>
+      <c r="I15" s="147"/>
+      <c r="J15" s="135"/>
     </row>
     <row r="16" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="139"/>
-      <c r="B16" s="163" t="s">
+      <c r="A16" s="133"/>
+      <c r="B16" s="155" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="159"/>
-      <c r="D16" s="164"/>
-      <c r="E16" s="162"/>
-      <c r="F16" s="156" t="s">
+      <c r="C16" s="151"/>
+      <c r="D16" s="156"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="148" t="s">
         <v>106</v>
       </c>
-      <c r="G16" s="157"/>
-      <c r="H16" s="155"/>
-      <c r="I16" s="155"/>
-      <c r="J16" s="141"/>
+      <c r="G16" s="149"/>
+      <c r="H16" s="147"/>
+      <c r="I16" s="147"/>
+      <c r="J16" s="135"/>
     </row>
     <row r="17" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="139"/>
-      <c r="B17" s="154" t="s">
+      <c r="A17" s="133"/>
+      <c r="B17" s="146" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="155"/>
-      <c r="D17" s="155"/>
-      <c r="E17" s="162"/>
-      <c r="F17" s="156" t="s">
+      <c r="C17" s="147"/>
+      <c r="D17" s="147"/>
+      <c r="E17" s="154"/>
+      <c r="F17" s="148" t="s">
         <v>110</v>
       </c>
-      <c r="G17" s="157"/>
-      <c r="H17" s="155"/>
-      <c r="I17" s="155"/>
-      <c r="J17" s="141"/>
+      <c r="G17" s="149"/>
+      <c r="H17" s="147"/>
+      <c r="I17" s="147"/>
+      <c r="J17" s="135"/>
     </row>
     <row r="18" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="139"/>
-      <c r="B18" s="154" t="s">
+      <c r="A18" s="133"/>
+      <c r="B18" s="146" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="155"/>
-      <c r="D18" s="155"/>
-      <c r="E18" s="162"/>
-      <c r="F18" s="161" t="s">
+      <c r="C18" s="147"/>
+      <c r="D18" s="147"/>
+      <c r="E18" s="154"/>
+      <c r="F18" s="153" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="157"/>
-      <c r="H18" s="155"/>
-      <c r="I18" s="155"/>
-      <c r="J18" s="141"/>
+      <c r="G18" s="149"/>
+      <c r="H18" s="147"/>
+      <c r="I18" s="147"/>
+      <c r="J18" s="135"/>
     </row>
     <row r="19" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="139"/>
-      <c r="B19" s="154" t="s">
+      <c r="A19" s="133"/>
+      <c r="B19" s="146" t="s">
         <v>110</v>
       </c>
-      <c r="C19" s="155"/>
-      <c r="D19" s="155"/>
-      <c r="E19" s="162"/>
-      <c r="F19" s="161" t="s">
+      <c r="C19" s="147"/>
+      <c r="D19" s="147"/>
+      <c r="E19" s="154"/>
+      <c r="F19" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="G19" s="157"/>
-      <c r="H19" s="155"/>
-      <c r="I19" s="155"/>
-      <c r="J19" s="141"/>
+      <c r="G19" s="149"/>
+      <c r="H19" s="147"/>
+      <c r="I19" s="147"/>
+      <c r="J19" s="135"/>
     </row>
     <row r="20" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="139"/>
-      <c r="B20" s="154" t="s">
+      <c r="A20" s="133"/>
+      <c r="B20" s="146" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="155"/>
-      <c r="D20" s="155"/>
-      <c r="E20" s="162"/>
-      <c r="F20" s="165" t="s">
+      <c r="C20" s="147"/>
+      <c r="D20" s="147"/>
+      <c r="E20" s="154"/>
+      <c r="F20" s="157" t="s">
         <v>91</v>
       </c>
-      <c r="G20" s="157"/>
-      <c r="H20" s="155"/>
-      <c r="I20" s="155"/>
-      <c r="J20" s="141"/>
+      <c r="G20" s="149"/>
+      <c r="H20" s="147"/>
+      <c r="I20" s="147"/>
+      <c r="J20" s="135"/>
     </row>
     <row r="21" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="139"/>
-      <c r="B21" s="154" t="s">
+      <c r="A21" s="133"/>
+      <c r="B21" s="146" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="155"/>
-      <c r="D21" s="155"/>
-      <c r="E21" s="162"/>
-      <c r="F21" s="165" t="s">
+      <c r="C21" s="147"/>
+      <c r="D21" s="147"/>
+      <c r="E21" s="154"/>
+      <c r="F21" s="157" t="s">
         <v>111</v>
       </c>
-      <c r="G21" s="157"/>
-      <c r="H21" s="153"/>
-      <c r="I21" s="155"/>
-      <c r="J21" s="141"/>
-    </row>
-    <row r="22" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="139"/>
-      <c r="B22" s="166" t="s">
+      <c r="G21" s="149"/>
+      <c r="H21" s="145"/>
+      <c r="I21" s="147"/>
+      <c r="J21" s="135"/>
+    </row>
+    <row r="22" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="133"/>
+      <c r="B22" s="155" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="167"/>
-      <c r="D22" s="167"/>
-      <c r="E22" s="162"/>
-      <c r="F22" s="165" t="s">
+      <c r="C22" s="156"/>
+      <c r="D22" s="156"/>
+      <c r="E22" s="154"/>
+      <c r="F22" s="157" t="s">
         <v>112</v>
       </c>
-      <c r="G22" s="157"/>
-      <c r="H22" s="153"/>
-      <c r="I22" s="155"/>
-      <c r="J22" s="141"/>
+      <c r="G22" s="149"/>
+      <c r="H22" s="145"/>
+      <c r="I22" s="147"/>
+      <c r="J22" s="135"/>
     </row>
     <row r="23" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="139"/>
-      <c r="B23" s="168" t="s">
+      <c r="A23" s="133"/>
+      <c r="B23" s="155" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="156"/>
+      <c r="D23" s="156"/>
+      <c r="E23" s="154"/>
+      <c r="F23" s="157" t="s">
+        <v>113</v>
+      </c>
+      <c r="G23" s="149"/>
+      <c r="H23" s="145"/>
+      <c r="I23" s="147"/>
+      <c r="J23" s="135"/>
+    </row>
+    <row r="24" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="133"/>
+      <c r="B24" s="157" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="157"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="154"/>
+      <c r="F24" s="163" t="s">
+        <v>114</v>
+      </c>
+      <c r="G24" s="164"/>
+      <c r="H24" s="145"/>
+      <c r="I24" s="147"/>
+      <c r="J24" s="135"/>
+    </row>
+    <row r="25" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="133"/>
+      <c r="B25" s="157" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="157"/>
+      <c r="D25" s="157"/>
+      <c r="E25" s="154"/>
+      <c r="F25" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="169">
-        <f>SUM(C6:C22)</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="169"/>
-      <c r="E23" s="162"/>
-      <c r="F23" s="165" t="s">
-        <v>113</v>
-      </c>
-      <c r="G23" s="157"/>
-      <c r="H23" s="153"/>
-      <c r="I23" s="155"/>
-      <c r="J23" s="141"/>
-    </row>
-    <row r="24" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="139"/>
-      <c r="B24" s="170" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="155">
-        <f>C23*16%</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="155"/>
-      <c r="E24" s="162"/>
-      <c r="F24" s="171" t="s">
-        <v>114</v>
-      </c>
-      <c r="G24" s="172"/>
-      <c r="H24" s="153"/>
-      <c r="I24" s="155"/>
-      <c r="J24" s="141"/>
-    </row>
-    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="139"/>
-      <c r="B25" s="173" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="174">
-        <f>SUM(C23:C24)</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="174"/>
-      <c r="E25" s="162"/>
-      <c r="F25" s="168" t="s">
-        <v>0</v>
-      </c>
-      <c r="G25" s="175"/>
-      <c r="H25" s="176">
+      <c r="G25" s="167"/>
+      <c r="H25" s="168">
         <f>SUM(H6:H24)</f>
         <v>0</v>
       </c>
-      <c r="I25" s="176">
+      <c r="I25" s="168">
         <f>SUM(I6:I24)</f>
         <v>0</v>
       </c>
-      <c r="J25" s="141"/>
-    </row>
-    <row r="26" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="139"/>
-      <c r="B26" s="151" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="153"/>
-      <c r="D26" s="153"/>
-      <c r="E26" s="162"/>
-      <c r="F26" s="170" t="s">
+      <c r="J25" s="135"/>
+    </row>
+    <row r="26" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="133"/>
+      <c r="B26" s="158" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="159"/>
+      <c r="D26" s="159"/>
+      <c r="E26" s="154"/>
+      <c r="F26" s="162" t="s">
         <v>83</v>
       </c>
-      <c r="G26" s="177"/>
-      <c r="H26" s="155">
+      <c r="G26" s="169"/>
+      <c r="H26" s="147">
         <f>H25*16%</f>
         <v>0</v>
       </c>
-      <c r="I26" s="155">
+      <c r="I26" s="147">
         <f>I25*16%</f>
         <v>0</v>
       </c>
-      <c r="J26" s="141"/>
+      <c r="J26" s="135"/>
     </row>
     <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="139"/>
-      <c r="B27" s="154" t="s">
-        <v>85</v>
-      </c>
-      <c r="C27" s="153"/>
-      <c r="D27" s="153"/>
-      <c r="E27" s="162"/>
-      <c r="F27" s="173" t="s">
+      <c r="A27" s="133"/>
+      <c r="B27" s="160" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="161">
+        <f>SUM(C6:C26)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="161"/>
+      <c r="E27" s="154"/>
+      <c r="F27" s="165" t="s">
         <v>1</v>
       </c>
-      <c r="G27" s="178">
+      <c r="G27" s="170">
         <f>SUM(G6:G26)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="174">
+      <c r="H27" s="166">
         <f>+H25+H26</f>
         <v>0</v>
       </c>
-      <c r="I27" s="174">
+      <c r="I27" s="166">
         <f>+I25+I26</f>
         <v>0</v>
       </c>
-      <c r="J27" s="141"/>
+      <c r="J27" s="135"/>
     </row>
     <row r="28" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="139"/>
-      <c r="B28" s="154" t="s">
+      <c r="A28" s="133"/>
+      <c r="B28" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="147">
+        <f>C27*16%</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="147"/>
+      <c r="E28" s="154"/>
+      <c r="F28" s="143" t="s">
+        <v>84</v>
+      </c>
+      <c r="G28" s="143"/>
+      <c r="H28" s="171"/>
+      <c r="I28" s="171"/>
+      <c r="J28" s="135"/>
+    </row>
+    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="133"/>
+      <c r="B29" s="165" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="166">
+        <f>SUM(C27:C28)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="166"/>
+      <c r="E29" s="154"/>
+      <c r="F29" s="148" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="149"/>
+      <c r="H29" s="147"/>
+      <c r="I29" s="147"/>
+      <c r="J29" s="135"/>
+    </row>
+    <row r="30" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="133"/>
+      <c r="B30" s="143" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="145"/>
+      <c r="D30" s="145"/>
+      <c r="E30" s="154"/>
+      <c r="F30" s="148" t="s">
+        <v>103</v>
+      </c>
+      <c r="G30" s="149"/>
+      <c r="H30" s="147"/>
+      <c r="I30" s="147"/>
+      <c r="J30" s="135"/>
+    </row>
+    <row r="31" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="133"/>
+      <c r="B31" s="146" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="145"/>
+      <c r="D31" s="145"/>
+      <c r="E31" s="154"/>
+      <c r="F31" s="148" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="155"/>
-      <c r="D28" s="152"/>
-      <c r="E28" s="162"/>
-      <c r="F28" s="151" t="s">
-        <v>84</v>
-      </c>
-      <c r="G28" s="151"/>
-      <c r="H28" s="179"/>
-      <c r="I28" s="179"/>
-      <c r="J28" s="141"/>
-    </row>
-    <row r="29" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="139"/>
-      <c r="B29" s="154" t="s">
+      <c r="G31" s="149"/>
+      <c r="H31" s="147"/>
+      <c r="I31" s="147"/>
+      <c r="J31" s="135"/>
+    </row>
+    <row r="32" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="133"/>
+      <c r="B32" s="146" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="147"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="154"/>
+      <c r="F32" s="148" t="s">
         <v>104</v>
       </c>
-      <c r="C29" s="155"/>
-      <c r="D29" s="152"/>
-      <c r="E29" s="162"/>
-      <c r="F29" s="156" t="s">
-        <v>85</v>
-      </c>
-      <c r="G29" s="157"/>
-      <c r="H29" s="155"/>
-      <c r="I29" s="155"/>
-      <c r="J29" s="141"/>
-    </row>
-    <row r="30" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="139"/>
-      <c r="B30" s="154" t="s">
+      <c r="G32" s="149"/>
+      <c r="H32" s="147"/>
+      <c r="I32" s="147"/>
+      <c r="J32" s="135"/>
+    </row>
+    <row r="33" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="133"/>
+      <c r="B33" s="146" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="147"/>
+      <c r="D33" s="144"/>
+      <c r="E33" s="154"/>
+      <c r="F33" s="148" t="s">
         <v>105</v>
       </c>
-      <c r="C30" s="155"/>
-      <c r="D30" s="152"/>
-      <c r="E30" s="162"/>
-      <c r="F30" s="156" t="s">
-        <v>103</v>
-      </c>
-      <c r="G30" s="157"/>
-      <c r="H30" s="155"/>
-      <c r="I30" s="155"/>
-      <c r="J30" s="141"/>
-    </row>
-    <row r="31" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="139"/>
-      <c r="B31" s="154" t="s">
+      <c r="G33" s="149"/>
+      <c r="H33" s="147"/>
+      <c r="I33" s="147"/>
+      <c r="J33" s="135"/>
+    </row>
+    <row r="34" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="133"/>
+      <c r="B34" s="146" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="147"/>
+      <c r="D34" s="144"/>
+      <c r="E34" s="154"/>
+      <c r="F34" s="148" t="s">
+        <v>107</v>
+      </c>
+      <c r="G34" s="149"/>
+      <c r="H34" s="147"/>
+      <c r="I34" s="147"/>
+      <c r="J34" s="135"/>
+    </row>
+    <row r="35" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="133"/>
+      <c r="B35" s="146" t="s">
         <v>106</v>
       </c>
-      <c r="C31" s="155"/>
-      <c r="D31" s="152"/>
-      <c r="E31" s="162"/>
-      <c r="F31" s="156" t="s">
-        <v>86</v>
-      </c>
-      <c r="G31" s="157"/>
-      <c r="H31" s="155"/>
-      <c r="I31" s="155"/>
-      <c r="J31" s="141"/>
-    </row>
-    <row r="32" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="139"/>
-      <c r="B32" s="154" t="s">
+      <c r="C35" s="147"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="154"/>
+      <c r="F35" s="148" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35" s="149"/>
+      <c r="H35" s="147"/>
+      <c r="I35" s="147"/>
+      <c r="J35" s="135"/>
+    </row>
+    <row r="36" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="133"/>
+      <c r="B36" s="146" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="155"/>
-      <c r="D32" s="152"/>
-      <c r="E32" s="162"/>
-      <c r="F32" s="156" t="s">
-        <v>104</v>
-      </c>
-      <c r="G32" s="157"/>
-      <c r="H32" s="155"/>
-      <c r="I32" s="155"/>
-      <c r="J32" s="141"/>
-    </row>
-    <row r="33" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="139"/>
-      <c r="B33" s="154" t="s">
+      <c r="C36" s="147"/>
+      <c r="D36" s="144"/>
+      <c r="E36" s="154"/>
+      <c r="F36" s="148" t="s">
+        <v>108</v>
+      </c>
+      <c r="G36" s="149"/>
+      <c r="H36" s="147"/>
+      <c r="I36" s="147"/>
+      <c r="J36" s="135"/>
+    </row>
+    <row r="37" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="133"/>
+      <c r="B37" s="146" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="155"/>
-      <c r="D33" s="152"/>
-      <c r="E33" s="162"/>
-      <c r="F33" s="156" t="s">
-        <v>105</v>
-      </c>
-      <c r="G33" s="157"/>
-      <c r="H33" s="155"/>
-      <c r="I33" s="155"/>
-      <c r="J33" s="141"/>
-    </row>
-    <row r="34" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="139"/>
-      <c r="B34" s="154" t="s">
+      <c r="C37" s="147"/>
+      <c r="D37" s="144"/>
+      <c r="E37" s="154"/>
+      <c r="F37" s="148" t="s">
+        <v>109</v>
+      </c>
+      <c r="G37" s="149"/>
+      <c r="H37" s="147"/>
+      <c r="I37" s="147"/>
+      <c r="J37" s="135"/>
+    </row>
+    <row r="38" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="133"/>
+      <c r="B38" s="146" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="155"/>
-      <c r="D34" s="152"/>
-      <c r="E34" s="162"/>
-      <c r="F34" s="156" t="s">
-        <v>107</v>
-      </c>
-      <c r="G34" s="157"/>
-      <c r="H34" s="155"/>
-      <c r="I34" s="155"/>
-      <c r="J34" s="141"/>
-    </row>
-    <row r="35" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="139"/>
-      <c r="B35" s="154" t="s">
+      <c r="C38" s="147"/>
+      <c r="D38" s="144"/>
+      <c r="E38" s="154"/>
+      <c r="F38" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="G38" s="149"/>
+      <c r="H38" s="147"/>
+      <c r="I38" s="147"/>
+      <c r="J38" s="135"/>
+    </row>
+    <row r="39" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="133"/>
+      <c r="B39" s="146" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="155"/>
-      <c r="D35" s="155"/>
-      <c r="E35" s="162"/>
-      <c r="F35" s="156" t="s">
+      <c r="C39" s="147"/>
+      <c r="D39" s="147"/>
+      <c r="E39" s="154"/>
+      <c r="F39" s="148" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39" s="149"/>
+      <c r="H39" s="147"/>
+      <c r="I39" s="147"/>
+      <c r="J39" s="135"/>
+    </row>
+    <row r="40" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="135"/>
+      <c r="B40" s="153" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="147"/>
+      <c r="D40" s="144"/>
+      <c r="E40" s="154"/>
+      <c r="F40" s="148" t="s">
+        <v>110</v>
+      </c>
+      <c r="G40" s="149"/>
+      <c r="H40" s="147"/>
+      <c r="I40" s="147"/>
+      <c r="J40" s="135"/>
+    </row>
+    <row r="41" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="135"/>
+      <c r="B41" s="155" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="147"/>
+      <c r="D41" s="144"/>
+      <c r="E41" s="154"/>
+      <c r="F41" s="148" t="s">
+        <v>90</v>
+      </c>
+      <c r="G41" s="149"/>
+      <c r="H41" s="147"/>
+      <c r="I41" s="147"/>
+      <c r="J41" s="135"/>
+    </row>
+    <row r="42" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="135"/>
+      <c r="B42" s="146" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="156"/>
+      <c r="D42" s="172"/>
+      <c r="E42" s="154"/>
+      <c r="F42" s="148" t="s">
+        <v>89</v>
+      </c>
+      <c r="G42" s="149"/>
+      <c r="H42" s="147"/>
+      <c r="I42" s="147"/>
+      <c r="J42" s="135"/>
+    </row>
+    <row r="43" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="135"/>
+      <c r="B43" s="146" t="s">
         <v>93</v>
       </c>
-      <c r="G35" s="157"/>
-      <c r="H35" s="155"/>
-      <c r="I35" s="155"/>
-      <c r="J35" s="141"/>
-    </row>
-    <row r="36" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="139"/>
-      <c r="B36" s="161" t="s">
-        <v>82</v>
-      </c>
-      <c r="C36" s="155"/>
-      <c r="D36" s="152"/>
-      <c r="E36" s="162"/>
-      <c r="F36" s="156" t="s">
-        <v>108</v>
-      </c>
-      <c r="G36" s="157"/>
-      <c r="H36" s="155"/>
-      <c r="I36" s="155"/>
-      <c r="J36" s="141"/>
-    </row>
-    <row r="37" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="139"/>
-      <c r="B37" s="163" t="s">
+      <c r="C43" s="156"/>
+      <c r="D43" s="172"/>
+      <c r="E43" s="154"/>
+      <c r="F43" s="148" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="155"/>
-      <c r="D37" s="152"/>
-      <c r="E37" s="162"/>
-      <c r="F37" s="156" t="s">
-        <v>109</v>
-      </c>
-      <c r="G37" s="157"/>
-      <c r="H37" s="155"/>
-      <c r="I37" s="155"/>
-      <c r="J37" s="141"/>
-    </row>
-    <row r="38" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="139"/>
-      <c r="B38" s="154" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" s="164"/>
-      <c r="D38" s="180"/>
-      <c r="E38" s="162"/>
-      <c r="F38" s="156" t="s">
+      <c r="G43" s="149"/>
+      <c r="H43" s="147"/>
+      <c r="I43" s="147"/>
+      <c r="J43" s="135"/>
+    </row>
+    <row r="44" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="135"/>
+      <c r="B44" s="146" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" s="156"/>
+      <c r="D44" s="172"/>
+      <c r="E44" s="154"/>
+      <c r="F44" s="148" t="s">
+        <v>111</v>
+      </c>
+      <c r="G44" s="149"/>
+      <c r="H44" s="145"/>
+      <c r="I44" s="147"/>
+      <c r="J44" s="135"/>
+    </row>
+    <row r="45" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="135"/>
+      <c r="B45" s="146" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="156"/>
+      <c r="D45" s="172"/>
+      <c r="E45" s="154"/>
+      <c r="F45" s="148" t="s">
+        <v>112</v>
+      </c>
+      <c r="G45" s="149"/>
+      <c r="H45" s="145"/>
+      <c r="I45" s="147"/>
+      <c r="J45" s="135"/>
+    </row>
+    <row r="46" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="135"/>
+      <c r="B46" s="146" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="156"/>
+      <c r="D46" s="172"/>
+      <c r="E46" s="154"/>
+      <c r="F46" s="148" t="s">
+        <v>113</v>
+      </c>
+      <c r="G46" s="149"/>
+      <c r="H46" s="145"/>
+      <c r="I46" s="147"/>
+      <c r="J46" s="135"/>
+    </row>
+    <row r="47" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="135"/>
+      <c r="B47" s="155" t="s">
         <v>96</v>
       </c>
-      <c r="G38" s="157"/>
-      <c r="H38" s="155"/>
-      <c r="I38" s="155"/>
-      <c r="J38" s="141"/>
-    </row>
-    <row r="39" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="139"/>
-      <c r="B39" s="154" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="164"/>
-      <c r="D39" s="180"/>
-      <c r="E39" s="162"/>
-      <c r="F39" s="156" t="s">
-        <v>106</v>
-      </c>
-      <c r="G39" s="157"/>
-      <c r="H39" s="155"/>
-      <c r="I39" s="155"/>
-      <c r="J39" s="141"/>
-    </row>
-    <row r="40" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="141"/>
-      <c r="B40" s="154" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" s="164"/>
-      <c r="D40" s="180"/>
-      <c r="E40" s="162"/>
-      <c r="F40" s="156" t="s">
-        <v>110</v>
-      </c>
-      <c r="G40" s="157"/>
-      <c r="H40" s="155"/>
-      <c r="I40" s="155"/>
-      <c r="J40" s="141"/>
-    </row>
-    <row r="41" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="141"/>
-      <c r="B41" s="154" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" s="164"/>
-      <c r="D41" s="180"/>
-      <c r="E41" s="162"/>
-      <c r="F41" s="161" t="s">
-        <v>90</v>
-      </c>
-      <c r="G41" s="157"/>
-      <c r="H41" s="155"/>
-      <c r="I41" s="155"/>
-      <c r="J41" s="141"/>
-    </row>
-    <row r="42" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="141"/>
-      <c r="B42" s="154" t="s">
-        <v>95</v>
-      </c>
-      <c r="C42" s="164"/>
-      <c r="D42" s="180"/>
-      <c r="E42" s="162"/>
-      <c r="F42" s="161" t="s">
-        <v>89</v>
-      </c>
-      <c r="G42" s="157"/>
-      <c r="H42" s="155"/>
-      <c r="I42" s="155"/>
-      <c r="J42" s="141"/>
-    </row>
-    <row r="43" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="141"/>
-      <c r="B43" s="166" t="s">
-        <v>96</v>
-      </c>
-      <c r="C43" s="167"/>
-      <c r="D43" s="181"/>
-      <c r="E43" s="162"/>
-      <c r="F43" s="161" t="s">
-        <v>91</v>
-      </c>
-      <c r="G43" s="157"/>
-      <c r="H43" s="155"/>
-      <c r="I43" s="155"/>
-      <c r="J43" s="141"/>
-    </row>
-    <row r="44" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="141"/>
-      <c r="B44" s="168" t="s">
+      <c r="C47" s="156"/>
+      <c r="D47" s="172"/>
+      <c r="E47" s="154"/>
+      <c r="F47" s="148" t="s">
+        <v>114</v>
+      </c>
+      <c r="G47" s="164"/>
+      <c r="H47" s="145"/>
+      <c r="I47" s="147"/>
+      <c r="J47" s="135"/>
+    </row>
+    <row r="48" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="135"/>
+      <c r="B48" s="155" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="155"/>
+      <c r="D48" s="155"/>
+      <c r="E48" s="154"/>
+      <c r="F48" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="176">
-        <f>SUM(C27:C43)</f>
-        <v>0</v>
-      </c>
-      <c r="D44" s="176"/>
-      <c r="E44" s="162"/>
-      <c r="F44" s="161" t="s">
-        <v>111</v>
-      </c>
-      <c r="G44" s="157"/>
-      <c r="H44" s="153"/>
-      <c r="I44" s="155"/>
-      <c r="J44" s="141"/>
-    </row>
-    <row r="45" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="141"/>
-      <c r="B45" s="170" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="155">
-        <f>C44*16%</f>
-        <v>0</v>
-      </c>
-      <c r="D45" s="153"/>
-      <c r="E45" s="162"/>
-      <c r="F45" s="161" t="s">
-        <v>112</v>
-      </c>
-      <c r="G45" s="157"/>
-      <c r="H45" s="153"/>
-      <c r="I45" s="155"/>
-      <c r="J45" s="141"/>
-    </row>
-    <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="141"/>
-      <c r="B46" s="173" t="s">
-        <v>1</v>
-      </c>
-      <c r="C46" s="174">
-        <f>SUM(C44:C45)</f>
-        <v>0</v>
-      </c>
-      <c r="D46" s="174"/>
-      <c r="E46" s="162"/>
-      <c r="F46" s="161" t="s">
-        <v>113</v>
-      </c>
-      <c r="G46" s="157"/>
-      <c r="H46" s="153"/>
-      <c r="I46" s="155"/>
-      <c r="J46" s="141"/>
-    </row>
-    <row r="47" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="141"/>
-      <c r="B47" s="139"/>
-      <c r="C47" s="139"/>
-      <c r="D47" s="139"/>
-      <c r="E47" s="162"/>
-      <c r="F47" s="171" t="s">
-        <v>114</v>
-      </c>
-      <c r="G47" s="172"/>
-      <c r="H47" s="153"/>
-      <c r="I47" s="155"/>
-      <c r="J47" s="141"/>
-    </row>
-    <row r="48" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="141"/>
-      <c r="B48" s="162"/>
-      <c r="C48" s="162"/>
-      <c r="D48" s="162"/>
-      <c r="E48" s="162"/>
-      <c r="F48" s="168" t="s">
-        <v>0</v>
-      </c>
-      <c r="G48" s="175"/>
-      <c r="H48" s="176">
+      <c r="G48" s="167"/>
+      <c r="H48" s="168">
         <f>SUM(H29:H47)</f>
         <v>0</v>
       </c>
-      <c r="I48" s="176">
+      <c r="I48" s="168">
         <f>SUM(I41:I47)</f>
         <v>0</v>
       </c>
-      <c r="J48" s="141"/>
+      <c r="J48" s="135"/>
     </row>
     <row r="49" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="141"/>
-      <c r="B49" s="162"/>
-      <c r="C49" s="162"/>
-      <c r="D49" s="162"/>
-      <c r="E49" s="162"/>
-      <c r="F49" s="170" t="s">
+      <c r="A49" s="135"/>
+      <c r="B49" s="157" t="s">
+        <v>112</v>
+      </c>
+      <c r="C49" s="157"/>
+      <c r="D49" s="157"/>
+      <c r="E49" s="154"/>
+      <c r="F49" s="162" t="s">
         <v>83</v>
       </c>
-      <c r="G49" s="177"/>
-      <c r="H49" s="155">
+      <c r="G49" s="169"/>
+      <c r="H49" s="147">
         <f>H48*16%</f>
         <v>0</v>
       </c>
-      <c r="I49" s="155">
+      <c r="I49" s="147">
         <f>I48*16%</f>
         <v>0</v>
       </c>
-      <c r="J49" s="141"/>
+      <c r="J49" s="135"/>
     </row>
     <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="141"/>
-      <c r="B50" s="162"/>
-      <c r="C50" s="162"/>
-      <c r="D50" s="162"/>
-      <c r="E50" s="162"/>
-      <c r="F50" s="173" t="s">
+      <c r="A50" s="135"/>
+      <c r="B50" s="157" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" s="157"/>
+      <c r="D50" s="157"/>
+      <c r="E50" s="154"/>
+      <c r="F50" s="165" t="s">
         <v>1</v>
       </c>
-      <c r="G50" s="178">
+      <c r="G50" s="170">
         <f>SUM(G29:G49)</f>
         <v>0</v>
       </c>
-      <c r="H50" s="174">
+      <c r="H50" s="166">
         <f>SUM(H48:H49)</f>
         <v>0</v>
       </c>
-      <c r="I50" s="174">
+      <c r="I50" s="166">
         <f>SUM(I48:I49)</f>
         <v>0</v>
       </c>
-      <c r="J50" s="141"/>
+      <c r="J50" s="135"/>
+    </row>
+    <row r="51" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="158" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="158"/>
+      <c r="D51" s="158"/>
+    </row>
+    <row r="52" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="B52" s="160" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="168">
+        <f>SUM(C31:C51)</f>
+        <v>0</v>
+      </c>
+      <c r="D52" s="168"/>
+    </row>
+    <row r="53" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="B53" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="C53" s="147">
+        <f>C52*16%</f>
+        <v>0</v>
+      </c>
+      <c r="D53" s="145"/>
+    </row>
+    <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B54" s="165" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="166">
+        <f>SUM(C52:C53)</f>
+        <v>0</v>
+      </c>
+      <c r="D54" s="166"/>
+    </row>
+    <row r="55" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="B55" s="133"/>
+      <c r="C55" s="133"/>
+      <c r="D55" s="133"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B56" s="154"/>
+      <c r="C56" s="154"/>
+      <c r="D56" s="154"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B57" s="154"/>
+      <c r="C57" s="154"/>
+      <c r="D57" s="154"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B58" s="154"/>
+      <c r="C58" s="154"/>
+      <c r="D58" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -12774,4 +12990,156 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="173"/>
+    <col min="2" max="2" width="37" style="173" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" style="173" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="173" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" style="173" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="173" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="173"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="177" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="177" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="177" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="177" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="177" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="177" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E2" s="174"/>
+      <c r="G2" s="178">
+        <f>E2+F2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E3" s="174"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E4" s="174"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="174"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="175"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="174"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="174"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="174"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="175"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="174"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="174"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="174"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="175"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="174"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="174"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="174"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="174"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="174"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="175"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="174"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="174"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="174"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="175"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="174"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="174"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="174"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="175"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="174"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="174"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="174"/>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="175"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="174"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="176"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:G1">
+    <sortState ref="B2:G2">
+      <sortCondition ref="C1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ultimos cambios 06 diciembre
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10995" tabRatio="789"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10995" tabRatio="789" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="NOMINA TOTAL" sheetId="27" r:id="rId1"/>
@@ -5123,7 +5123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BG12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
@@ -5934,15 +5934,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="T11:T12"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="Z11:Z12"/>
-    <mergeCell ref="Y11:Y12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
     <mergeCell ref="AD11:AD12"/>
     <mergeCell ref="AC11:AC12"/>
     <mergeCell ref="G11:G12"/>
@@ -5959,6 +5950,15 @@
     <mergeCell ref="AB11:AB12"/>
     <mergeCell ref="P11:P12"/>
     <mergeCell ref="S11:S12"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="Z11:Z12"/>
+    <mergeCell ref="Y11:Y12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12059,8 +12059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12417,7 +12417,7 @@
         <v>96</v>
       </c>
       <c r="C22" s="156"/>
-      <c r="D22" s="156"/>
+      <c r="D22" s="147"/>
       <c r="E22" s="154"/>
       <c r="F22" s="157" t="s">
         <v>112</v>
@@ -12433,7 +12433,7 @@
         <v>111</v>
       </c>
       <c r="C23" s="156"/>
-      <c r="D23" s="156"/>
+      <c r="D23" s="147"/>
       <c r="E23" s="154"/>
       <c r="F23" s="157" t="s">
         <v>113</v>
@@ -12449,7 +12449,7 @@
         <v>112</v>
       </c>
       <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
+      <c r="D24" s="147"/>
       <c r="E24" s="154"/>
       <c r="F24" s="163" t="s">
         <v>114</v>
@@ -12465,7 +12465,7 @@
         <v>113</v>
       </c>
       <c r="C25" s="157"/>
-      <c r="D25" s="157"/>
+      <c r="D25" s="147"/>
       <c r="E25" s="154"/>
       <c r="F25" s="160" t="s">
         <v>0</v>
@@ -12487,7 +12487,7 @@
         <v>121</v>
       </c>
       <c r="C26" s="159"/>
-      <c r="D26" s="159"/>
+      <c r="D26" s="147"/>
       <c r="E26" s="154"/>
       <c r="F26" s="162" t="s">
         <v>83</v>
@@ -12512,7 +12512,10 @@
         <f>SUM(C6:C26)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="161"/>
+      <c r="D27" s="161">
+        <f>SUM(D6:D26)</f>
+        <v>0</v>
+      </c>
       <c r="E27" s="154"/>
       <c r="F27" s="165" t="s">
         <v>1</v>
@@ -12540,7 +12543,10 @@
         <f>C27*16%</f>
         <v>0</v>
       </c>
-      <c r="D28" s="147"/>
+      <c r="D28" s="147">
+        <f>D27*16%</f>
+        <v>0</v>
+      </c>
       <c r="E28" s="154"/>
       <c r="F28" s="143" t="s">
         <v>84</v>
@@ -12559,7 +12565,10 @@
         <f>SUM(C27:C28)</f>
         <v>0</v>
       </c>
-      <c r="D29" s="166"/>
+      <c r="D29" s="166">
+        <f>SUM(D27:D28)</f>
+        <v>0</v>
+      </c>
       <c r="E29" s="154"/>
       <c r="F29" s="148" t="s">
         <v>85</v>
@@ -12847,7 +12856,7 @@
         <v>96</v>
       </c>
       <c r="C47" s="156"/>
-      <c r="D47" s="172"/>
+      <c r="D47" s="156"/>
       <c r="E47" s="154"/>
       <c r="F47" s="148" t="s">
         <v>114</v>
@@ -12863,7 +12872,7 @@
         <v>111</v>
       </c>
       <c r="C48" s="155"/>
-      <c r="D48" s="155"/>
+      <c r="D48" s="156"/>
       <c r="E48" s="154"/>
       <c r="F48" s="160" t="s">
         <v>0</v>
@@ -12885,7 +12894,7 @@
         <v>112</v>
       </c>
       <c r="C49" s="157"/>
-      <c r="D49" s="157"/>
+      <c r="D49" s="156"/>
       <c r="E49" s="154"/>
       <c r="F49" s="162" t="s">
         <v>83</v>
@@ -12907,7 +12916,7 @@
         <v>113</v>
       </c>
       <c r="C50" s="157"/>
-      <c r="D50" s="157"/>
+      <c r="D50" s="156"/>
       <c r="E50" s="154"/>
       <c r="F50" s="165" t="s">
         <v>1</v>
@@ -12931,7 +12940,7 @@
         <v>121</v>
       </c>
       <c r="C51" s="158"/>
-      <c r="D51" s="158"/>
+      <c r="D51" s="156"/>
     </row>
     <row r="52" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B52" s="160" t="s">
@@ -12941,7 +12950,10 @@
         <f>SUM(C31:C51)</f>
         <v>0</v>
       </c>
-      <c r="D52" s="168"/>
+      <c r="D52" s="168">
+        <f>SUM(D31:D51)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B53" s="162" t="s">
@@ -12951,7 +12963,10 @@
         <f>C52*16%</f>
         <v>0</v>
       </c>
-      <c r="D53" s="145"/>
+      <c r="D53" s="147">
+        <f>D52*16%</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B54" s="165" t="s">
@@ -12961,7 +12976,10 @@
         <f>SUM(C52:C53)</f>
         <v>0</v>
       </c>
-      <c r="D54" s="166"/>
+      <c r="D54" s="166">
+        <f>SUM(D52:D53)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B55" s="133"/>

</xml_diff>

<commit_message>
Cmabios en buscar y reportes con el CS en descanso
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10995" tabRatio="789" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7755" tabRatio="789" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NOMINA TOTAL" sheetId="27" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="122">
   <si>
     <t>SUBTOTAL</t>
   </si>
@@ -785,7 +785,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -954,6 +954,54 @@
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF0000FD"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF0000FD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2451,7 +2499,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2820,6 +2868,24 @@
     </xf>
     <xf numFmtId="43" fontId="33" fillId="0" borderId="0" xfId="1488" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="42" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="203" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="13" xfId="203" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="14" xfId="1318" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="15" xfId="1318" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="15" xfId="1318" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="16" xfId="1318" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5139,7 +5205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BG12"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="V1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
@@ -5776,83 +5842,83 @@
       <c r="BG10" s="50"/>
     </row>
     <row r="11" spans="2:59" s="85" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="180" t="s">
+      <c r="B11" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="180" t="s">
+      <c r="C11" s="186" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="180" t="s">
+      <c r="D11" s="186" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="180" t="s">
+      <c r="E11" s="186" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="180" t="s">
+      <c r="F11" s="186" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="180" t="s">
+      <c r="G11" s="186" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="180" t="s">
+      <c r="H11" s="186" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="180" t="s">
+      <c r="I11" s="186" t="s">
         <v>71</v>
       </c>
-      <c r="J11" s="180" t="s">
+      <c r="J11" s="186" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="180" t="s">
+      <c r="K11" s="186" t="s">
         <v>59</v>
       </c>
-      <c r="L11" s="180" t="s">
+      <c r="L11" s="186" t="s">
         <v>4</v>
       </c>
-      <c r="M11" s="180" t="s">
+      <c r="M11" s="186" t="s">
         <v>62</v>
       </c>
-      <c r="N11" s="180" t="s">
+      <c r="N11" s="186" t="s">
         <v>72</v>
       </c>
       <c r="O11" s="129"/>
-      <c r="P11" s="180" t="s">
+      <c r="P11" s="186" t="s">
         <v>52</v>
       </c>
       <c r="Q11" s="132"/>
       <c r="R11" s="132"/>
-      <c r="S11" s="180" t="s">
+      <c r="S11" s="186" t="s">
         <v>58</v>
       </c>
-      <c r="T11" s="180" t="s">
+      <c r="T11" s="186" t="s">
         <v>17</v>
       </c>
-      <c r="U11" s="180" t="s">
+      <c r="U11" s="186" t="s">
         <v>19</v>
       </c>
-      <c r="V11" s="180" t="s">
+      <c r="V11" s="186" t="s">
         <v>73</v>
       </c>
       <c r="W11" s="86"/>
-      <c r="X11" s="180" t="s">
+      <c r="X11" s="186" t="s">
         <v>74</v>
       </c>
-      <c r="Y11" s="180" t="s">
+      <c r="Y11" s="186" t="s">
         <v>75</v>
       </c>
-      <c r="Z11" s="180" t="s">
+      <c r="Z11" s="186" t="s">
         <v>5</v>
       </c>
-      <c r="AA11" s="180" t="s">
+      <c r="AA11" s="186" t="s">
         <v>0</v>
       </c>
-      <c r="AB11" s="181" t="s">
+      <c r="AB11" s="187" t="s">
         <v>20</v>
       </c>
-      <c r="AC11" s="180" t="s">
+      <c r="AC11" s="186" t="s">
         <v>1</v>
       </c>
-      <c r="AD11" s="180"/>
+      <c r="AD11" s="186"/>
       <c r="AF11" s="84"/>
       <c r="AG11" s="84"/>
       <c r="AH11" s="84"/>
@@ -5882,23 +5948,23 @@
       <c r="BF11" s="84"/>
     </row>
     <row r="12" spans="2:59" s="87" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="180"/>
-      <c r="C12" s="180"/>
-      <c r="D12" s="180"/>
-      <c r="E12" s="180"/>
-      <c r="F12" s="180"/>
-      <c r="G12" s="180"/>
-      <c r="H12" s="180"/>
-      <c r="I12" s="180"/>
-      <c r="J12" s="180"/>
-      <c r="K12" s="180"/>
-      <c r="L12" s="180"/>
-      <c r="M12" s="180"/>
-      <c r="N12" s="180"/>
+      <c r="B12" s="186"/>
+      <c r="C12" s="186"/>
+      <c r="D12" s="186"/>
+      <c r="E12" s="186"/>
+      <c r="F12" s="186"/>
+      <c r="G12" s="186"/>
+      <c r="H12" s="186"/>
+      <c r="I12" s="186"/>
+      <c r="J12" s="186"/>
+      <c r="K12" s="186"/>
+      <c r="L12" s="186"/>
+      <c r="M12" s="186"/>
+      <c r="N12" s="186"/>
       <c r="O12" s="129" t="s">
         <v>76</v>
       </c>
-      <c r="P12" s="180" t="s">
+      <c r="P12" s="186" t="s">
         <v>63</v>
       </c>
       <c r="Q12" s="132" t="s">
@@ -5907,18 +5973,18 @@
       <c r="R12" s="132" t="s">
         <v>115</v>
       </c>
-      <c r="S12" s="180"/>
-      <c r="T12" s="180"/>
-      <c r="U12" s="180"/>
-      <c r="V12" s="180"/>
+      <c r="S12" s="186"/>
+      <c r="T12" s="186"/>
+      <c r="U12" s="186"/>
+      <c r="V12" s="186"/>
       <c r="W12" s="86"/>
-      <c r="X12" s="180"/>
-      <c r="Y12" s="180"/>
-      <c r="Z12" s="180"/>
-      <c r="AA12" s="180"/>
-      <c r="AB12" s="181"/>
-      <c r="AC12" s="180"/>
-      <c r="AD12" s="180"/>
+      <c r="X12" s="186"/>
+      <c r="Y12" s="186"/>
+      <c r="Z12" s="186"/>
+      <c r="AA12" s="186"/>
+      <c r="AB12" s="187"/>
+      <c r="AC12" s="186"/>
+      <c r="AD12" s="186"/>
       <c r="AE12" s="88"/>
       <c r="AF12" s="89"/>
       <c r="AG12" s="89"/>
@@ -5986,7 +6052,7 @@
   <dimension ref="A1:KB47"/>
   <sheetViews>
     <sheetView topLeftCell="AM1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AQ8" sqref="AQ8"/>
+      <selection activeCell="BE4" sqref="BE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6031,13 +6097,13 @@
   <sheetData>
     <row r="1" spans="1:288" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="27"/>
-      <c r="B1" s="182" t="s">
+      <c r="B1" s="188" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
-      <c r="F1" s="183"/>
+      <c r="C1" s="189"/>
+      <c r="D1" s="189"/>
+      <c r="E1" s="189"/>
+      <c r="F1" s="189"/>
       <c r="G1" s="65"/>
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
@@ -6135,13 +6201,13 @@
     </row>
     <row r="3" spans="1:288" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="190" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="183"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="183"/>
-      <c r="F3" s="183"/>
+      <c r="C3" s="189"/>
+      <c r="D3" s="189"/>
+      <c r="E3" s="189"/>
+      <c r="F3" s="189"/>
       <c r="G3" s="67"/>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
@@ -6193,13 +6259,13 @@
     </row>
     <row r="4" spans="1:288" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
-      <c r="B4" s="185" t="s">
+      <c r="B4" s="191" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="186"/>
-      <c r="D4" s="186"/>
-      <c r="E4" s="186"/>
-      <c r="F4" s="186"/>
+      <c r="C4" s="192"/>
+      <c r="D4" s="192"/>
+      <c r="E4" s="192"/>
+      <c r="F4" s="192"/>
       <c r="G4" s="67"/>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
@@ -6624,28 +6690,28 @@
       <c r="AO8" s="128" t="s">
         <v>115</v>
       </c>
-      <c r="AP8" s="127" t="s">
+      <c r="AP8" s="180" t="s">
         <v>53</v>
       </c>
-      <c r="AQ8" s="130" t="s">
+      <c r="AQ8" s="182" t="s">
         <v>28</v>
       </c>
-      <c r="AR8" s="130" t="s">
+      <c r="AR8" s="183" t="s">
         <v>67</v>
       </c>
-      <c r="AS8" s="130" t="s">
+      <c r="AS8" s="183" t="s">
         <v>10</v>
       </c>
-      <c r="AT8" s="130" t="s">
+      <c r="AT8" s="183" t="s">
         <v>68</v>
       </c>
-      <c r="AU8" s="131" t="s">
+      <c r="AU8" s="184" t="s">
         <v>69</v>
       </c>
-      <c r="AV8" s="130" t="s">
+      <c r="AV8" s="185" t="s">
         <v>70</v>
       </c>
-      <c r="AW8" s="128" t="s">
+      <c r="AW8" s="181" t="s">
         <v>99</v>
       </c>
       <c r="AX8" s="128" t="s">
@@ -6977,12 +7043,15 @@
       <c r="AQ10" s="48"/>
       <c r="AR10" s="48"/>
       <c r="AS10" s="48"/>
-      <c r="AT10" s="48"/>
-      <c r="AU10" s="48"/>
-      <c r="AV10" s="54"/>
-      <c r="AW10" s="79"/>
-      <c r="AX10" s="79"/>
-      <c r="AY10" s="79"/>
+      <c r="AT10" s="83"/>
+      <c r="AU10" s="83"/>
+      <c r="AV10" s="83"/>
+      <c r="AW10" s="83"/>
+      <c r="AX10" s="83"/>
+      <c r="AY10" s="83"/>
+      <c r="AZ10" s="83"/>
+      <c r="BA10" s="83"/>
+      <c r="BB10" s="83"/>
     </row>
     <row r="11" spans="1:288" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="49"/>
@@ -7024,9 +7093,15 @@
       <c r="AQ11" s="103"/>
       <c r="AR11" s="103"/>
       <c r="AS11" s="103"/>
-      <c r="AT11" s="103"/>
-      <c r="AU11" s="103"/>
+      <c r="AT11" s="83"/>
+      <c r="AU11" s="83"/>
       <c r="AV11" s="83"/>
+      <c r="AW11" s="83"/>
+      <c r="AX11" s="83"/>
+      <c r="AY11" s="83"/>
+      <c r="AZ11" s="83"/>
+      <c r="BA11" s="83"/>
+      <c r="BB11" s="83"/>
     </row>
     <row r="12" spans="1:288" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="46"/>
@@ -7074,12 +7149,15 @@
       <c r="AQ12" s="48"/>
       <c r="AR12" s="48"/>
       <c r="AS12" s="48"/>
-      <c r="AT12" s="48"/>
-      <c r="AU12" s="48"/>
-      <c r="AV12" s="54"/>
-      <c r="AW12" s="79"/>
-      <c r="AX12" s="79"/>
-      <c r="AY12" s="79"/>
+      <c r="AT12" s="83"/>
+      <c r="AU12" s="83"/>
+      <c r="AV12" s="83"/>
+      <c r="AW12" s="83"/>
+      <c r="AX12" s="83"/>
+      <c r="AY12" s="83"/>
+      <c r="AZ12" s="83"/>
+      <c r="BA12" s="83"/>
+      <c r="BB12" s="83"/>
     </row>
     <row r="13" spans="1:288" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="46"/>
@@ -7127,11 +7205,15 @@
       <c r="AQ13" s="48"/>
       <c r="AR13" s="48"/>
       <c r="AS13" s="48"/>
-      <c r="AT13" s="48"/>
-      <c r="AU13" s="48"/>
-      <c r="AW13" s="79"/>
-      <c r="AX13" s="79"/>
-      <c r="AY13" s="79"/>
+      <c r="AT13" s="83"/>
+      <c r="AU13" s="83"/>
+      <c r="AV13" s="83"/>
+      <c r="AW13" s="83"/>
+      <c r="AX13" s="83"/>
+      <c r="AY13" s="83"/>
+      <c r="AZ13" s="83"/>
+      <c r="BA13" s="83"/>
+      <c r="BB13" s="83"/>
     </row>
     <row r="14" spans="1:288" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="46"/>
@@ -7179,11 +7261,15 @@
       <c r="AQ14" s="48"/>
       <c r="AR14" s="48"/>
       <c r="AS14" s="48"/>
-      <c r="AT14" s="48"/>
-      <c r="AU14" s="48"/>
-      <c r="AW14" s="79"/>
-      <c r="AX14" s="79"/>
-      <c r="AY14" s="79"/>
+      <c r="AT14" s="83"/>
+      <c r="AU14" s="83"/>
+      <c r="AV14" s="83"/>
+      <c r="AW14" s="83"/>
+      <c r="AX14" s="83"/>
+      <c r="AY14" s="83"/>
+      <c r="AZ14" s="83"/>
+      <c r="BA14" s="83"/>
+      <c r="BB14" s="83"/>
     </row>
     <row r="15" spans="1:288" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="46"/>
@@ -7231,11 +7317,15 @@
       <c r="AQ15" s="48"/>
       <c r="AR15" s="48"/>
       <c r="AS15" s="48"/>
-      <c r="AT15" s="48"/>
-      <c r="AU15" s="48"/>
-      <c r="AW15" s="79"/>
-      <c r="AX15" s="79"/>
-      <c r="AY15" s="79"/>
+      <c r="AT15" s="83"/>
+      <c r="AU15" s="83"/>
+      <c r="AV15" s="83"/>
+      <c r="AW15" s="83"/>
+      <c r="AX15" s="83"/>
+      <c r="AY15" s="83"/>
+      <c r="AZ15" s="83"/>
+      <c r="BA15" s="83"/>
+      <c r="BB15" s="83"/>
     </row>
     <row r="16" spans="1:288" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="46"/>
@@ -7283,13 +7373,17 @@
       <c r="AQ16" s="48"/>
       <c r="AR16" s="48"/>
       <c r="AS16" s="48"/>
-      <c r="AT16" s="48"/>
-      <c r="AU16" s="48"/>
-      <c r="AW16" s="79"/>
-      <c r="AX16" s="79"/>
-      <c r="AY16" s="79"/>
-    </row>
-    <row r="17" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT16" s="83"/>
+      <c r="AU16" s="83"/>
+      <c r="AV16" s="83"/>
+      <c r="AW16" s="83"/>
+      <c r="AX16" s="83"/>
+      <c r="AY16" s="83"/>
+      <c r="AZ16" s="83"/>
+      <c r="BA16" s="83"/>
+      <c r="BB16" s="83"/>
+    </row>
+    <row r="17" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="46"/>
       <c r="B17" s="38"/>
       <c r="C17" s="69"/>
@@ -7335,13 +7429,17 @@
       <c r="AQ17" s="48"/>
       <c r="AR17" s="48"/>
       <c r="AS17" s="48"/>
-      <c r="AT17" s="48"/>
-      <c r="AU17" s="48"/>
-      <c r="AW17" s="79"/>
-      <c r="AX17" s="79"/>
-      <c r="AY17" s="79"/>
-    </row>
-    <row r="18" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT17" s="83"/>
+      <c r="AU17" s="83"/>
+      <c r="AV17" s="83"/>
+      <c r="AW17" s="83"/>
+      <c r="AX17" s="83"/>
+      <c r="AY17" s="83"/>
+      <c r="AZ17" s="83"/>
+      <c r="BA17" s="83"/>
+      <c r="BB17" s="83"/>
+    </row>
+    <row r="18" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="46"/>
       <c r="B18" s="38"/>
       <c r="C18" s="69"/>
@@ -7387,13 +7485,17 @@
       <c r="AQ18" s="48"/>
       <c r="AR18" s="48"/>
       <c r="AS18" s="48"/>
-      <c r="AT18" s="48"/>
-      <c r="AU18" s="48"/>
-      <c r="AW18" s="79"/>
-      <c r="AX18" s="79"/>
-      <c r="AY18" s="79"/>
-    </row>
-    <row r="19" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT18" s="83"/>
+      <c r="AU18" s="83"/>
+      <c r="AV18" s="83"/>
+      <c r="AW18" s="83"/>
+      <c r="AX18" s="83"/>
+      <c r="AY18" s="83"/>
+      <c r="AZ18" s="83"/>
+      <c r="BA18" s="83"/>
+      <c r="BB18" s="83"/>
+    </row>
+    <row r="19" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="39"/>
       <c r="B19" s="38"/>
       <c r="C19" s="69"/>
@@ -7439,13 +7541,17 @@
       <c r="AQ19" s="48"/>
       <c r="AR19" s="48"/>
       <c r="AS19" s="48"/>
-      <c r="AT19" s="48"/>
-      <c r="AU19" s="48"/>
-      <c r="AW19" s="79"/>
-      <c r="AX19" s="79"/>
-      <c r="AY19" s="79"/>
-    </row>
-    <row r="20" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT19" s="83"/>
+      <c r="AU19" s="83"/>
+      <c r="AV19" s="83"/>
+      <c r="AW19" s="83"/>
+      <c r="AX19" s="83"/>
+      <c r="AY19" s="83"/>
+      <c r="AZ19" s="83"/>
+      <c r="BA19" s="83"/>
+      <c r="BB19" s="83"/>
+    </row>
+    <row r="20" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="26"/>
       <c r="B20" s="25"/>
       <c r="C20" s="69"/>
@@ -7491,10 +7597,17 @@
       <c r="AQ20" s="48"/>
       <c r="AR20" s="48"/>
       <c r="AS20" s="48"/>
-      <c r="AT20" s="48"/>
-      <c r="AU20" s="48"/>
-    </row>
-    <row r="21" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT20" s="83"/>
+      <c r="AU20" s="83"/>
+      <c r="AV20" s="83"/>
+      <c r="AW20" s="83"/>
+      <c r="AX20" s="83"/>
+      <c r="AY20" s="83"/>
+      <c r="AZ20" s="83"/>
+      <c r="BA20" s="83"/>
+      <c r="BB20" s="83"/>
+    </row>
+    <row r="21" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="26"/>
       <c r="B21" s="25"/>
       <c r="C21" s="69"/>
@@ -7540,10 +7653,17 @@
       <c r="AQ21" s="48"/>
       <c r="AR21" s="48"/>
       <c r="AS21" s="48"/>
-      <c r="AT21" s="48"/>
-      <c r="AU21" s="48"/>
-    </row>
-    <row r="22" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT21" s="83"/>
+      <c r="AU21" s="83"/>
+      <c r="AV21" s="83"/>
+      <c r="AW21" s="83"/>
+      <c r="AX21" s="83"/>
+      <c r="AY21" s="83"/>
+      <c r="AZ21" s="83"/>
+      <c r="BA21" s="83"/>
+      <c r="BB21" s="83"/>
+    </row>
+    <row r="22" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="26"/>
       <c r="B22" s="25"/>
       <c r="C22" s="69"/>
@@ -7589,10 +7709,17 @@
       <c r="AQ22" s="48"/>
       <c r="AR22" s="48"/>
       <c r="AS22" s="48"/>
-      <c r="AT22" s="48"/>
-      <c r="AU22" s="48"/>
-    </row>
-    <row r="23" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT22" s="83"/>
+      <c r="AU22" s="83"/>
+      <c r="AV22" s="83"/>
+      <c r="AW22" s="83"/>
+      <c r="AX22" s="83"/>
+      <c r="AY22" s="83"/>
+      <c r="AZ22" s="83"/>
+      <c r="BA22" s="83"/>
+      <c r="BB22" s="83"/>
+    </row>
+    <row r="23" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="35"/>
       <c r="B23" s="30"/>
       <c r="C23" s="67"/>
@@ -7638,10 +7765,17 @@
       <c r="AQ23" s="48"/>
       <c r="AR23" s="48"/>
       <c r="AS23" s="48"/>
-      <c r="AT23" s="48"/>
-      <c r="AU23" s="48"/>
-    </row>
-    <row r="24" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AT23" s="83"/>
+      <c r="AU23" s="83"/>
+      <c r="AV23" s="83"/>
+      <c r="AW23" s="83"/>
+      <c r="AX23" s="83"/>
+      <c r="AY23" s="83"/>
+      <c r="AZ23" s="83"/>
+      <c r="BA23" s="83"/>
+      <c r="BB23" s="83"/>
+    </row>
+    <row r="24" spans="1:54" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
       <c r="B24" s="24"/>
       <c r="C24" s="70"/>
@@ -7687,10 +7821,17 @@
       <c r="AQ24" s="48"/>
       <c r="AR24" s="48"/>
       <c r="AS24" s="48"/>
-      <c r="AT24" s="48"/>
-      <c r="AU24" s="48"/>
-    </row>
-    <row r="25" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AT24" s="83"/>
+      <c r="AU24" s="83"/>
+      <c r="AV24" s="83"/>
+      <c r="AW24" s="83"/>
+      <c r="AX24" s="83"/>
+      <c r="AY24" s="83"/>
+      <c r="AZ24" s="83"/>
+      <c r="BA24" s="83"/>
+      <c r="BB24" s="83"/>
+    </row>
+    <row r="25" spans="1:54" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="19"/>
       <c r="C25" s="71"/>
@@ -7736,10 +7877,17 @@
       <c r="AQ25" s="19"/>
       <c r="AR25" s="19"/>
       <c r="AS25" s="19"/>
-      <c r="AT25" s="19"/>
-      <c r="AU25" s="19"/>
-    </row>
-    <row r="26" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AT25" s="83"/>
+      <c r="AU25" s="83"/>
+      <c r="AV25" s="83"/>
+      <c r="AW25" s="83"/>
+      <c r="AX25" s="83"/>
+      <c r="AY25" s="83"/>
+      <c r="AZ25" s="83"/>
+      <c r="BA25" s="83"/>
+      <c r="BB25" s="83"/>
+    </row>
+    <row r="26" spans="1:54" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="31"/>
       <c r="B26" s="24"/>
       <c r="C26" s="65"/>
@@ -7785,10 +7933,17 @@
       <c r="AQ26" s="24"/>
       <c r="AR26" s="24"/>
       <c r="AS26" s="24"/>
-      <c r="AT26" s="24"/>
-      <c r="AU26" s="24"/>
-    </row>
-    <row r="27" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT26" s="83"/>
+      <c r="AU26" s="83"/>
+      <c r="AV26" s="83"/>
+      <c r="AW26" s="83"/>
+      <c r="AX26" s="83"/>
+      <c r="AY26" s="83"/>
+      <c r="AZ26" s="83"/>
+      <c r="BA26" s="83"/>
+      <c r="BB26" s="83"/>
+    </row>
+    <row r="27" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="26"/>
       <c r="B27" s="25"/>
       <c r="C27" s="69"/>
@@ -7834,10 +7989,17 @@
       <c r="AQ27" s="40"/>
       <c r="AR27" s="40"/>
       <c r="AS27" s="40"/>
-      <c r="AT27" s="40"/>
-      <c r="AU27" s="40"/>
-    </row>
-    <row r="28" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT27" s="83"/>
+      <c r="AU27" s="83"/>
+      <c r="AV27" s="83"/>
+      <c r="AW27" s="83"/>
+      <c r="AX27" s="83"/>
+      <c r="AY27" s="83"/>
+      <c r="AZ27" s="83"/>
+      <c r="BA27" s="83"/>
+      <c r="BB27" s="83"/>
+    </row>
+    <row r="28" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="26"/>
       <c r="B28" s="25"/>
       <c r="C28" s="69"/>
@@ -7883,10 +8045,17 @@
       <c r="AQ28" s="40"/>
       <c r="AR28" s="40"/>
       <c r="AS28" s="40"/>
-      <c r="AT28" s="40"/>
-      <c r="AU28" s="40"/>
-    </row>
-    <row r="29" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT28" s="83"/>
+      <c r="AU28" s="83"/>
+      <c r="AV28" s="83"/>
+      <c r="AW28" s="83"/>
+      <c r="AX28" s="83"/>
+      <c r="AY28" s="83"/>
+      <c r="AZ28" s="83"/>
+      <c r="BA28" s="83"/>
+      <c r="BB28" s="83"/>
+    </row>
+    <row r="29" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="35"/>
       <c r="B29" s="30"/>
       <c r="C29" s="67"/>
@@ -7932,10 +8101,17 @@
       <c r="AQ29" s="30"/>
       <c r="AR29" s="30"/>
       <c r="AS29" s="30"/>
-      <c r="AT29" s="30"/>
-      <c r="AU29" s="30"/>
-    </row>
-    <row r="30" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AT29" s="83"/>
+      <c r="AU29" s="83"/>
+      <c r="AV29" s="83"/>
+      <c r="AW29" s="83"/>
+      <c r="AX29" s="83"/>
+      <c r="AY29" s="83"/>
+      <c r="AZ29" s="83"/>
+      <c r="BA29" s="83"/>
+      <c r="BB29" s="83"/>
+    </row>
+    <row r="30" spans="1:54" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" s="24"/>
       <c r="C30" s="70"/>
@@ -7981,10 +8157,17 @@
       <c r="AQ30" s="36"/>
       <c r="AR30" s="36"/>
       <c r="AS30" s="36"/>
-      <c r="AT30" s="36"/>
-      <c r="AU30" s="36"/>
-    </row>
-    <row r="31" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AT30" s="83"/>
+      <c r="AU30" s="83"/>
+      <c r="AV30" s="83"/>
+      <c r="AW30" s="83"/>
+      <c r="AX30" s="83"/>
+      <c r="AY30" s="83"/>
+      <c r="AZ30" s="83"/>
+      <c r="BA30" s="83"/>
+      <c r="BB30" s="83"/>
+    </row>
+    <row r="31" spans="1:54" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="72"/>
@@ -8030,10 +8213,17 @@
       <c r="AQ31" s="22"/>
       <c r="AR31" s="22"/>
       <c r="AS31" s="22"/>
-      <c r="AT31" s="22"/>
-      <c r="AU31" s="22"/>
-    </row>
-    <row r="32" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AT31" s="83"/>
+      <c r="AU31" s="83"/>
+      <c r="AV31" s="83"/>
+      <c r="AW31" s="83"/>
+      <c r="AX31" s="83"/>
+      <c r="AY31" s="83"/>
+      <c r="AZ31" s="83"/>
+      <c r="BA31" s="83"/>
+      <c r="BB31" s="83"/>
+    </row>
+    <row r="32" spans="1:54" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
       <c r="B32" s="24"/>
       <c r="C32" s="65"/>
@@ -8079,10 +8269,17 @@
       <c r="AQ32" s="24"/>
       <c r="AR32" s="24"/>
       <c r="AS32" s="24"/>
-      <c r="AT32" s="24"/>
-      <c r="AU32" s="24"/>
-    </row>
-    <row r="33" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT32" s="83"/>
+      <c r="AU32" s="83"/>
+      <c r="AV32" s="83"/>
+      <c r="AW32" s="83"/>
+      <c r="AX32" s="83"/>
+      <c r="AY32" s="83"/>
+      <c r="AZ32" s="83"/>
+      <c r="BA32" s="83"/>
+      <c r="BB32" s="83"/>
+    </row>
+    <row r="33" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="26"/>
       <c r="B33" s="25"/>
       <c r="C33" s="69"/>
@@ -8128,10 +8325,17 @@
       <c r="AQ33" s="40"/>
       <c r="AR33" s="40"/>
       <c r="AS33" s="40"/>
-      <c r="AT33" s="40"/>
-      <c r="AU33" s="40"/>
-    </row>
-    <row r="34" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT33" s="83"/>
+      <c r="AU33" s="83"/>
+      <c r="AV33" s="83"/>
+      <c r="AW33" s="83"/>
+      <c r="AX33" s="83"/>
+      <c r="AY33" s="83"/>
+      <c r="AZ33" s="83"/>
+      <c r="BA33" s="83"/>
+      <c r="BB33" s="83"/>
+    </row>
+    <row r="34" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="26"/>
       <c r="B34" s="25"/>
       <c r="C34" s="69"/>
@@ -8177,10 +8381,17 @@
       <c r="AQ34" s="40"/>
       <c r="AR34" s="40"/>
       <c r="AS34" s="40"/>
-      <c r="AT34" s="40"/>
-      <c r="AU34" s="40"/>
-    </row>
-    <row r="35" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT34" s="83"/>
+      <c r="AU34" s="83"/>
+      <c r="AV34" s="83"/>
+      <c r="AW34" s="83"/>
+      <c r="AX34" s="83"/>
+      <c r="AY34" s="83"/>
+      <c r="AZ34" s="83"/>
+      <c r="BA34" s="83"/>
+      <c r="BB34" s="83"/>
+    </row>
+    <row r="35" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="35"/>
       <c r="B35" s="30"/>
       <c r="C35" s="67"/>
@@ -8226,10 +8437,17 @@
       <c r="AQ35" s="30"/>
       <c r="AR35" s="30"/>
       <c r="AS35" s="30"/>
-      <c r="AT35" s="30"/>
-      <c r="AU35" s="30"/>
-    </row>
-    <row r="36" spans="1:47" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AT35" s="83"/>
+      <c r="AU35" s="83"/>
+      <c r="AV35" s="83"/>
+      <c r="AW35" s="83"/>
+      <c r="AX35" s="83"/>
+      <c r="AY35" s="83"/>
+      <c r="AZ35" s="83"/>
+      <c r="BA35" s="83"/>
+      <c r="BB35" s="83"/>
+    </row>
+    <row r="36" spans="1:54" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
       <c r="B36" s="24"/>
       <c r="C36" s="70"/>
@@ -8275,10 +8493,17 @@
       <c r="AQ36" s="36"/>
       <c r="AR36" s="36"/>
       <c r="AS36" s="36"/>
-      <c r="AT36" s="36"/>
-      <c r="AU36" s="36"/>
-    </row>
-    <row r="37" spans="1:47" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AT36" s="83"/>
+      <c r="AU36" s="83"/>
+      <c r="AV36" s="83"/>
+      <c r="AW36" s="83"/>
+      <c r="AX36" s="83"/>
+      <c r="AY36" s="83"/>
+      <c r="AZ36" s="83"/>
+      <c r="BA36" s="83"/>
+      <c r="BB36" s="83"/>
+    </row>
+    <row r="37" spans="1:54" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="72"/>
@@ -8324,10 +8549,17 @@
       <c r="AQ37" s="22"/>
       <c r="AR37" s="22"/>
       <c r="AS37" s="22"/>
-      <c r="AT37" s="22"/>
-      <c r="AU37" s="22"/>
-    </row>
-    <row r="38" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+      <c r="AT37" s="83"/>
+      <c r="AU37" s="83"/>
+      <c r="AV37" s="83"/>
+      <c r="AW37" s="83"/>
+      <c r="AX37" s="83"/>
+      <c r="AY37" s="83"/>
+      <c r="AZ37" s="83"/>
+      <c r="BA37" s="83"/>
+      <c r="BB37" s="83"/>
+    </row>
+    <row r="38" spans="1:54" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
       <c r="B38" s="24"/>
       <c r="C38" s="65"/>
@@ -8373,10 +8605,17 @@
       <c r="AQ38" s="24"/>
       <c r="AR38" s="24"/>
       <c r="AS38" s="24"/>
-      <c r="AT38" s="24"/>
-      <c r="AU38" s="24"/>
-    </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AT38" s="83"/>
+      <c r="AU38" s="83"/>
+      <c r="AV38" s="83"/>
+      <c r="AW38" s="83"/>
+      <c r="AX38" s="83"/>
+      <c r="AY38" s="83"/>
+      <c r="AZ38" s="83"/>
+      <c r="BA38" s="83"/>
+      <c r="BB38" s="83"/>
+    </row>
+    <row r="39" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A39" s="26"/>
       <c r="B39" s="25"/>
       <c r="C39" s="69"/>
@@ -8422,10 +8661,17 @@
       <c r="AQ39" s="40"/>
       <c r="AR39" s="40"/>
       <c r="AS39" s="40"/>
-      <c r="AT39" s="40"/>
-      <c r="AU39" s="40"/>
-    </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AT39" s="83"/>
+      <c r="AU39" s="83"/>
+      <c r="AV39" s="83"/>
+      <c r="AW39" s="83"/>
+      <c r="AX39" s="83"/>
+      <c r="AY39" s="83"/>
+      <c r="AZ39" s="83"/>
+      <c r="BA39" s="83"/>
+      <c r="BB39" s="83"/>
+    </row>
+    <row r="40" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A40" s="26"/>
       <c r="B40" s="25"/>
       <c r="C40" s="69"/>
@@ -8471,10 +8717,17 @@
       <c r="AQ40" s="40"/>
       <c r="AR40" s="40"/>
       <c r="AS40" s="40"/>
-      <c r="AT40" s="40"/>
-      <c r="AU40" s="40"/>
-    </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AT40" s="83"/>
+      <c r="AU40" s="83"/>
+      <c r="AV40" s="83"/>
+      <c r="AW40" s="83"/>
+      <c r="AX40" s="83"/>
+      <c r="AY40" s="83"/>
+      <c r="AZ40" s="83"/>
+      <c r="BA40" s="83"/>
+      <c r="BB40" s="83"/>
+    </row>
+    <row r="41" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A41" s="35"/>
       <c r="B41" s="30"/>
       <c r="C41" s="67"/>
@@ -8520,10 +8773,17 @@
       <c r="AQ41" s="30"/>
       <c r="AR41" s="30"/>
       <c r="AS41" s="30"/>
-      <c r="AT41" s="30"/>
-      <c r="AU41" s="30"/>
-    </row>
-    <row r="42" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+      <c r="AT41" s="83"/>
+      <c r="AU41" s="83"/>
+      <c r="AV41" s="83"/>
+      <c r="AW41" s="83"/>
+      <c r="AX41" s="83"/>
+      <c r="AY41" s="83"/>
+      <c r="AZ41" s="83"/>
+      <c r="BA41" s="83"/>
+      <c r="BB41" s="83"/>
+    </row>
+    <row r="42" spans="1:54" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="24"/>
       <c r="C42" s="70"/>
@@ -8572,7 +8832,7 @@
       <c r="AT42" s="36"/>
       <c r="AU42" s="36"/>
     </row>
-    <row r="43" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:54" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
       <c r="B43" s="21"/>
       <c r="C43" s="72"/>
@@ -8621,7 +8881,7 @@
       <c r="AT43" s="22"/>
       <c r="AU43" s="22"/>
     </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A44" s="34"/>
       <c r="B44" s="30"/>
       <c r="C44" s="67"/>
@@ -8670,7 +8930,7 @@
       <c r="AT44" s="30"/>
       <c r="AU44" s="30"/>
     </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A45" s="35"/>
       <c r="B45" s="25"/>
       <c r="C45" s="70"/>
@@ -8719,7 +8979,7 @@
       <c r="AT45" s="36"/>
       <c r="AU45" s="36"/>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:54" x14ac:dyDescent="0.2">
       <c r="X47" s="8"/>
       <c r="AE47" s="8"/>
       <c r="AF47" s="8"/>
@@ -8738,10 +8998,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CQ59"/>
+  <dimension ref="A1:CW59"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AN12" sqref="AN12"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AT11" sqref="AT11:AZ51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8778,19 +9038,21 @@
     <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="13.42578125" customWidth="1"/>
     <col min="42" max="42" width="11.42578125" style="10"/>
-    <col min="43" max="45" width="0" style="10" hidden="1" customWidth="1"/>
-    <col min="46" max="52" width="11.42578125" style="10"/>
+    <col min="43" max="47" width="14.28515625" customWidth="1"/>
+    <col min="48" max="48" width="12.28515625" customWidth="1"/>
+    <col min="49" max="51" width="11.42578125" style="10" hidden="1" customWidth="1"/>
+    <col min="52" max="58" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:101" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="27"/>
-      <c r="B1" s="182" t="s">
+      <c r="B1" s="188" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
-      <c r="F1" s="183"/>
+      <c r="C1" s="189"/>
+      <c r="D1" s="189"/>
+      <c r="E1" s="189"/>
+      <c r="F1" s="189"/>
       <c r="G1" s="24"/>
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
@@ -8826,8 +9088,13 @@
       <c r="AM1" s="24"/>
       <c r="AN1" s="24"/>
       <c r="AO1" s="24"/>
-    </row>
-    <row r="2" spans="1:95" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="24"/>
+      <c r="AT1" s="24"/>
+      <c r="AU1" s="24"/>
+    </row>
+    <row r="2" spans="1:101" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="51" t="s">
         <v>23</v>
@@ -8871,16 +9138,21 @@
       <c r="AM2" s="24"/>
       <c r="AN2" s="24"/>
       <c r="AO2" s="24"/>
-    </row>
-    <row r="3" spans="1:95" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AQ2" s="24"/>
+      <c r="AR2" s="24"/>
+      <c r="AS2" s="24"/>
+      <c r="AT2" s="24"/>
+      <c r="AU2" s="24"/>
+    </row>
+    <row r="3" spans="1:101" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="190" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="183"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="183"/>
-      <c r="F3" s="183"/>
+      <c r="C3" s="189"/>
+      <c r="D3" s="189"/>
+      <c r="E3" s="189"/>
+      <c r="F3" s="189"/>
       <c r="G3" s="30"/>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
@@ -8917,26 +9189,31 @@
       <c r="AN3" s="24"/>
       <c r="AO3" s="24"/>
       <c r="AP3" s="110"/>
-      <c r="AQ3" s="110"/>
-      <c r="AR3" s="110"/>
-      <c r="AS3" s="110"/>
-      <c r="AT3" s="110"/>
-      <c r="AU3" s="110"/>
-      <c r="AV3" s="110"/>
+      <c r="AQ3" s="24"/>
+      <c r="AR3" s="24"/>
+      <c r="AS3" s="24"/>
+      <c r="AT3" s="24"/>
+      <c r="AU3" s="24"/>
       <c r="AW3" s="110"/>
       <c r="AX3" s="110"/>
       <c r="AY3" s="110"/>
       <c r="AZ3" s="110"/>
-    </row>
-    <row r="4" spans="1:95" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="BA3" s="110"/>
+      <c r="BB3" s="110"/>
+      <c r="BC3" s="110"/>
+      <c r="BD3" s="110"/>
+      <c r="BE3" s="110"/>
+      <c r="BF3" s="110"/>
+    </row>
+    <row r="4" spans="1:101" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
-      <c r="B4" s="185" t="s">
+      <c r="B4" s="191" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="186"/>
-      <c r="D4" s="186"/>
-      <c r="E4" s="186"/>
-      <c r="F4" s="186"/>
+      <c r="C4" s="192"/>
+      <c r="D4" s="192"/>
+      <c r="E4" s="192"/>
+      <c r="F4" s="192"/>
       <c r="G4" s="67"/>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
@@ -8972,8 +9249,13 @@
       <c r="AM4" s="24"/>
       <c r="AN4" s="24"/>
       <c r="AO4" s="24"/>
-    </row>
-    <row r="5" spans="1:95" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ4" s="24"/>
+      <c r="AR4" s="24"/>
+      <c r="AS4" s="24"/>
+      <c r="AT4" s="24"/>
+      <c r="AU4" s="24"/>
+    </row>
+    <row r="5" spans="1:101" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="29" t="s">
         <v>21</v>
@@ -9017,8 +9299,13 @@
       <c r="AM5" s="24"/>
       <c r="AN5" s="24"/>
       <c r="AO5" s="24"/>
-    </row>
-    <row r="6" spans="1:95" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ5" s="24"/>
+      <c r="AR5" s="24"/>
+      <c r="AS5" s="24"/>
+      <c r="AT5" s="24"/>
+      <c r="AU5" s="24"/>
+    </row>
+    <row r="6" spans="1:101" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="29" t="s">
         <v>22</v>
@@ -9062,12 +9349,12 @@
       <c r="AM6" s="24"/>
       <c r="AN6" s="24"/>
       <c r="AO6" s="24"/>
-      <c r="BA6"/>
-      <c r="BB6"/>
-      <c r="BC6"/>
-      <c r="BD6"/>
-      <c r="BE6"/>
-      <c r="BF6"/>
+      <c r="AQ6" s="24"/>
+      <c r="AR6" s="24"/>
+      <c r="AS6" s="24"/>
+      <c r="AT6" s="24"/>
+      <c r="AU6" s="24"/>
+      <c r="AV6"/>
       <c r="BG6"/>
       <c r="BH6"/>
       <c r="BI6"/>
@@ -9105,8 +9392,14 @@
       <c r="CO6"/>
       <c r="CP6"/>
       <c r="CQ6"/>
-    </row>
-    <row r="7" spans="1:95" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="CR6"/>
+      <c r="CS6"/>
+      <c r="CT6"/>
+      <c r="CU6"/>
+      <c r="CV6"/>
+      <c r="CW6"/>
+    </row>
+    <row r="7" spans="1:101" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
@@ -9135,22 +9428,17 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="18"/>
       <c r="AP7" s="110"/>
-      <c r="AQ7" s="110"/>
-      <c r="AR7" s="110"/>
-      <c r="AS7" s="110"/>
-      <c r="AT7" s="110"/>
-      <c r="AU7" s="110"/>
       <c r="AV7" s="110"/>
       <c r="AW7" s="110"/>
       <c r="AX7" s="110"/>
       <c r="AY7" s="110"/>
       <c r="AZ7" s="110"/>
-      <c r="BA7" s="9"/>
-      <c r="BB7" s="9"/>
-      <c r="BC7" s="9"/>
-      <c r="BD7" s="9"/>
-      <c r="BE7" s="9"/>
-      <c r="BF7" s="9"/>
+      <c r="BA7" s="110"/>
+      <c r="BB7" s="110"/>
+      <c r="BC7" s="110"/>
+      <c r="BD7" s="110"/>
+      <c r="BE7" s="110"/>
+      <c r="BF7" s="110"/>
       <c r="BG7" s="9"/>
       <c r="BH7" s="9"/>
       <c r="BI7" s="9"/>
@@ -9188,8 +9476,14 @@
       <c r="CO7" s="9"/>
       <c r="CP7" s="9"/>
       <c r="CQ7" s="9"/>
-    </row>
-    <row r="8" spans="1:95" s="45" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="CR7" s="9"/>
+      <c r="CS7" s="9"/>
+      <c r="CT7" s="9"/>
+      <c r="CU7" s="9"/>
+      <c r="CV7" s="9"/>
+      <c r="CW7" s="9"/>
+    </row>
+    <row r="8" spans="1:101" s="45" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
         <v>16</v>
       </c>
@@ -9316,21 +9610,33 @@
       <c r="AP8" s="127" t="s">
         <v>53</v>
       </c>
-      <c r="AQ8" s="128" t="s">
+      <c r="AQ8" s="130" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR8" s="130" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS8" s="130" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT8" s="130" t="s">
+        <v>68</v>
+      </c>
+      <c r="AU8" s="131" t="s">
+        <v>69</v>
+      </c>
+      <c r="AV8" s="130" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW8" s="128" t="s">
         <v>99</v>
       </c>
-      <c r="AR8" s="128" t="s">
+      <c r="AX8" s="128" t="s">
         <v>100</v>
       </c>
-      <c r="AS8" s="128" t="s">
+      <c r="AY8" s="128" t="s">
         <v>101</v>
       </c>
-      <c r="AT8" s="10"/>
-      <c r="AU8" s="10"/>
-      <c r="AV8" s="10"/>
-      <c r="AW8" s="10"/>
-      <c r="AX8" s="10"/>
-      <c r="AY8" s="10"/>
       <c r="AZ8" s="10"/>
       <c r="BA8" s="10"/>
       <c r="BB8" s="10"/>
@@ -9375,8 +9681,14 @@
       <c r="CO8" s="10"/>
       <c r="CP8" s="10"/>
       <c r="CQ8" s="10"/>
-    </row>
-    <row r="9" spans="1:95" s="79" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="CR8" s="10"/>
+      <c r="CS8" s="10"/>
+      <c r="CT8" s="10"/>
+      <c r="CU8" s="10"/>
+      <c r="CV8" s="10"/>
+      <c r="CW8" s="10"/>
+    </row>
+    <row r="9" spans="1:101" s="79" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="49"/>
       <c r="B9" s="5"/>
       <c r="C9" s="63"/>
@@ -9413,8 +9725,14 @@
       <c r="AL9" s="102"/>
       <c r="AM9" s="102"/>
       <c r="AN9" s="103"/>
-    </row>
-    <row r="10" spans="1:95" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ9" s="83"/>
+      <c r="AR9" s="83"/>
+      <c r="AS9" s="83"/>
+      <c r="AT9" s="83"/>
+      <c r="AU9" s="83"/>
+      <c r="AV9" s="83"/>
+    </row>
+    <row r="10" spans="1:101" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="49"/>
       <c r="B10" s="5"/>
       <c r="C10" s="63"/>
@@ -9452,8 +9770,14 @@
       <c r="AM10" s="102"/>
       <c r="AN10" s="103"/>
       <c r="AO10" s="119"/>
-    </row>
-    <row r="11" spans="1:95" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ10" s="48"/>
+      <c r="AR10" s="48"/>
+      <c r="AS10" s="48"/>
+      <c r="AT10" s="48"/>
+      <c r="AU10" s="48"/>
+      <c r="AV10" s="54"/>
+    </row>
+    <row r="11" spans="1:101" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="49"/>
       <c r="B11" s="5"/>
       <c r="C11" s="63"/>
@@ -9491,8 +9815,18 @@
       <c r="AM11" s="102"/>
       <c r="AN11" s="103"/>
       <c r="AO11" s="102"/>
-    </row>
-    <row r="12" spans="1:95" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ11" s="103"/>
+      <c r="AR11" s="103"/>
+      <c r="AS11" s="103"/>
+      <c r="AT11" s="48"/>
+      <c r="AU11" s="48"/>
+      <c r="AV11" s="48"/>
+      <c r="AW11" s="48"/>
+      <c r="AX11" s="48"/>
+      <c r="AY11" s="48"/>
+      <c r="AZ11" s="48"/>
+    </row>
+    <row r="12" spans="1:101" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
       <c r="B12" s="5"/>
       <c r="C12" s="63"/>
@@ -9530,8 +9864,18 @@
       <c r="AM12" s="102"/>
       <c r="AN12" s="103"/>
       <c r="AO12" s="48"/>
-    </row>
-    <row r="13" spans="1:95" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ12" s="48"/>
+      <c r="AR12" s="48"/>
+      <c r="AS12" s="48"/>
+      <c r="AT12" s="48"/>
+      <c r="AU12" s="48"/>
+      <c r="AV12" s="48"/>
+      <c r="AW12" s="48"/>
+      <c r="AX12" s="48"/>
+      <c r="AY12" s="48"/>
+      <c r="AZ12" s="48"/>
+    </row>
+    <row r="13" spans="1:101" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="5"/>
       <c r="C13" s="63"/>
@@ -9569,8 +9913,18 @@
       <c r="AM13" s="102"/>
       <c r="AN13" s="103"/>
       <c r="AO13" s="48"/>
-    </row>
-    <row r="14" spans="1:95" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ13" s="48"/>
+      <c r="AR13" s="48"/>
+      <c r="AS13" s="48"/>
+      <c r="AT13" s="48"/>
+      <c r="AU13" s="48"/>
+      <c r="AV13" s="48"/>
+      <c r="AW13" s="48"/>
+      <c r="AX13" s="48"/>
+      <c r="AY13" s="48"/>
+      <c r="AZ13" s="48"/>
+    </row>
+    <row r="14" spans="1:101" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="49"/>
       <c r="B14" s="5"/>
       <c r="C14" s="63"/>
@@ -9608,8 +9962,18 @@
       <c r="AM14" s="102"/>
       <c r="AN14" s="103"/>
       <c r="AO14" s="48"/>
-    </row>
-    <row r="15" spans="1:95" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ14" s="48"/>
+      <c r="AR14" s="48"/>
+      <c r="AS14" s="48"/>
+      <c r="AT14" s="48"/>
+      <c r="AU14" s="48"/>
+      <c r="AV14" s="48"/>
+      <c r="AW14" s="48"/>
+      <c r="AX14" s="48"/>
+      <c r="AY14" s="48"/>
+      <c r="AZ14" s="48"/>
+    </row>
+    <row r="15" spans="1:101" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="49"/>
       <c r="B15" s="5"/>
       <c r="C15" s="63"/>
@@ -9647,8 +10011,18 @@
       <c r="AM15" s="102"/>
       <c r="AN15" s="103"/>
       <c r="AO15" s="48"/>
-    </row>
-    <row r="16" spans="1:95" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ15" s="48"/>
+      <c r="AR15" s="48"/>
+      <c r="AS15" s="48"/>
+      <c r="AT15" s="48"/>
+      <c r="AU15" s="48"/>
+      <c r="AV15" s="48"/>
+      <c r="AW15" s="48"/>
+      <c r="AX15" s="48"/>
+      <c r="AY15" s="48"/>
+      <c r="AZ15" s="48"/>
+    </row>
+    <row r="16" spans="1:101" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="49"/>
       <c r="B16" s="5"/>
       <c r="C16" s="63"/>
@@ -9686,8 +10060,18 @@
       <c r="AM16" s="102"/>
       <c r="AN16" s="103"/>
       <c r="AO16" s="48"/>
-    </row>
-    <row r="17" spans="1:41" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ16" s="48"/>
+      <c r="AR16" s="48"/>
+      <c r="AS16" s="48"/>
+      <c r="AT16" s="48"/>
+      <c r="AU16" s="48"/>
+      <c r="AV16" s="48"/>
+      <c r="AW16" s="48"/>
+      <c r="AX16" s="48"/>
+      <c r="AY16" s="48"/>
+      <c r="AZ16" s="48"/>
+    </row>
+    <row r="17" spans="1:52" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="49"/>
       <c r="B17" s="5"/>
       <c r="C17" s="63"/>
@@ -9725,8 +10109,18 @@
       <c r="AM17" s="102"/>
       <c r="AN17" s="103"/>
       <c r="AO17" s="48"/>
-    </row>
-    <row r="18" spans="1:41" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ17" s="48"/>
+      <c r="AR17" s="48"/>
+      <c r="AS17" s="48"/>
+      <c r="AT17" s="48"/>
+      <c r="AU17" s="48"/>
+      <c r="AV17" s="48"/>
+      <c r="AW17" s="48"/>
+      <c r="AX17" s="48"/>
+      <c r="AY17" s="48"/>
+      <c r="AZ17" s="48"/>
+    </row>
+    <row r="18" spans="1:52" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="49"/>
       <c r="B18" s="5"/>
       <c r="C18" s="63"/>
@@ -9763,8 +10157,18 @@
       <c r="AM18" s="102"/>
       <c r="AN18" s="103"/>
       <c r="AO18" s="48"/>
-    </row>
-    <row r="19" spans="1:41" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ18" s="48"/>
+      <c r="AR18" s="48"/>
+      <c r="AS18" s="48"/>
+      <c r="AT18" s="48"/>
+      <c r="AU18" s="48"/>
+      <c r="AV18" s="48"/>
+      <c r="AW18" s="48"/>
+      <c r="AX18" s="48"/>
+      <c r="AY18" s="48"/>
+      <c r="AZ18" s="48"/>
+    </row>
+    <row r="19" spans="1:52" s="79" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="49"/>
       <c r="B19" s="5"/>
       <c r="C19" s="63"/>
@@ -9800,8 +10204,18 @@
       <c r="AM19" s="102"/>
       <c r="AN19" s="103"/>
       <c r="AO19" s="48"/>
-    </row>
-    <row r="20" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ19" s="48"/>
+      <c r="AR19" s="48"/>
+      <c r="AS19" s="48"/>
+      <c r="AT19" s="48"/>
+      <c r="AU19" s="48"/>
+      <c r="AV19" s="48"/>
+      <c r="AW19" s="48"/>
+      <c r="AX19" s="48"/>
+      <c r="AY19" s="48"/>
+      <c r="AZ19" s="48"/>
+    </row>
+    <row r="20" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="46"/>
       <c r="B20" s="38"/>
       <c r="C20" s="40"/>
@@ -9843,8 +10257,19 @@
       <c r="AM20" s="54"/>
       <c r="AN20" s="54"/>
       <c r="AO20" s="48"/>
-    </row>
-    <row r="21" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AP20" s="79"/>
+      <c r="AQ20" s="48"/>
+      <c r="AR20" s="48"/>
+      <c r="AS20" s="48"/>
+      <c r="AT20" s="48"/>
+      <c r="AU20" s="48"/>
+      <c r="AV20" s="48"/>
+      <c r="AW20" s="48"/>
+      <c r="AX20" s="48"/>
+      <c r="AY20" s="48"/>
+      <c r="AZ20" s="48"/>
+    </row>
+    <row r="21" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="46"/>
       <c r="B21" s="38"/>
       <c r="C21" s="40"/>
@@ -9886,8 +10311,18 @@
       <c r="AM21" s="48"/>
       <c r="AN21" s="48"/>
       <c r="AO21" s="48"/>
-    </row>
-    <row r="22" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ21" s="48"/>
+      <c r="AR21" s="48"/>
+      <c r="AS21" s="48"/>
+      <c r="AT21" s="48"/>
+      <c r="AU21" s="48"/>
+      <c r="AV21" s="48"/>
+      <c r="AW21" s="48"/>
+      <c r="AX21" s="48"/>
+      <c r="AY21" s="48"/>
+      <c r="AZ21" s="48"/>
+    </row>
+    <row r="22" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="46"/>
       <c r="B22" s="38"/>
       <c r="C22" s="40"/>
@@ -9929,8 +10364,18 @@
       <c r="AM22" s="48"/>
       <c r="AN22" s="48"/>
       <c r="AO22" s="48"/>
-    </row>
-    <row r="23" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ22" s="48"/>
+      <c r="AR22" s="48"/>
+      <c r="AS22" s="48"/>
+      <c r="AT22" s="48"/>
+      <c r="AU22" s="48"/>
+      <c r="AV22" s="48"/>
+      <c r="AW22" s="48"/>
+      <c r="AX22" s="48"/>
+      <c r="AY22" s="48"/>
+      <c r="AZ22" s="48"/>
+    </row>
+    <row r="23" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="46"/>
       <c r="B23" s="38"/>
       <c r="C23" s="40"/>
@@ -9972,8 +10417,18 @@
       <c r="AM23" s="48"/>
       <c r="AN23" s="48"/>
       <c r="AO23" s="48"/>
-    </row>
-    <row r="24" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ23" s="48"/>
+      <c r="AR23" s="48"/>
+      <c r="AS23" s="48"/>
+      <c r="AT23" s="48"/>
+      <c r="AU23" s="48"/>
+      <c r="AV23" s="48"/>
+      <c r="AW23" s="48"/>
+      <c r="AX23" s="48"/>
+      <c r="AY23" s="48"/>
+      <c r="AZ23" s="48"/>
+    </row>
+    <row r="24" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="46"/>
       <c r="B24" s="38"/>
       <c r="C24" s="40"/>
@@ -10015,8 +10470,18 @@
       <c r="AM24" s="48"/>
       <c r="AN24" s="48"/>
       <c r="AO24" s="48"/>
-    </row>
-    <row r="25" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ24" s="48"/>
+      <c r="AR24" s="48"/>
+      <c r="AS24" s="48"/>
+      <c r="AT24" s="48"/>
+      <c r="AU24" s="48"/>
+      <c r="AV24" s="48"/>
+      <c r="AW24" s="48"/>
+      <c r="AX24" s="48"/>
+      <c r="AY24" s="48"/>
+      <c r="AZ24" s="48"/>
+    </row>
+    <row r="25" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
       <c r="B25" s="38"/>
       <c r="C25" s="40"/>
@@ -10058,8 +10523,18 @@
       <c r="AM25" s="48"/>
       <c r="AN25" s="48"/>
       <c r="AO25" s="19"/>
-    </row>
-    <row r="26" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ25" s="19"/>
+      <c r="AR25" s="19"/>
+      <c r="AS25" s="19"/>
+      <c r="AT25" s="48"/>
+      <c r="AU25" s="48"/>
+      <c r="AV25" s="48"/>
+      <c r="AW25" s="48"/>
+      <c r="AX25" s="48"/>
+      <c r="AY25" s="48"/>
+      <c r="AZ25" s="48"/>
+    </row>
+    <row r="26" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="46"/>
       <c r="B26" s="38"/>
       <c r="C26" s="40"/>
@@ -10101,8 +10576,18 @@
       <c r="AM26" s="48"/>
       <c r="AN26" s="48"/>
       <c r="AO26" s="24"/>
-    </row>
-    <row r="27" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ26" s="24"/>
+      <c r="AR26" s="24"/>
+      <c r="AS26" s="24"/>
+      <c r="AT26" s="48"/>
+      <c r="AU26" s="48"/>
+      <c r="AV26" s="48"/>
+      <c r="AW26" s="48"/>
+      <c r="AX26" s="48"/>
+      <c r="AY26" s="48"/>
+      <c r="AZ26" s="48"/>
+    </row>
+    <row r="27" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="46"/>
       <c r="B27" s="38"/>
       <c r="C27" s="40"/>
@@ -10144,8 +10629,18 @@
       <c r="AM27" s="48"/>
       <c r="AN27" s="48"/>
       <c r="AO27" s="40"/>
-    </row>
-    <row r="28" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ27" s="40"/>
+      <c r="AR27" s="40"/>
+      <c r="AS27" s="40"/>
+      <c r="AT27" s="48"/>
+      <c r="AU27" s="48"/>
+      <c r="AV27" s="48"/>
+      <c r="AW27" s="48"/>
+      <c r="AX27" s="48"/>
+      <c r="AY27" s="48"/>
+      <c r="AZ27" s="48"/>
+    </row>
+    <row r="28" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="46"/>
       <c r="B28" s="38"/>
       <c r="C28" s="40"/>
@@ -10187,8 +10682,18 @@
       <c r="AM28" s="48"/>
       <c r="AN28" s="48"/>
       <c r="AO28" s="40"/>
-    </row>
-    <row r="29" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ28" s="40"/>
+      <c r="AR28" s="40"/>
+      <c r="AS28" s="40"/>
+      <c r="AT28" s="48"/>
+      <c r="AU28" s="48"/>
+      <c r="AV28" s="48"/>
+      <c r="AW28" s="48"/>
+      <c r="AX28" s="48"/>
+      <c r="AY28" s="48"/>
+      <c r="AZ28" s="48"/>
+    </row>
+    <row r="29" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="46"/>
       <c r="B29" s="38"/>
       <c r="C29" s="40"/>
@@ -10230,8 +10735,18 @@
       <c r="AM29" s="48"/>
       <c r="AN29" s="48"/>
       <c r="AO29" s="30"/>
-    </row>
-    <row r="30" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ29" s="30"/>
+      <c r="AR29" s="30"/>
+      <c r="AS29" s="30"/>
+      <c r="AT29" s="48"/>
+      <c r="AU29" s="48"/>
+      <c r="AV29" s="48"/>
+      <c r="AW29" s="48"/>
+      <c r="AX29" s="48"/>
+      <c r="AY29" s="48"/>
+      <c r="AZ29" s="48"/>
+    </row>
+    <row r="30" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="46"/>
       <c r="B30" s="38"/>
       <c r="C30" s="40"/>
@@ -10273,8 +10788,18 @@
       <c r="AM30" s="48"/>
       <c r="AN30" s="48"/>
       <c r="AO30" s="36"/>
-    </row>
-    <row r="31" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ30" s="36"/>
+      <c r="AR30" s="36"/>
+      <c r="AS30" s="36"/>
+      <c r="AT30" s="48"/>
+      <c r="AU30" s="48"/>
+      <c r="AV30" s="48"/>
+      <c r="AW30" s="48"/>
+      <c r="AX30" s="48"/>
+      <c r="AY30" s="48"/>
+      <c r="AZ30" s="48"/>
+    </row>
+    <row r="31" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="39"/>
       <c r="B31" s="38"/>
       <c r="C31" s="40"/>
@@ -10316,8 +10841,18 @@
       <c r="AM31" s="48"/>
       <c r="AN31" s="48"/>
       <c r="AO31" s="22"/>
-    </row>
-    <row r="32" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ31" s="22"/>
+      <c r="AR31" s="22"/>
+      <c r="AS31" s="22"/>
+      <c r="AT31" s="48"/>
+      <c r="AU31" s="48"/>
+      <c r="AV31" s="48"/>
+      <c r="AW31" s="48"/>
+      <c r="AX31" s="48"/>
+      <c r="AY31" s="48"/>
+      <c r="AZ31" s="48"/>
+    </row>
+    <row r="32" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="39"/>
       <c r="B32" s="38"/>
       <c r="C32" s="40"/>
@@ -10359,8 +10894,18 @@
       <c r="AM32" s="48"/>
       <c r="AN32" s="48"/>
       <c r="AO32" s="24"/>
-    </row>
-    <row r="33" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ32" s="24"/>
+      <c r="AR32" s="24"/>
+      <c r="AS32" s="24"/>
+      <c r="AT32" s="48"/>
+      <c r="AU32" s="48"/>
+      <c r="AV32" s="48"/>
+      <c r="AW32" s="48"/>
+      <c r="AX32" s="48"/>
+      <c r="AY32" s="48"/>
+      <c r="AZ32" s="48"/>
+    </row>
+    <row r="33" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="39"/>
       <c r="B33" s="38"/>
       <c r="C33" s="40"/>
@@ -10402,8 +10947,18 @@
       <c r="AM33" s="48"/>
       <c r="AN33" s="48"/>
       <c r="AO33" s="40"/>
-    </row>
-    <row r="34" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ33" s="40"/>
+      <c r="AR33" s="40"/>
+      <c r="AS33" s="40"/>
+      <c r="AT33" s="48"/>
+      <c r="AU33" s="48"/>
+      <c r="AV33" s="48"/>
+      <c r="AW33" s="48"/>
+      <c r="AX33" s="48"/>
+      <c r="AY33" s="48"/>
+      <c r="AZ33" s="48"/>
+    </row>
+    <row r="34" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="39"/>
       <c r="B34" s="38"/>
       <c r="C34" s="40"/>
@@ -10445,8 +11000,18 @@
       <c r="AM34" s="48"/>
       <c r="AN34" s="48"/>
       <c r="AO34" s="40"/>
-    </row>
-    <row r="35" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ34" s="40"/>
+      <c r="AR34" s="40"/>
+      <c r="AS34" s="40"/>
+      <c r="AT34" s="48"/>
+      <c r="AU34" s="48"/>
+      <c r="AV34" s="48"/>
+      <c r="AW34" s="48"/>
+      <c r="AX34" s="48"/>
+      <c r="AY34" s="48"/>
+      <c r="AZ34" s="48"/>
+    </row>
+    <row r="35" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="35"/>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
@@ -10488,8 +11053,18 @@
       <c r="AM35" s="48"/>
       <c r="AN35" s="48"/>
       <c r="AO35" s="30"/>
-    </row>
-    <row r="36" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ35" s="30"/>
+      <c r="AR35" s="30"/>
+      <c r="AS35" s="30"/>
+      <c r="AT35" s="48"/>
+      <c r="AU35" s="48"/>
+      <c r="AV35" s="48"/>
+      <c r="AW35" s="48"/>
+      <c r="AX35" s="48"/>
+      <c r="AY35" s="48"/>
+      <c r="AZ35" s="48"/>
+    </row>
+    <row r="36" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
       <c r="B36" s="24"/>
       <c r="C36" s="36"/>
@@ -10531,8 +11106,18 @@
       <c r="AM36" s="48"/>
       <c r="AN36" s="48"/>
       <c r="AO36" s="36"/>
-    </row>
-    <row r="37" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ36" s="36"/>
+      <c r="AR36" s="36"/>
+      <c r="AS36" s="36"/>
+      <c r="AT36" s="48"/>
+      <c r="AU36" s="48"/>
+      <c r="AV36" s="48"/>
+      <c r="AW36" s="48"/>
+      <c r="AX36" s="48"/>
+      <c r="AY36" s="48"/>
+      <c r="AZ36" s="48"/>
+    </row>
+    <row r="37" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
@@ -10574,8 +11159,18 @@
       <c r="AM37" s="19"/>
       <c r="AN37" s="19"/>
       <c r="AO37" s="22"/>
-    </row>
-    <row r="38" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ37" s="22"/>
+      <c r="AR37" s="22"/>
+      <c r="AS37" s="22"/>
+      <c r="AT37" s="48"/>
+      <c r="AU37" s="48"/>
+      <c r="AV37" s="48"/>
+      <c r="AW37" s="48"/>
+      <c r="AX37" s="48"/>
+      <c r="AY37" s="48"/>
+      <c r="AZ37" s="48"/>
+    </row>
+    <row r="38" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
       <c r="B38" s="24"/>
       <c r="C38" s="24"/>
@@ -10617,8 +11212,18 @@
       <c r="AM38" s="24"/>
       <c r="AN38" s="24"/>
       <c r="AO38" s="24"/>
-    </row>
-    <row r="39" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ38" s="24"/>
+      <c r="AR38" s="24"/>
+      <c r="AS38" s="24"/>
+      <c r="AT38" s="48"/>
+      <c r="AU38" s="48"/>
+      <c r="AV38" s="48"/>
+      <c r="AW38" s="48"/>
+      <c r="AX38" s="48"/>
+      <c r="AY38" s="48"/>
+      <c r="AZ38" s="48"/>
+    </row>
+    <row r="39" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="39"/>
       <c r="B39" s="38"/>
       <c r="C39" s="40"/>
@@ -10660,8 +11265,18 @@
       <c r="AM39" s="40"/>
       <c r="AN39" s="40"/>
       <c r="AO39" s="40"/>
-    </row>
-    <row r="40" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ39" s="40"/>
+      <c r="AR39" s="40"/>
+      <c r="AS39" s="40"/>
+      <c r="AT39" s="48"/>
+      <c r="AU39" s="48"/>
+      <c r="AV39" s="48"/>
+      <c r="AW39" s="48"/>
+      <c r="AX39" s="48"/>
+      <c r="AY39" s="48"/>
+      <c r="AZ39" s="48"/>
+    </row>
+    <row r="40" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="39"/>
       <c r="B40" s="38"/>
       <c r="C40" s="40"/>
@@ -10703,8 +11318,18 @@
       <c r="AM40" s="40"/>
       <c r="AN40" s="40"/>
       <c r="AO40" s="40"/>
-    </row>
-    <row r="41" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ40" s="40"/>
+      <c r="AR40" s="40"/>
+      <c r="AS40" s="40"/>
+      <c r="AT40" s="48"/>
+      <c r="AU40" s="48"/>
+      <c r="AV40" s="48"/>
+      <c r="AW40" s="48"/>
+      <c r="AX40" s="48"/>
+      <c r="AY40" s="48"/>
+      <c r="AZ40" s="48"/>
+    </row>
+    <row r="41" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="35"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
@@ -10746,8 +11371,18 @@
       <c r="AM41" s="30"/>
       <c r="AN41" s="30"/>
       <c r="AO41" s="30"/>
-    </row>
-    <row r="42" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ41" s="30"/>
+      <c r="AR41" s="30"/>
+      <c r="AS41" s="30"/>
+      <c r="AT41" s="48"/>
+      <c r="AU41" s="48"/>
+      <c r="AV41" s="48"/>
+      <c r="AW41" s="48"/>
+      <c r="AX41" s="48"/>
+      <c r="AY41" s="48"/>
+      <c r="AZ41" s="48"/>
+    </row>
+    <row r="42" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="24"/>
       <c r="C42" s="36"/>
@@ -10789,8 +11424,18 @@
       <c r="AM42" s="36"/>
       <c r="AN42" s="36"/>
       <c r="AO42" s="36"/>
-    </row>
-    <row r="43" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ42" s="36"/>
+      <c r="AR42" s="36"/>
+      <c r="AS42" s="36"/>
+      <c r="AT42" s="48"/>
+      <c r="AU42" s="48"/>
+      <c r="AV42" s="48"/>
+      <c r="AW42" s="48"/>
+      <c r="AX42" s="48"/>
+      <c r="AY42" s="48"/>
+      <c r="AZ42" s="48"/>
+    </row>
+    <row r="43" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
       <c r="B43" s="21"/>
       <c r="C43" s="22"/>
@@ -10832,8 +11477,18 @@
       <c r="AM43" s="22"/>
       <c r="AN43" s="22"/>
       <c r="AO43" s="22"/>
-    </row>
-    <row r="44" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ43" s="22"/>
+      <c r="AR43" s="22"/>
+      <c r="AS43" s="22"/>
+      <c r="AT43" s="48"/>
+      <c r="AU43" s="48"/>
+      <c r="AV43" s="48"/>
+      <c r="AW43" s="48"/>
+      <c r="AX43" s="48"/>
+      <c r="AY43" s="48"/>
+      <c r="AZ43" s="48"/>
+    </row>
+    <row r="44" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="31"/>
       <c r="B44" s="24"/>
       <c r="C44" s="24"/>
@@ -10875,8 +11530,18 @@
       <c r="AM44" s="24"/>
       <c r="AN44" s="24"/>
       <c r="AO44" s="30"/>
-    </row>
-    <row r="45" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ44" s="30"/>
+      <c r="AR44" s="30"/>
+      <c r="AS44" s="30"/>
+      <c r="AT44" s="48"/>
+      <c r="AU44" s="48"/>
+      <c r="AV44" s="48"/>
+      <c r="AW44" s="48"/>
+      <c r="AX44" s="48"/>
+      <c r="AY44" s="48"/>
+      <c r="AZ44" s="48"/>
+    </row>
+    <row r="45" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="39"/>
       <c r="B45" s="38"/>
       <c r="C45" s="40"/>
@@ -10918,8 +11583,18 @@
       <c r="AM45" s="40"/>
       <c r="AN45" s="40"/>
       <c r="AO45" s="36"/>
-    </row>
-    <row r="46" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ45" s="36"/>
+      <c r="AR45" s="36"/>
+      <c r="AS45" s="36"/>
+      <c r="AT45" s="48"/>
+      <c r="AU45" s="48"/>
+      <c r="AV45" s="48"/>
+      <c r="AW45" s="48"/>
+      <c r="AX45" s="48"/>
+      <c r="AY45" s="48"/>
+      <c r="AZ45" s="48"/>
+    </row>
+    <row r="46" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="39"/>
       <c r="B46" s="38"/>
       <c r="C46" s="40"/>
@@ -10961,8 +11636,18 @@
       <c r="AM46" s="40"/>
       <c r="AN46" s="40"/>
       <c r="AO46"/>
-    </row>
-    <row r="47" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AQ46"/>
+      <c r="AR46"/>
+      <c r="AS46"/>
+      <c r="AT46" s="48"/>
+      <c r="AU46" s="48"/>
+      <c r="AV46" s="48"/>
+      <c r="AW46" s="48"/>
+      <c r="AX46" s="48"/>
+      <c r="AY46" s="48"/>
+      <c r="AZ46" s="48"/>
+    </row>
+    <row r="47" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="35"/>
       <c r="B47" s="30"/>
       <c r="C47" s="30"/>
@@ -11004,8 +11689,18 @@
       <c r="AM47" s="30"/>
       <c r="AN47" s="30"/>
       <c r="AO47"/>
-    </row>
-    <row r="48" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ47"/>
+      <c r="AR47"/>
+      <c r="AS47"/>
+      <c r="AT47" s="48"/>
+      <c r="AU47" s="48"/>
+      <c r="AV47" s="48"/>
+      <c r="AW47" s="48"/>
+      <c r="AX47" s="48"/>
+      <c r="AY47" s="48"/>
+      <c r="AZ47" s="48"/>
+    </row>
+    <row r="48" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="24"/>
       <c r="B48" s="24"/>
       <c r="C48" s="36"/>
@@ -11047,8 +11742,18 @@
       <c r="AM48" s="36"/>
       <c r="AN48" s="36"/>
       <c r="AO48"/>
-    </row>
-    <row r="49" spans="1:41" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ48"/>
+      <c r="AR48"/>
+      <c r="AS48"/>
+      <c r="AT48" s="48"/>
+      <c r="AU48" s="48"/>
+      <c r="AV48" s="48"/>
+      <c r="AW48" s="48"/>
+      <c r="AX48" s="48"/>
+      <c r="AY48" s="48"/>
+      <c r="AZ48" s="48"/>
+    </row>
+    <row r="49" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="21"/>
       <c r="B49" s="21"/>
       <c r="C49" s="22"/>
@@ -11090,8 +11795,18 @@
       <c r="AM49" s="22"/>
       <c r="AN49" s="22"/>
       <c r="AO49"/>
-    </row>
-    <row r="50" spans="1:41" ht="15" x14ac:dyDescent="0.25">
+      <c r="AQ49"/>
+      <c r="AR49"/>
+      <c r="AS49"/>
+      <c r="AT49" s="48"/>
+      <c r="AU49" s="48"/>
+      <c r="AV49" s="48"/>
+      <c r="AW49" s="48"/>
+      <c r="AX49" s="48"/>
+      <c r="AY49" s="48"/>
+      <c r="AZ49" s="48"/>
+    </row>
+    <row r="50" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="31"/>
       <c r="B50" s="24"/>
       <c r="C50" s="24"/>
@@ -11130,8 +11845,15 @@
       <c r="AL50" s="24"/>
       <c r="AM50" s="24"/>
       <c r="AN50" s="24"/>
-    </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AT50" s="48"/>
+      <c r="AU50" s="48"/>
+      <c r="AV50" s="48"/>
+      <c r="AW50" s="48"/>
+      <c r="AX50" s="48"/>
+      <c r="AY50" s="48"/>
+      <c r="AZ50" s="48"/>
+    </row>
+    <row r="51" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A51" s="39"/>
       <c r="B51" s="38"/>
       <c r="C51" s="40"/>
@@ -11170,8 +11892,15 @@
       <c r="AL51" s="40"/>
       <c r="AM51" s="40"/>
       <c r="AN51" s="40"/>
-    </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AT51" s="48"/>
+      <c r="AU51" s="48"/>
+      <c r="AV51" s="48"/>
+      <c r="AW51" s="48"/>
+      <c r="AX51" s="48"/>
+      <c r="AY51" s="48"/>
+      <c r="AZ51" s="48"/>
+    </row>
+    <row r="52" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A52" s="39"/>
       <c r="B52" s="38"/>
       <c r="C52" s="40"/>
@@ -11211,7 +11940,7 @@
       <c r="AM52" s="40"/>
       <c r="AN52" s="40"/>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A53" s="35"/>
       <c r="B53" s="30"/>
       <c r="C53" s="30"/>
@@ -11251,7 +11980,7 @@
       <c r="AM53" s="30"/>
       <c r="AN53" s="30"/>
     </row>
-    <row r="54" spans="1:41" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="24"/>
       <c r="B54" s="24"/>
       <c r="C54" s="36"/>
@@ -11291,7 +12020,7 @@
       <c r="AM54" s="36"/>
       <c r="AN54" s="36"/>
     </row>
-    <row r="55" spans="1:41" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="22"/>
@@ -11331,7 +12060,7 @@
       <c r="AM55" s="22"/>
       <c r="AN55" s="22"/>
     </row>
-    <row r="56" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A56" s="34"/>
       <c r="B56" s="30"/>
       <c r="C56" s="30"/>
@@ -11371,7 +12100,7 @@
       <c r="AM56" s="30"/>
       <c r="AN56" s="30"/>
     </row>
-    <row r="57" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A57" s="35"/>
       <c r="B57" s="38"/>
       <c r="C57" s="36"/>
@@ -11411,7 +12140,7 @@
       <c r="AM57" s="36"/>
       <c r="AN57" s="36"/>
     </row>
-    <row r="59" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:52" x14ac:dyDescent="0.2">
       <c r="X59" s="8"/>
       <c r="AE59" s="8"/>
       <c r="AF59" s="8"/>
@@ -11433,7 +12162,7 @@
   <dimension ref="B4:M56"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="110" zoomScaleNormal="70" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12075,7 +12804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -12116,17 +12845,17 @@
       <c r="B3" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="187">
+      <c r="C3" s="193">
         <v>43374</v>
       </c>
-      <c r="D3" s="188"/>
+      <c r="D3" s="194"/>
       <c r="E3" s="137"/>
       <c r="F3" s="136" t="s">
         <v>77</v>
       </c>
       <c r="G3" s="138"/>
-      <c r="H3" s="187"/>
-      <c r="I3" s="188"/>
+      <c r="H3" s="193"/>
+      <c r="I3" s="194"/>
       <c r="J3" s="135"/>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
COMISION 4% Y 3.5%
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
@@ -291,12 +291,6 @@
     </r>
   </si>
   <si>
-    <t>COMISIÓN  OPERADORA 2%)</t>
-  </si>
-  <si>
-    <t>COMISIÓN ASIMILADOS (2%)</t>
-  </si>
-  <si>
     <t>DESCUENTO ASIMILADOS</t>
   </si>
   <si>
@@ -679,6 +673,12 @@
   </si>
   <si>
     <t>INFONAVIT BIM ANT ASIM</t>
+  </si>
+  <si>
+    <t>COMISIÓN  OPERADORA 4%)</t>
+  </si>
+  <si>
+    <t>COMISIÓN ASIMILADOS (3.5%)</t>
   </si>
 </sst>
 </file>
@@ -3195,11 +3195,11 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1113" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5441,11 +5441,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:BJ13"/>
+  <dimension ref="B1:BJ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5470,7 +5470,7 @@
     <col min="22" max="22" width="17" customWidth="1"/>
     <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="1.85546875" customWidth="1"/>
+    <col min="25" max="25" width="4.28515625" customWidth="1"/>
     <col min="26" max="26" width="15.42578125" customWidth="1"/>
     <col min="27" max="27" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -5480,7 +5480,7 @@
     <col min="32" max="32" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:62" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -5541,7 +5541,7 @@
       <c r="BI1" s="50"/>
       <c r="BJ1" s="50"/>
     </row>
-    <row r="2" spans="1:62" s="1" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:62" s="1" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
@@ -5606,7 +5606,7 @@
       <c r="BI2" s="50"/>
       <c r="BJ2" s="50"/>
     </row>
-    <row r="3" spans="1:62" s="43" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:62" s="43" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
       <c r="D3" s="41"/>
@@ -5669,7 +5669,7 @@
       <c r="BI3" s="50"/>
       <c r="BJ3" s="50"/>
     </row>
-    <row r="4" spans="1:62" s="43" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:62" s="43" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
       <c r="D4" s="41"/>
@@ -5732,7 +5732,7 @@
       <c r="BI4" s="50"/>
       <c r="BJ4" s="50"/>
     </row>
-    <row r="5" spans="1:62" s="43" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:62" s="43" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
       <c r="D5" s="41"/>
@@ -5795,7 +5795,7 @@
       <c r="BI5" s="50"/>
       <c r="BJ5" s="50"/>
     </row>
-    <row r="6" spans="1:62" s="43" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:62" s="43" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
@@ -5858,7 +5858,7 @@
       <c r="BI6" s="50"/>
       <c r="BJ6" s="50"/>
     </row>
-    <row r="7" spans="1:62" s="43" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:62" s="43" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="41"/>
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
@@ -5921,7 +5921,7 @@
       <c r="BI7" s="50"/>
       <c r="BJ7" s="50"/>
     </row>
-    <row r="8" spans="1:62" s="43" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:62" s="43" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
       <c r="D8" s="41"/>
@@ -5984,7 +5984,7 @@
       <c r="BI8" s="50"/>
       <c r="BJ8" s="50"/>
     </row>
-    <row r="9" spans="1:62" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:62" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -6047,7 +6047,7 @@
       <c r="BI9" s="50"/>
       <c r="BJ9" s="50"/>
     </row>
-    <row r="10" spans="1:62" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:62" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="114"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -6110,7 +6110,7 @@
       <c r="BI10" s="50"/>
       <c r="BJ10" s="50"/>
     </row>
-    <row r="11" spans="1:62" s="85" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:62" s="85" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="197" t="s">
         <v>15</v>
       </c>
@@ -6147,11 +6147,11 @@
       <c r="M11" s="197" t="s">
         <v>62</v>
       </c>
-      <c r="N11" s="198" t="s">
-        <v>130</v>
-      </c>
-      <c r="O11" s="198" t="s">
-        <v>203</v>
+      <c r="N11" s="199" t="s">
+        <v>128</v>
+      </c>
+      <c r="O11" s="199" t="s">
+        <v>201</v>
       </c>
       <c r="P11" s="197" t="s">
         <v>72</v>
@@ -6176,10 +6176,10 @@
       </c>
       <c r="Y11" s="86"/>
       <c r="Z11" s="197" t="s">
-        <v>74</v>
+        <v>202</v>
       </c>
       <c r="AA11" s="197" t="s">
-        <v>75</v>
+        <v>203</v>
       </c>
       <c r="AB11" s="197" t="s">
         <v>5</v>
@@ -6187,11 +6187,11 @@
       <c r="AC11" s="197" t="s">
         <v>0</v>
       </c>
-      <c r="AD11" s="199" t="s">
+      <c r="AD11" s="198" t="s">
         <v>20</v>
       </c>
       <c r="AE11" s="197" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="AF11" s="197" t="s">
         <v>1</v>
@@ -6225,7 +6225,7 @@
       <c r="BH11" s="84"/>
       <c r="BI11" s="84"/>
     </row>
-    <row r="12" spans="1:62" s="87" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:62" s="87" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="197"/>
       <c r="C12" s="197"/>
       <c r="D12" s="197"/>
@@ -6238,11 +6238,11 @@
       <c r="K12" s="197"/>
       <c r="L12" s="197"/>
       <c r="M12" s="197"/>
-      <c r="N12" s="198"/>
-      <c r="O12" s="198"/>
+      <c r="N12" s="199"/>
+      <c r="O12" s="199"/>
       <c r="P12" s="197"/>
       <c r="Q12" s="129" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R12" s="197" t="s">
         <v>63</v>
@@ -6251,7 +6251,7 @@
         <v>66</v>
       </c>
       <c r="T12" s="132" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U12" s="197"/>
       <c r="V12" s="197"/>
@@ -6262,7 +6262,7 @@
       <c r="AA12" s="197"/>
       <c r="AB12" s="197"/>
       <c r="AC12" s="197"/>
-      <c r="AD12" s="199"/>
+      <c r="AD12" s="198"/>
       <c r="AE12" s="197"/>
       <c r="AF12" s="197"/>
       <c r="AG12" s="197"/>
@@ -6295,10 +6295,7 @@
       <c r="BH12" s="89"/>
       <c r="BI12" s="89"/>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
+    <row r="13" spans="2:62" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>2</v>
       </c>
@@ -6368,9 +6365,6 @@
       <c r="X13">
         <v>24</v>
       </c>
-      <c r="Y13">
-        <v>25</v>
-      </c>
       <c r="Z13">
         <v>26</v>
       </c>
@@ -6395,14 +6389,11 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="Z11:Z12"/>
-    <mergeCell ref="AB11:AB12"/>
-    <mergeCell ref="AA11:AA12"/>
-    <mergeCell ref="AE11:AE12"/>
-    <mergeCell ref="AG11:AG12"/>
-    <mergeCell ref="AF11:AF12"/>
-    <mergeCell ref="AC11:AC12"/>
-    <mergeCell ref="AD11:AD12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="M11:M12"/>
     <mergeCell ref="X11:X12"/>
@@ -6418,11 +6409,14 @@
     <mergeCell ref="V11:V12"/>
     <mergeCell ref="N11:N12"/>
     <mergeCell ref="O11:O12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="Z11:Z12"/>
+    <mergeCell ref="AB11:AB12"/>
+    <mergeCell ref="AA11:AA12"/>
+    <mergeCell ref="AE11:AE12"/>
+    <mergeCell ref="AG11:AG12"/>
+    <mergeCell ref="AF11:AF12"/>
+    <mergeCell ref="AC11:AC12"/>
+    <mergeCell ref="AD11:AD12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7055,10 +7049,10 @@
         <v>10</v>
       </c>
       <c r="AJ8" s="45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AK8" s="45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AL8" s="45" t="s">
         <v>52</v>
@@ -7070,7 +7064,7 @@
         <v>66</v>
       </c>
       <c r="AO8" s="128" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AP8" s="180" t="s">
         <v>53</v>
@@ -7094,13 +7088,13 @@
         <v>70</v>
       </c>
       <c r="AW8" s="181" t="s">
+        <v>97</v>
+      </c>
+      <c r="AX8" s="128" t="s">
+        <v>98</v>
+      </c>
+      <c r="AY8" s="128" t="s">
         <v>99</v>
-      </c>
-      <c r="AX8" s="128" t="s">
-        <v>100</v>
-      </c>
-      <c r="AY8" s="128" t="s">
-        <v>101</v>
       </c>
       <c r="AZ8" s="10"/>
       <c r="BA8" s="10"/>
@@ -9973,10 +9967,10 @@
         <v>10</v>
       </c>
       <c r="AJ8" s="45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AK8" s="45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AL8" s="45" t="s">
         <v>52</v>
@@ -9988,7 +9982,7 @@
         <v>66</v>
       </c>
       <c r="AO8" s="128" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AP8" s="127" t="s">
         <v>53</v>
@@ -10012,13 +10006,13 @@
         <v>70</v>
       </c>
       <c r="AW8" s="128" t="s">
+        <v>97</v>
+      </c>
+      <c r="AX8" s="128" t="s">
+        <v>98</v>
+      </c>
+      <c r="AY8" s="128" t="s">
         <v>99</v>
-      </c>
-      <c r="AX8" s="128" t="s">
-        <v>100</v>
-      </c>
-      <c r="AY8" s="128" t="s">
-        <v>101</v>
       </c>
       <c r="AZ8" s="10"/>
       <c r="BA8" s="10"/>
@@ -13212,7 +13206,7 @@
         <v>hoja.Cell("T" &amp; sep</v>
       </c>
       <c r="F1" s="190" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G1" s="187" t="str">
         <f>+A1&amp;C4</f>
@@ -13223,473 +13217,473 @@
       <c r="A2" s="196"/>
       <c r="B2" s="196"/>
       <c r="C2" s="192" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E2" s="189" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;" sep + 1"</f>
         <v>hoja.Cell("T" &amp;  sep + 1</v>
       </c>
       <c r="F2" s="190" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="187" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="187" t="str">
         <f>+B1</f>
         <v xml:space="preserve"> leon</v>
       </c>
       <c r="C3" s="192" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E3" s="189" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;"sep + 3"</f>
         <v>hoja.Cell("T" &amp; sep + 3</v>
       </c>
       <c r="F3" s="190" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C4" s="73" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E4" s="189" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;"sep + 4"</f>
         <v>hoja.Cell("T" &amp; sep + 4</v>
       </c>
       <c r="F4" s="190" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C5" s="191" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E5" s="189" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;"sep + 5"</f>
         <v>hoja.Cell("T" &amp; sep + 5</v>
       </c>
       <c r="F5" s="190" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C6" s="194" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E6" s="189" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;"sep + 6"</f>
         <v>hoja.Cell("T" &amp; sep + 6</v>
       </c>
       <c r="F6" s="190" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G6" s="187" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C7" s="194" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E7" s="188"/>
       <c r="F7" s="190"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C8" s="194" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E8" s="187" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;"sep + 7"</f>
         <v>hoja.Cell("T" &amp; sep + 7</v>
       </c>
       <c r="F8" s="190" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C9" s="194" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E9" s="187" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;"sep + 8"</f>
         <v>hoja.Cell("T" &amp; sep + 8</v>
       </c>
       <c r="F9" s="190" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C10" s="194" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E10" s="187" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;"sep + 9"</f>
         <v>hoja.Cell("T" &amp; sep + 9</v>
       </c>
       <c r="F10" s="190" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C11" s="191" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C12" s="191" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B13" s="187" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C13" s="191" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C14" s="191" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E14" s="187" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C11</f>
         <v xml:space="preserve">hoja.Cell("V" &amp; sep +3 </v>
       </c>
       <c r="F14" s="187" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G14" s="187" t="str">
         <f>C5&amp;B1&amp;C6&amp;B1&amp;C7&amp;B1&amp;C8&amp;B1&amp;C9</f>
         <v>"=V" &amp; leon+1 &amp; " + X" &amp; leon+1 &amp; " + Z"&amp; leon+1 &amp; "+AB" &amp; leon+1</v>
       </c>
       <c r="H14" s="187" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C15" s="191" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E15" s="187" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C12</f>
         <v>hoja.Cell("V" &amp; sep +4</v>
       </c>
       <c r="F15" s="187" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G15" s="187" t="str">
         <f>+C10&amp;C2&amp;C4&amp;C11&amp;C15</f>
         <v>"=V" &amp; sep +3  &amp; "*16%"</v>
       </c>
       <c r="H15" s="187" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C16" s="191" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E16" s="187" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C13</f>
         <v>hoja.Cell("V" &amp; sep +5</v>
       </c>
       <c r="F16" s="187" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G16" s="187" t="str">
         <f>+C10&amp;C2&amp;C4&amp;C11&amp;C16</f>
         <v>"=V" &amp; sep +3  &amp;" *6%"</v>
       </c>
       <c r="H16" s="187" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C17" s="191" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E17" s="187" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C14</f>
         <v xml:space="preserve">hoja.Cell("V" &amp; sep +6 </v>
       </c>
       <c r="F17" s="187" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G17" s="187" t="str">
         <f>+C10&amp;C2&amp;C4&amp;C11&amp;C17&amp;C4&amp;C18&amp;C2&amp;C4&amp;C12&amp;C17&amp;C4&amp;C19&amp;C2&amp;C4&amp;C13</f>
         <v>"=V" &amp; sep +3  &amp; "+V" &amp; sep +4 &amp; "-V" &amp; sep +5</v>
       </c>
       <c r="H17" s="187" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C18" s="191" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F18" s="187"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C19" s="191" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E19" s="187" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C23</f>
         <v>hoja.Cell("V" &amp; sep +7</v>
       </c>
       <c r="F19" s="187" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G19" s="187" t="str">
         <f>+C20&amp;B1&amp;C21&amp;B1&amp;C22&amp;B1&amp;C9</f>
         <v>"=W" &amp; leon+1 &amp; "+AA" &amp; leon+1 &amp; "+Q" &amp; leon+1</v>
       </c>
       <c r="H19" s="187" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C20" s="191" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E20" s="187" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C24</f>
         <v>hoja.Cell("V" &amp; sep +8</v>
       </c>
       <c r="F20" s="187" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G20" s="187" t="str">
         <f>+C10&amp;C2&amp;C4&amp;C23&amp;C15</f>
         <v>"=V" &amp; sep +7 &amp; "*16%"</v>
       </c>
       <c r="H20" s="187" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C21" s="194" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E21" s="187" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C25</f>
         <v>hoja.Cell("V" &amp; sep +9</v>
       </c>
       <c r="F21" s="187" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G21" s="187" t="str">
         <f>+C10&amp;C2&amp;C4&amp;C23&amp;C17&amp;C4&amp;C18&amp;C2&amp;C4&amp;C24</f>
         <v>"=V" &amp; sep +7 &amp; "+V" &amp; sep +8</v>
       </c>
       <c r="H21" s="187" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C22" s="194" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F22" s="187"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C23" s="191" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E23" s="187" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C26</f>
         <v>hoja.Cell("V" &amp; sep +10</v>
       </c>
       <c r="F23" s="187" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G23" s="187" t="str">
         <f>+C10&amp;C2&amp;C4&amp;C14&amp;C17&amp;C4&amp;C18&amp;C2&amp;C4&amp;C25</f>
         <v>"=V" &amp; sep +6  &amp; "+V" &amp; sep +9</v>
       </c>
       <c r="H23" s="187" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C24" s="191" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="187" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B25" s="187" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C25" s="191" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="187" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B26" s="187" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C26" s="191" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C28" s="191" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E28" s="205" t="str">
         <f>+C28&amp;C4&amp;C3&amp;C4&amp;C25&amp;","&amp;C4&amp;C2&amp;C4&amp;C25&amp;")"</f>
@@ -13697,19 +13691,19 @@
       </c>
       <c r="F28" s="205"/>
       <c r="G28" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C29" s="191" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E29" t="str">
         <f>+C28&amp;C4&amp;C3&amp;C4&amp;C14&amp;","&amp;C4&amp;C2&amp;C4&amp;C14&amp;")"</f>
         <v>hoja.Range("T" &amp; sep +6 ,"V" &amp; sep +6 )</v>
       </c>
       <c r="G29" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -13718,7 +13712,7 @@
         <v>hoja.Cell("T" &amp; sep)</v>
       </c>
       <c r="F30" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -13773,13 +13767,13 @@
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="133"/>
       <c r="B3" s="136" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" s="206"/>
       <c r="D3" s="207"/>
       <c r="E3" s="137"/>
       <c r="F3" s="136" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G3" s="138"/>
       <c r="H3" s="206"/>
@@ -13789,33 +13783,33 @@
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="133"/>
       <c r="B4" s="139" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="140" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="140" t="s">
         <v>78</v>
-      </c>
-      <c r="C4" s="140" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="140" t="s">
-        <v>80</v>
       </c>
       <c r="E4" s="141"/>
       <c r="F4" s="139" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="142" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="140" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="140" t="s">
         <v>78</v>
-      </c>
-      <c r="G4" s="142" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="140" t="s">
-        <v>79</v>
-      </c>
-      <c r="I4" s="140" t="s">
-        <v>80</v>
       </c>
       <c r="J4" s="135"/>
     </row>
     <row r="5" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A5" s="133"/>
       <c r="B5" s="143" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" s="144"/>
       <c r="D5" s="144"/>
@@ -13832,13 +13826,13 @@
     <row r="6" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A6" s="133"/>
       <c r="B6" s="146" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C6" s="147"/>
       <c r="D6" s="147"/>
       <c r="E6" s="134"/>
       <c r="F6" s="148" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G6" s="149"/>
       <c r="H6" s="147"/>
@@ -13848,13 +13842,13 @@
     <row r="7" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A7" s="133"/>
       <c r="B7" s="146" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" s="147"/>
       <c r="D7" s="147"/>
       <c r="E7" s="150"/>
       <c r="F7" s="148" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G7" s="149"/>
       <c r="H7" s="147"/>
@@ -13864,13 +13858,13 @@
     <row r="8" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A8" s="133"/>
       <c r="B8" s="146" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C8" s="147"/>
       <c r="D8" s="147"/>
       <c r="E8" s="151"/>
       <c r="F8" s="148" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G8" s="149"/>
       <c r="H8" s="147"/>
@@ -13880,13 +13874,13 @@
     <row r="9" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A9" s="133"/>
       <c r="B9" s="146" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C9" s="147"/>
       <c r="D9" s="147"/>
       <c r="E9" s="152"/>
       <c r="F9" s="148" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G9" s="149"/>
       <c r="H9" s="147"/>
@@ -13896,13 +13890,13 @@
     <row r="10" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A10" s="133"/>
       <c r="B10" s="146" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C10" s="147"/>
       <c r="D10" s="147"/>
       <c r="E10" s="150"/>
       <c r="F10" s="148" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G10" s="149"/>
       <c r="H10" s="147"/>
@@ -13912,13 +13906,13 @@
     <row r="11" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A11" s="133"/>
       <c r="B11" s="146" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" s="147"/>
       <c r="D11" s="147"/>
       <c r="E11" s="150"/>
       <c r="F11" s="148" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G11" s="149"/>
       <c r="H11" s="147"/>
@@ -13928,13 +13922,13 @@
     <row r="12" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A12" s="133"/>
       <c r="B12" s="146" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C12" s="147"/>
       <c r="D12" s="147"/>
       <c r="E12" s="151"/>
       <c r="F12" s="148" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G12" s="149"/>
       <c r="H12" s="147"/>
@@ -13944,13 +13938,13 @@
     <row r="13" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A13" s="133"/>
       <c r="B13" s="146" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C13" s="147"/>
       <c r="D13" s="147"/>
       <c r="E13" s="151"/>
       <c r="F13" s="148" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G13" s="149"/>
       <c r="H13" s="147"/>
@@ -13960,13 +13954,13 @@
     <row r="14" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A14" s="133"/>
       <c r="B14" s="146" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C14" s="151"/>
       <c r="D14" s="147"/>
       <c r="E14" s="152"/>
       <c r="F14" s="148" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G14" s="149"/>
       <c r="H14" s="147"/>
@@ -13976,13 +13970,13 @@
     <row r="15" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A15" s="133"/>
       <c r="B15" s="153" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C15" s="147"/>
       <c r="D15" s="147"/>
       <c r="E15" s="154"/>
       <c r="F15" s="148" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G15" s="149"/>
       <c r="H15" s="147"/>
@@ -13992,13 +13986,13 @@
     <row r="16" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A16" s="133"/>
       <c r="B16" s="155" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C16" s="151"/>
       <c r="D16" s="156"/>
       <c r="E16" s="154"/>
       <c r="F16" s="148" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G16" s="149"/>
       <c r="H16" s="147"/>
@@ -14008,13 +14002,13 @@
     <row r="17" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A17" s="133"/>
       <c r="B17" s="146" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C17" s="147"/>
       <c r="D17" s="147"/>
       <c r="E17" s="154"/>
       <c r="F17" s="148" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G17" s="149"/>
       <c r="H17" s="147"/>
@@ -14024,13 +14018,13 @@
     <row r="18" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A18" s="133"/>
       <c r="B18" s="146" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C18" s="147"/>
       <c r="D18" s="147"/>
       <c r="E18" s="154"/>
       <c r="F18" s="153" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G18" s="149"/>
       <c r="H18" s="147"/>
@@ -14040,13 +14034,13 @@
     <row r="19" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A19" s="133"/>
       <c r="B19" s="146" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C19" s="147"/>
       <c r="D19" s="147"/>
       <c r="E19" s="154"/>
       <c r="F19" s="153" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G19" s="149"/>
       <c r="H19" s="147"/>
@@ -14056,13 +14050,13 @@
     <row r="20" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A20" s="133"/>
       <c r="B20" s="146" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C20" s="147"/>
       <c r="D20" s="147"/>
       <c r="E20" s="154"/>
       <c r="F20" s="157" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G20" s="149"/>
       <c r="H20" s="147"/>
@@ -14072,13 +14066,13 @@
     <row r="21" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A21" s="133"/>
       <c r="B21" s="146" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C21" s="147"/>
       <c r="D21" s="147"/>
       <c r="E21" s="154"/>
       <c r="F21" s="157" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G21" s="149"/>
       <c r="H21" s="145"/>
@@ -14088,13 +14082,13 @@
     <row r="22" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A22" s="133"/>
       <c r="B22" s="146" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C22" s="147"/>
       <c r="D22" s="147"/>
       <c r="E22" s="154"/>
       <c r="F22" s="157" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G22" s="149"/>
       <c r="H22" s="145"/>
@@ -14104,13 +14098,13 @@
     <row r="23" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A23" s="133"/>
       <c r="B23" s="155" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C23" s="156"/>
       <c r="D23" s="147"/>
       <c r="E23" s="154"/>
       <c r="F23" s="157" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G23" s="149"/>
       <c r="H23" s="145"/>
@@ -14120,13 +14114,13 @@
     <row r="24" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="133"/>
       <c r="B24" s="155" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C24" s="156"/>
       <c r="D24" s="147"/>
       <c r="E24" s="154"/>
       <c r="F24" s="163" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G24" s="164"/>
       <c r="H24" s="145"/>
@@ -14136,7 +14130,7 @@
     <row r="25" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A25" s="133"/>
       <c r="B25" s="157" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C25" s="157"/>
       <c r="D25" s="147"/>
@@ -14158,13 +14152,13 @@
     <row r="26" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A26" s="133"/>
       <c r="B26" s="157" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C26" s="157"/>
       <c r="D26" s="147"/>
       <c r="E26" s="154"/>
       <c r="F26" s="162" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G26" s="169"/>
       <c r="H26" s="147">
@@ -14180,7 +14174,7 @@
     <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="133"/>
       <c r="B27" s="158" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C27" s="159"/>
       <c r="D27" s="147"/>
@@ -14228,7 +14222,7 @@
     <row r="29" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A29" s="133"/>
       <c r="B29" s="162" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C29" s="147">
         <f>C28*16%</f>
@@ -14240,7 +14234,7 @@
       </c>
       <c r="E29" s="154"/>
       <c r="F29" s="148" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G29" s="149"/>
       <c r="H29" s="147"/>
@@ -14250,7 +14244,7 @@
     <row r="30" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A30" s="133"/>
       <c r="B30" s="162" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C30" s="147">
         <f>+C28*6%</f>
@@ -14262,7 +14256,7 @@
       </c>
       <c r="E30" s="154"/>
       <c r="F30" s="148" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G30" s="149"/>
       <c r="H30" s="147"/>
@@ -14284,7 +14278,7 @@
       </c>
       <c r="E31" s="154"/>
       <c r="F31" s="148" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G31" s="149"/>
       <c r="H31" s="147"/>
@@ -14294,13 +14288,13 @@
     <row r="32" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A32" s="133"/>
       <c r="B32" s="143" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C32" s="145"/>
       <c r="D32" s="145"/>
       <c r="E32" s="154"/>
       <c r="F32" s="148" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G32" s="149"/>
       <c r="H32" s="147"/>
@@ -14310,13 +14304,13 @@
     <row r="33" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A33" s="133"/>
       <c r="B33" s="146" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C33" s="145"/>
       <c r="D33" s="145"/>
       <c r="E33" s="154"/>
       <c r="F33" s="148" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G33" s="149"/>
       <c r="H33" s="147"/>
@@ -14326,13 +14320,13 @@
     <row r="34" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A34" s="133"/>
       <c r="B34" s="146" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C34" s="147"/>
       <c r="D34" s="144"/>
       <c r="E34" s="154"/>
       <c r="F34" s="148" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G34" s="149"/>
       <c r="H34" s="147"/>
@@ -14342,13 +14336,13 @@
     <row r="35" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A35" s="133"/>
       <c r="B35" s="146" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C35" s="147"/>
       <c r="D35" s="144"/>
       <c r="E35" s="154"/>
       <c r="F35" s="148" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G35" s="149"/>
       <c r="H35" s="147"/>
@@ -14358,13 +14352,13 @@
     <row r="36" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A36" s="133"/>
       <c r="B36" s="146" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C36" s="147"/>
       <c r="D36" s="144"/>
       <c r="E36" s="154"/>
       <c r="F36" s="148" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G36" s="149"/>
       <c r="H36" s="147"/>
@@ -14374,13 +14368,13 @@
     <row r="37" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A37" s="133"/>
       <c r="B37" s="146" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C37" s="147"/>
       <c r="D37" s="144"/>
       <c r="E37" s="154"/>
       <c r="F37" s="148" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G37" s="149"/>
       <c r="H37" s="147"/>
@@ -14390,13 +14384,13 @@
     <row r="38" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A38" s="133"/>
       <c r="B38" s="146" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C38" s="147"/>
       <c r="D38" s="144"/>
       <c r="E38" s="154"/>
       <c r="F38" s="148" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G38" s="149"/>
       <c r="H38" s="147"/>
@@ -14406,13 +14400,13 @@
     <row r="39" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A39" s="133"/>
       <c r="B39" s="146" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C39" s="147"/>
       <c r="D39" s="144"/>
       <c r="E39" s="154"/>
       <c r="F39" s="148" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G39" s="149"/>
       <c r="H39" s="147"/>
@@ -14422,13 +14416,13 @@
     <row r="40" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A40" s="135"/>
       <c r="B40" s="146" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C40" s="147"/>
       <c r="D40" s="144"/>
       <c r="E40" s="154"/>
       <c r="F40" s="148" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G40" s="149"/>
       <c r="H40" s="147"/>
@@ -14438,13 +14432,13 @@
     <row r="41" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A41" s="135"/>
       <c r="B41" s="146" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C41" s="147"/>
       <c r="D41" s="147"/>
       <c r="E41" s="154"/>
       <c r="F41" s="148" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G41" s="149"/>
       <c r="H41" s="147"/>
@@ -14454,13 +14448,13 @@
     <row r="42" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A42" s="135"/>
       <c r="B42" s="153" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C42" s="147"/>
       <c r="D42" s="144"/>
       <c r="E42" s="154"/>
       <c r="F42" s="148" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G42" s="149"/>
       <c r="H42" s="147"/>
@@ -14470,13 +14464,13 @@
     <row r="43" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A43" s="135"/>
       <c r="B43" s="155" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C43" s="147"/>
       <c r="D43" s="144"/>
       <c r="E43" s="154"/>
       <c r="F43" s="148" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G43" s="149"/>
       <c r="H43" s="147"/>
@@ -14486,13 +14480,13 @@
     <row r="44" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A44" s="135"/>
       <c r="B44" s="146" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C44" s="156"/>
       <c r="D44" s="172"/>
       <c r="E44" s="154"/>
       <c r="F44" s="148" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G44" s="149"/>
       <c r="H44" s="145"/>
@@ -14502,13 +14496,13 @@
     <row r="45" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A45" s="135"/>
       <c r="B45" s="146" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C45" s="147"/>
       <c r="D45" s="147"/>
       <c r="E45" s="154"/>
       <c r="F45" s="148" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G45" s="149"/>
       <c r="H45" s="145"/>
@@ -14518,13 +14512,13 @@
     <row r="46" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A46" s="135"/>
       <c r="B46" s="146" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C46" s="156"/>
       <c r="D46" s="172"/>
       <c r="E46" s="154"/>
       <c r="F46" s="148" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G46" s="149"/>
       <c r="H46" s="145"/>
@@ -14534,13 +14528,13 @@
     <row r="47" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="135"/>
       <c r="B47" s="146" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C47" s="156"/>
       <c r="D47" s="172"/>
       <c r="E47" s="154"/>
       <c r="F47" s="148" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G47" s="164"/>
       <c r="H47" s="145"/>
@@ -14550,7 +14544,7 @@
     <row r="48" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A48" s="135"/>
       <c r="B48" s="146" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C48" s="156"/>
       <c r="D48" s="172"/>
@@ -14572,13 +14566,13 @@
     <row r="49" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A49" s="135"/>
       <c r="B49" s="146" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C49" s="156"/>
       <c r="D49" s="172"/>
       <c r="E49" s="154"/>
       <c r="F49" s="162" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G49" s="169"/>
       <c r="H49" s="147">
@@ -14594,7 +14588,7 @@
     <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="135"/>
       <c r="B50" s="155" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C50" s="156"/>
       <c r="D50" s="156"/>
@@ -14618,28 +14612,28 @@
     </row>
     <row r="51" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B51" s="155" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C51" s="155"/>
       <c r="D51" s="156"/>
     </row>
     <row r="52" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B52" s="157" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C52" s="157"/>
       <c r="D52" s="156"/>
     </row>
     <row r="53" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B53" s="157" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C53" s="157"/>
       <c r="D53" s="156"/>
     </row>
     <row r="54" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="158" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C54" s="158"/>
       <c r="D54" s="156"/>
@@ -14659,7 +14653,7 @@
     </row>
     <row r="56" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B56" s="162" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C56" s="147">
         <f>C55*16%</f>
@@ -14735,10 +14729,10 @@
   <sheetData>
     <row r="1" spans="2:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="177" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C1" s="177" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D1" s="179" t="s">
         <v>7</v>
@@ -14750,13 +14744,13 @@
         <v>13</v>
       </c>
       <c r="G1" s="177" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="177" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="177" t="s">
         <v>118</v>
-      </c>
-      <c r="H1" s="177" t="s">
-        <v>119</v>
-      </c>
-      <c r="I1" s="177" t="s">
-        <v>120</v>
       </c>
       <c r="J1" s="177" t="s">
         <v>1</v>
@@ -14899,19 +14893,19 @@
         <v>6</v>
       </c>
       <c r="C1" s="186" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="186" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="186" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="186" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="186" t="s">
+      <c r="G1" s="186" t="s">
         <v>122</v>
-      </c>
-      <c r="E1" s="186" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" s="186" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" s="186" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
@@ -14949,19 +14943,19 @@
         <v>6</v>
       </c>
       <c r="C1" s="186" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="186" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="186" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="186" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="186" t="s">
+      <c r="G1" s="186" t="s">
         <v>122</v>
-      </c>
-      <c r="E1" s="186" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" s="186" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" s="186" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios nuevos nuevos de lalo
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
@@ -50,7 +50,7 @@
     <definedName name="TCF">[2]FOR!$B$8</definedName>
     <definedName name="VSDF">[2]FOR!$B$7</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual" calcCompleted="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -256,6 +256,597 @@
   </si>
   <si>
     <t xml:space="preserve">DESCUENTO SA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FACTURACIÓN </t>
+  </si>
+  <si>
+    <t>CONCEPTOS</t>
+  </si>
+  <si>
+    <t>TMM DIVISION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TMM SA</t>
+  </si>
+  <si>
+    <t>ISLA MONSERRAT</t>
+  </si>
+  <si>
+    <t>IVA</t>
+  </si>
+  <si>
+    <t>ISLA ARBOLEDA</t>
+  </si>
+  <si>
+    <t>ISLA AZTECA</t>
+  </si>
+  <si>
+    <t>ISLA CEDROS</t>
+  </si>
+  <si>
+    <t>ISLA MIRAMAR</t>
+  </si>
+  <si>
+    <t>ISLA VERDE</t>
+  </si>
+  <si>
+    <t>ISLA SANTA CRUZ</t>
+  </si>
+  <si>
+    <t>ISLA BLANCA</t>
+  </si>
+  <si>
+    <t>ISLA CIARI</t>
+  </si>
+  <si>
+    <t>ISLA JANITZIO</t>
+  </si>
+  <si>
+    <t>ISLA SAN IGNACIO</t>
+  </si>
+  <si>
+    <t>ISLA SAN GABRIEL</t>
+  </si>
+  <si>
+    <t>ISLA SAN DIEGO</t>
+  </si>
+  <si>
+    <t>AJUSTE INFONAVIT</t>
+  </si>
+  <si>
+    <t>INFONAVIT BIMESTRE ATERIOR</t>
+  </si>
+  <si>
+    <t>Prestamo Personal Asimilado</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>ISLA CRECIENTE</t>
+  </si>
+  <si>
+    <t>ISLA GRANDE</t>
+  </si>
+  <si>
+    <t>ISLA SAN JOSE</t>
+  </si>
+  <si>
+    <t>ISLA LEON</t>
+  </si>
+  <si>
+    <t>ISLA SAN LUIS</t>
+  </si>
+  <si>
+    <t>ISLA COLORADA</t>
+  </si>
+  <si>
+    <t>ISLA PASSAVERA</t>
+  </si>
+  <si>
+    <t>ISLA MARGOT MARIANNE</t>
+  </si>
+  <si>
+    <t>FONACOT</t>
+  </si>
+  <si>
+    <t>NOMBRE TRABAJADOR</t>
+  </si>
+  <si>
+    <t>NOMBRE BENFICIARIO</t>
+  </si>
+  <si>
+    <t>PORCENTAJE</t>
+  </si>
+  <si>
+    <t>MONTO ABORDO</t>
+  </si>
+  <si>
+    <t>MONTO DESCANSO</t>
+  </si>
+  <si>
+    <t>SUBSEA88</t>
+  </si>
+  <si>
+    <t>MONTO</t>
+  </si>
+  <si>
+    <t>DESCUENTO</t>
+  </si>
+  <si>
+    <t>TOTAL FALTANTE</t>
+  </si>
+  <si>
+    <t>TIPO DESCUENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESCUENTO </t>
+  </si>
+  <si>
+    <t>TOTAL COBRADO</t>
+  </si>
+  <si>
+    <t>RETENCION DEL 6%</t>
+  </si>
+  <si>
+    <t>RETENCION 6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "TMM DIVISION"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "DEPOSITO ROUTES SCOTIABANK"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "IVA"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "RETENCION 6%"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "DEPOSITO BIRYUSA SCOTIABANK"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "TOTAL DEPOSITO BIRYUSA"</t>
+  </si>
+  <si>
+    <t>).Value =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoja.Cell(sep + 4, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoja.Cell(sep + 5, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoja.Cell(sep + 7, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoja.Cell(sep + 9, </t>
+  </si>
+  <si>
+    <t>).Value ="</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoja.Cell(sep + 6, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoja.Cell(sep + 8, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoja.Cell(sep + 10, </t>
+  </si>
+  <si>
+    <t>hoja.Cell(sep + 3,</t>
+  </si>
+  <si>
+    <t>amarrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> azteca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cedros</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> miramar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> verde</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cruz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> montserrat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> blanca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ciari</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> janitzio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> luis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ignacio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gabriel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> diego</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jose</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> grande</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> creciente</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> colorada</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> subsea88</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> leon</t>
+  </si>
+  <si>
+    <t>passavera</t>
+  </si>
+  <si>
+    <t>margot</t>
+  </si>
+  <si>
+    <t>"=V" &amp;</t>
+  </si>
+  <si>
+    <t>+1</t>
+  </si>
+  <si>
+    <t>+1 &amp; " + X" &amp;</t>
+  </si>
+  <si>
+    <t>+1 &amp; " + Z"&amp;</t>
+  </si>
+  <si>
+    <t>+1 &amp; "+AB" &amp;</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "TOTAL DEPOSITO OPERADORA"</t>
+  </si>
+  <si>
+    <t>"=</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; sep +4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; sep +3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; sep +5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; "*16%"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;" *6%"</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; </t>
+  </si>
+  <si>
+    <t>+1 &amp; "+AA" &amp;</t>
+  </si>
+  <si>
+    <t>+1 &amp; "+Q" &amp;</t>
+  </si>
+  <si>
+    <t>"=W" &amp;</t>
+  </si>
+  <si>
+    <t>).FormulaA1 =</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; sep +7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; sep +8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; sep +9</t>
+  </si>
+  <si>
+    <t>.Style.Fill.BackgroundColor = XLColor.YellowProcess</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; sep +6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; sep +10</t>
+  </si>
+  <si>
+    <t>hoja.Range(</t>
+  </si>
+  <si>
+    <t>AMARRADOS</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>.Style.Fill.BackgroundColor = XLColor.PowderBlue</t>
+  </si>
+  <si>
+    <t>hoja.Cell(</t>
+  </si>
+  <si>
+    <t>NEVADO DE COLIMA</t>
+  </si>
+  <si>
+    <t>nevado</t>
+  </si>
+  <si>
+    <t>PROYECTO LODEROS1</t>
+  </si>
+  <si>
+    <t>PROYECTO MAERSK</t>
+  </si>
+  <si>
+    <t>loderos1</t>
+  </si>
+  <si>
+    <t>maersk</t>
+  </si>
+  <si>
+    <t>RED FISH</t>
+  </si>
+  <si>
+    <t>PROYECTO BELUGA 2</t>
+  </si>
+  <si>
+    <t>PROYECTO GO CANOPUS</t>
+  </si>
+  <si>
+    <t>SOVER</t>
+  </si>
+  <si>
+    <t>TRANSPORTES SOVER SA DE CV</t>
+  </si>
+  <si>
+    <t>VALORES AGREGADOS</t>
+  </si>
+  <si>
+    <t>PFB CORTO PLAZO</t>
+  </si>
+  <si>
+    <t>FONDO PFB 3%</t>
+  </si>
+  <si>
+    <t>COMISIÓN PLAN PENSIONES(8%)</t>
+  </si>
+  <si>
+    <t>IKE</t>
+  </si>
+  <si>
+    <t>PLAN FLEX LP</t>
+  </si>
+  <si>
+    <t>APOR PATRON PLAN FLEX LP</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>NETO</t>
+  </si>
+  <si>
+    <t>DESCUENTO PPP</t>
+  </si>
+  <si>
+    <t>TOTAL DEDUCCIONES</t>
+  </si>
+  <si>
+    <t>GANNET</t>
+  </si>
+  <si>
+    <t>Pension Alimentica  IKE</t>
+  </si>
+  <si>
+    <t>PENSION ALIMENTICIA PPP</t>
+  </si>
+  <si>
+    <t>DEP</t>
+  </si>
+  <si>
+    <t>AURORA PEARL</t>
+  </si>
+  <si>
+    <t>WORLD PERIDOT</t>
+  </si>
+  <si>
+    <t>AGENCIA GROESSINGER SAPI DE CV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  VSM IKE  </t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>INFONAVIT PPP</t>
+  </si>
+  <si>
+    <t>COMISIÓN  SOVER (4%)</t>
   </si>
   <si>
     <r>
@@ -269,602 +860,11 @@
         <rFont val="Century Gothic"/>
         <family val="2"/>
       </rPr>
-      <t>(ISR, INFONAVIT)</t>
+      <t>(ISR, INFONAVIT, PENSIONES SA/PPP..)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">FACTURACIÓN </t>
-  </si>
-  <si>
-    <t>CONCEPTOS</t>
-  </si>
-  <si>
-    <t>TMM DIVISION</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TMM SA</t>
-  </si>
-  <si>
-    <t>ISLA MONSERRAT</t>
-  </si>
-  <si>
-    <t>IVA</t>
-  </si>
-  <si>
-    <t>ISLA ARBOLEDA</t>
-  </si>
-  <si>
-    <t>ISLA AZTECA</t>
-  </si>
-  <si>
-    <t>ISLA CEDROS</t>
-  </si>
-  <si>
-    <t>ISLA MIRAMAR</t>
-  </si>
-  <si>
-    <t>ISLA VERDE</t>
-  </si>
-  <si>
-    <t>ISLA SANTA CRUZ</t>
-  </si>
-  <si>
-    <t>ISLA BLANCA</t>
-  </si>
-  <si>
-    <t>ISLA CIARI</t>
-  </si>
-  <si>
-    <t>ISLA JANITZIO</t>
-  </si>
-  <si>
-    <t>ISLA SAN IGNACIO</t>
-  </si>
-  <si>
-    <t>ISLA SAN GABRIEL</t>
-  </si>
-  <si>
-    <t>ISLA SAN DIEGO</t>
-  </si>
-  <si>
-    <t>AJUSTE INFONAVIT</t>
-  </si>
-  <si>
-    <t>INFONAVIT BIMESTRE ATERIOR</t>
-  </si>
-  <si>
-    <t>Prestamo Personal Asimilado</t>
-  </si>
-  <si>
-    <t>Adeudo_Infonavit_Asimilado</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>ISLA CRECIENTE</t>
-  </si>
-  <si>
-    <t>ISLA GRANDE</t>
-  </si>
-  <si>
-    <t>ISLA SAN JOSE</t>
-  </si>
-  <si>
-    <t>ISLA LEON</t>
-  </si>
-  <si>
-    <t>ISLA SAN LUIS</t>
-  </si>
-  <si>
-    <t>ISLA COLORADA</t>
-  </si>
-  <si>
-    <t>ISLA PASSAVERA</t>
-  </si>
-  <si>
-    <t>ISLA MARGOT MARIANNE</t>
-  </si>
-  <si>
-    <t>FONACOT</t>
-  </si>
-  <si>
-    <t>NOMBRE TRABAJADOR</t>
-  </si>
-  <si>
-    <t>NOMBRE BENFICIARIO</t>
-  </si>
-  <si>
-    <t>PORCENTAJE</t>
-  </si>
-  <si>
-    <t>MONTO ABORDO</t>
-  </si>
-  <si>
-    <t>MONTO DESCANSO</t>
-  </si>
-  <si>
-    <t>SUBSEA88</t>
-  </si>
-  <si>
-    <t>MONTO</t>
-  </si>
-  <si>
-    <t>DESCUENTO</t>
-  </si>
-  <si>
-    <t>TOTAL FALTANTE</t>
-  </si>
-  <si>
-    <t>TIPO DESCUENTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESCUENTO </t>
-  </si>
-  <si>
-    <t>TOTAL COBRADO</t>
-  </si>
-  <si>
-    <t>RETENCION DEL 6%</t>
-  </si>
-  <si>
-    <t>RETENCION 6%</t>
-  </si>
-  <si>
-    <t>INFONAVIT BIM ANTERIOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "TMM DIVISION"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "DEPOSITO ROUTES SCOTIABANK"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "IVA"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "RETENCION 6%"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "DEPOSITO BIRYUSA SCOTIABANK"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "TOTAL DEPOSITO BIRYUSA"</t>
-  </si>
-  <si>
-    <t>).Value =</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hoja.Cell(sep + 4, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">hoja.Cell(sep + 5, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">hoja.Cell(sep + 7, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">hoja.Cell(sep + 9, </t>
-  </si>
-  <si>
-    <t>).Value ="</t>
-  </si>
-  <si>
-    <t>"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hoja.Cell(sep + 6, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">hoja.Cell(sep + 8, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">hoja.Cell(sep + 10, </t>
-  </si>
-  <si>
-    <t>hoja.Cell(sep + 3,</t>
-  </si>
-  <si>
-    <t>amarrados</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> azteca</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cedros</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> miramar</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> verde</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cruz</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> montserrat</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> blanca</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ciari</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> janitzio</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> luis</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ignacio</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> gabriel</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> diego</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> jose</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> grande</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> creciente</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> colorada</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> subsea88</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> leon</t>
-  </si>
-  <si>
-    <t>passavera</t>
-  </si>
-  <si>
-    <t>margot</t>
-  </si>
-  <si>
-    <t>"=V" &amp;</t>
-  </si>
-  <si>
-    <t>+1</t>
-  </si>
-  <si>
-    <t>+1 &amp; " + X" &amp;</t>
-  </si>
-  <si>
-    <t>+1 &amp; " + Z"&amp;</t>
-  </si>
-  <si>
-    <t>+1 &amp; "+AB" &amp;</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "TOTAL DEPOSITO OPERADORA"</t>
-  </si>
-  <si>
-    <t>"=</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &amp; sep +4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &amp; sep +3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &amp; sep +5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &amp; "*16%"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &amp;" *6%"</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &amp; </t>
-  </si>
-  <si>
-    <t>+1 &amp; "+AA" &amp;</t>
-  </si>
-  <si>
-    <t>+1 &amp; "+Q" &amp;</t>
-  </si>
-  <si>
-    <t>"=W" &amp;</t>
-  </si>
-  <si>
-    <t>).FormulaA1 =</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &amp; sep +7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &amp; sep +8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &amp; sep +9</t>
-  </si>
-  <si>
-    <t>.Style.Fill.BackgroundColor = XLColor.YellowProcess</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &amp; sep +6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &amp; sep +10</t>
-  </si>
-  <si>
-    <t>hoja.Range(</t>
-  </si>
-  <si>
-    <t>AMARRADOS</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>.Style.Fill.BackgroundColor = XLColor.PowderBlue</t>
-  </si>
-  <si>
-    <t>hoja.Cell(</t>
-  </si>
-  <si>
-    <t>NEVADO DE COLIMA</t>
-  </si>
-  <si>
-    <t>nevado</t>
-  </si>
-  <si>
-    <t>PROYECTO LODEROS1</t>
-  </si>
-  <si>
-    <t>PROYECTO MAERSK</t>
-  </si>
-  <si>
-    <t>loderos1</t>
-  </si>
-  <si>
-    <t>maersk</t>
-  </si>
-  <si>
-    <t>RED FISH</t>
-  </si>
-  <si>
-    <t>PROYECTO BELUGA 2</t>
-  </si>
-  <si>
-    <t>PROYECTO GO CANOPUS</t>
-  </si>
-  <si>
-    <t>SOVER</t>
-  </si>
-  <si>
-    <t>TRANSPORTES SOVER SA DE CV</t>
-  </si>
-  <si>
-    <t>VALORES AGREGADOS</t>
-  </si>
-  <si>
-    <t>PFB CORTO PLAZO</t>
-  </si>
-  <si>
-    <t>FONDO PFB 3%</t>
-  </si>
-  <si>
-    <t>COMISIÓN  OPERADORA (4%)</t>
-  </si>
-  <si>
-    <t>COMISIÓN PLAN PENSIONES(8%)</t>
-  </si>
-  <si>
-    <t>IKE</t>
-  </si>
-  <si>
-    <t>PLAN FLEX LP</t>
-  </si>
-  <si>
-    <t>APOR PATRON PLAN FLEX LP</t>
-  </si>
-  <si>
-    <t>SA</t>
-  </si>
-  <si>
-    <t>NETO</t>
-  </si>
-  <si>
-    <t>DESCUENTO PPP</t>
-  </si>
-  <si>
-    <t>TOTAL DEDUCCIONES</t>
-  </si>
-  <si>
-    <t>GANNET</t>
-  </si>
-  <si>
-    <t>Pension Alimentica  IKE</t>
-  </si>
-  <si>
-    <t>PENSION ALIMENTICIA PPP</t>
-  </si>
-  <si>
-    <t>DEP</t>
-  </si>
-  <si>
-    <t>AURORA PEARL</t>
-  </si>
-  <si>
-    <t>WORLD PERIDOT</t>
-  </si>
-  <si>
-    <t>AGENCIA GROESSINGER SAPI DE CV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  VSM IKE  </t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>50</t>
+    <t>Adeudo_Infonavit_IKE</t>
   </si>
 </sst>
 </file>
@@ -878,7 +878,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;???_-;_-@_-"/>
   </numFmts>
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="47" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1169,6 +1169,11 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1527,7 +1532,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1491">
+  <cellStyleXfs count="1492">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3019,8 +3024,9 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3460,6 +3466,7 @@
     <xf numFmtId="4" fontId="16" fillId="15" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="33" fillId="0" borderId="0" xfId="1491" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3492,8 +3499,11 @@
     <xf numFmtId="0" fontId="27" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1491">
+  <cellStyles count="1492">
     <cellStyle name="Euro" xfId="1"/>
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Millares 2" xfId="3"/>
@@ -4939,6 +4949,7 @@
     <cellStyle name="Normal 98" xfId="1438"/>
     <cellStyle name="Normal 98 2" xfId="1439"/>
     <cellStyle name="Normal 99" xfId="1440"/>
+    <cellStyle name="Porcentaje" xfId="1491" builtinId="5"/>
     <cellStyle name="Porcentaje 2" xfId="1441"/>
     <cellStyle name="Porcentaje 2 10" xfId="1442"/>
     <cellStyle name="Porcentaje 2 10 2" xfId="1443"/>
@@ -5715,11 +5726,11 @@
   <dimension ref="B1:BK15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="W13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A11" sqref="A11"/>
       <selection pane="topRight" activeCell="F11" sqref="F11"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="AH11" sqref="AH11:AH12"/>
+      <selection pane="bottomRight" activeCell="AF11" sqref="AF1:AF1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5751,7 +5762,7 @@
     <col min="29" max="29" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.85546875" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="18.42578125" hidden="1" customWidth="1"/>
     <col min="33" max="33" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6396,90 +6407,90 @@
       <c r="BK10" s="50"/>
     </row>
     <row r="11" spans="2:63" s="84" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="209" t="s">
+      <c r="B11" s="210" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="209" t="s">
+      <c r="C11" s="210" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="209" t="s">
+      <c r="D11" s="210" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="209" t="s">
+      <c r="E11" s="210" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="209" t="s">
+      <c r="F11" s="210" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="209" t="s">
+      <c r="G11" s="210" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="209" t="s">
+      <c r="H11" s="210" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="209" t="s">
+      <c r="I11" s="210" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="209" t="s">
+      <c r="J11" s="210" t="s">
         <v>54</v>
       </c>
-      <c r="K11" s="209" t="s">
+      <c r="K11" s="210" t="s">
         <v>53</v>
       </c>
-      <c r="L11" s="209" t="s">
+      <c r="L11" s="210" t="s">
         <v>4</v>
       </c>
-      <c r="M11" s="209" t="s">
+      <c r="M11" s="210" t="s">
         <v>56</v>
       </c>
-      <c r="N11" s="211" t="s">
-        <v>114</v>
-      </c>
-      <c r="O11" s="211" t="s">
-        <v>210</v>
-      </c>
-      <c r="P11" s="209" t="s">
+      <c r="N11" s="212" t="s">
+        <v>262</v>
+      </c>
+      <c r="O11" s="212" t="s">
+        <v>206</v>
+      </c>
+      <c r="P11" s="210" t="s">
         <v>66</v>
       </c>
       <c r="Q11" s="128"/>
-      <c r="R11" s="209" t="s">
+      <c r="R11" s="210" t="s">
         <v>47</v>
       </c>
       <c r="S11" s="131"/>
       <c r="T11" s="131"/>
-      <c r="U11" s="209" t="s">
+      <c r="U11" s="210" t="s">
         <v>52</v>
       </c>
-      <c r="V11" s="209" t="s">
+      <c r="V11" s="210" t="s">
+        <v>191</v>
+      </c>
+      <c r="W11" s="211" t="s">
         <v>194</v>
       </c>
-      <c r="W11" s="210" t="s">
-        <v>197</v>
-      </c>
       <c r="X11" s="197"/>
-      <c r="Y11" s="209" t="s">
-        <v>67</v>
+      <c r="Y11" s="210" t="s">
+        <v>264</v>
       </c>
       <c r="Z11" s="85"/>
-      <c r="AA11" s="209" t="s">
-        <v>199</v>
-      </c>
-      <c r="AB11" s="210" t="s">
-        <v>200</v>
-      </c>
-      <c r="AC11" s="209" t="s">
+      <c r="AA11" s="210" t="s">
+        <v>263</v>
+      </c>
+      <c r="AB11" s="211" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC11" s="210" t="s">
         <v>5</v>
       </c>
-      <c r="AD11" s="209" t="s">
+      <c r="AD11" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="AE11" s="212" t="s">
+      <c r="AE11" s="213" t="s">
         <v>18</v>
       </c>
-      <c r="AF11" s="209" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG11" s="209" t="s">
+      <c r="AF11" s="210" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG11" s="210" t="s">
         <v>1</v>
       </c>
       <c r="AH11"/>
@@ -6512,48 +6523,48 @@
       <c r="BJ11" s="83"/>
     </row>
     <row r="12" spans="2:63" s="86" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="209"/>
-      <c r="C12" s="209"/>
-      <c r="D12" s="209"/>
-      <c r="E12" s="209"/>
-      <c r="F12" s="209"/>
-      <c r="G12" s="209"/>
-      <c r="H12" s="209"/>
-      <c r="I12" s="209"/>
-      <c r="J12" s="209"/>
-      <c r="K12" s="209"/>
-      <c r="L12" s="209"/>
-      <c r="M12" s="209"/>
-      <c r="N12" s="211"/>
-      <c r="O12" s="211"/>
-      <c r="P12" s="209"/>
+      <c r="B12" s="210"/>
+      <c r="C12" s="210"/>
+      <c r="D12" s="210"/>
+      <c r="E12" s="210"/>
+      <c r="F12" s="210"/>
+      <c r="G12" s="210"/>
+      <c r="H12" s="210"/>
+      <c r="I12" s="210"/>
+      <c r="J12" s="210"/>
+      <c r="K12" s="210"/>
+      <c r="L12" s="210"/>
+      <c r="M12" s="210"/>
+      <c r="N12" s="212"/>
+      <c r="O12" s="212"/>
+      <c r="P12" s="210"/>
       <c r="Q12" s="128" t="s">
-        <v>206</v>
-      </c>
-      <c r="R12" s="209" t="s">
+        <v>202</v>
+      </c>
+      <c r="R12" s="210" t="s">
         <v>57</v>
       </c>
       <c r="S12" s="131" t="s">
         <v>60</v>
       </c>
       <c r="T12" s="131" t="s">
-        <v>99</v>
-      </c>
-      <c r="U12" s="209"/>
-      <c r="V12" s="209"/>
-      <c r="W12" s="210"/>
+        <v>97</v>
+      </c>
+      <c r="U12" s="210"/>
+      <c r="V12" s="210"/>
+      <c r="W12" s="211"/>
       <c r="X12" s="197" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y12" s="209"/>
+        <v>195</v>
+      </c>
+      <c r="Y12" s="210"/>
       <c r="Z12" s="85"/>
-      <c r="AA12" s="209"/>
-      <c r="AB12" s="210"/>
-      <c r="AC12" s="209"/>
-      <c r="AD12" s="209"/>
-      <c r="AE12" s="212"/>
-      <c r="AF12" s="209"/>
-      <c r="AG12" s="209"/>
+      <c r="AA12" s="210"/>
+      <c r="AB12" s="211"/>
+      <c r="AC12" s="210"/>
+      <c r="AD12" s="210"/>
+      <c r="AE12" s="213"/>
+      <c r="AF12" s="210"/>
+      <c r="AG12" s="210"/>
       <c r="AH12"/>
       <c r="AI12" s="87"/>
       <c r="AJ12" s="88"/>
@@ -6722,10 +6733,10 @@
   <dimension ref="A1:KJ51"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="10" ySplit="8" topLeftCell="AU9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="8" topLeftCell="BE9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="N9" sqref="L9:BG9"/>
+      <selection pane="bottomRight" activeCell="BF1" sqref="BF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6763,19 +6774,20 @@
     <col min="41" max="42" width="13.42578125" customWidth="1"/>
     <col min="43" max="49" width="14.28515625" customWidth="1"/>
     <col min="50" max="50" width="12.28515625" customWidth="1"/>
-    <col min="51" max="58" width="11.42578125" style="10" customWidth="1"/>
+    <col min="51" max="57" width="11.42578125" style="10" customWidth="1"/>
+    <col min="58" max="58" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:296" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="27"/>
-      <c r="B1" s="213" t="s">
+      <c r="B1" s="214" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="214"/>
-      <c r="D1" s="214"/>
-      <c r="E1" s="214"/>
-      <c r="F1" s="214"/>
+      <c r="C1" s="215"/>
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
+      <c r="F1" s="215"/>
       <c r="G1" s="64"/>
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
@@ -6824,7 +6836,7 @@
     <row r="2" spans="1:296" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="195" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C2" s="65"/>
       <c r="D2" s="51"/>
@@ -6877,13 +6889,13 @@
     </row>
     <row r="3" spans="1:296" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
-      <c r="B3" s="215" t="s">
+      <c r="B3" s="216" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="214"/>
-      <c r="D3" s="214"/>
-      <c r="E3" s="214"/>
-      <c r="F3" s="214"/>
+      <c r="C3" s="215"/>
+      <c r="D3" s="215"/>
+      <c r="E3" s="215"/>
+      <c r="F3" s="215"/>
       <c r="G3" s="66"/>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
@@ -6937,13 +6949,13 @@
     </row>
     <row r="4" spans="1:296" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
-      <c r="B4" s="216" t="s">
+      <c r="B4" s="217" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="217"/>
-      <c r="D4" s="217"/>
-      <c r="E4" s="217"/>
-      <c r="F4" s="217"/>
+      <c r="C4" s="218"/>
+      <c r="D4" s="218"/>
+      <c r="E4" s="218"/>
+      <c r="F4" s="218"/>
       <c r="G4" s="66"/>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
@@ -7297,7 +7309,7 @@
         <v>49</v>
       </c>
       <c r="O8" s="208" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="P8" s="45" t="s">
         <v>30</v>
@@ -7345,10 +7357,10 @@
         <v>43</v>
       </c>
       <c r="AE8" s="200" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="AF8" s="200" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="AG8" s="202" t="s">
         <v>44</v>
@@ -7369,10 +7381,10 @@
         <v>10</v>
       </c>
       <c r="AM8" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AN8" s="45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AO8" s="45" t="s">
         <v>47</v>
@@ -7384,22 +7396,22 @@
         <v>60</v>
       </c>
       <c r="AR8" s="127" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AS8" s="200" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="AT8" s="200" t="s">
+        <v>199</v>
+      </c>
+      <c r="AU8" s="205" t="s">
         <v>203</v>
       </c>
-      <c r="AU8" s="205" t="s">
-        <v>207</v>
-      </c>
       <c r="AV8" s="201" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="AW8" s="173" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AX8" s="175" t="s">
         <v>23</v>
@@ -7414,7 +7426,7 @@
         <v>62</v>
       </c>
       <c r="BB8" s="196" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="BC8" s="177" t="s">
         <v>63</v>
@@ -7423,13 +7435,13 @@
         <v>64</v>
       </c>
       <c r="BE8" s="174" t="s">
-        <v>88</v>
-      </c>
-      <c r="BF8" s="127" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="BF8" s="222" t="s">
+        <v>265</v>
       </c>
       <c r="BG8" s="200" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="BH8" s="10"/>
       <c r="BI8" s="10"/>
@@ -9938,13 +9950,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja3"/>
-  <dimension ref="A1:CW59"/>
+  <dimension ref="A1:CV59"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="8" ySplit="8" topLeftCell="AC9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="8" topLeftCell="AM9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9:AX9"/>
+      <selection pane="bottomRight" activeCell="AQ44" sqref="AQ44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9983,20 +9995,21 @@
     <col min="42" max="42" width="11.42578125" style="10"/>
     <col min="43" max="47" width="14.28515625" customWidth="1"/>
     <col min="48" max="48" width="12.42578125" customWidth="1"/>
-    <col min="49" max="50" width="11.42578125" style="10" customWidth="1"/>
-    <col min="51" max="51" width="11.42578125" style="10" hidden="1" customWidth="1"/>
-    <col min="52" max="58" width="11.42578125" style="10"/>
+    <col min="49" max="49" width="11.42578125" style="10" customWidth="1"/>
+    <col min="50" max="50" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.42578125" style="10" customWidth="1"/>
+    <col min="52" max="57" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:100" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="27"/>
-      <c r="B1" s="213" t="s">
+      <c r="B1" s="214" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="214"/>
-      <c r="D1" s="214"/>
-      <c r="E1" s="214"/>
-      <c r="F1" s="214"/>
+      <c r="C1" s="215"/>
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
+      <c r="F1" s="215"/>
       <c r="G1" s="24"/>
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
@@ -10038,10 +10051,10 @@
       <c r="AT1" s="24"/>
       <c r="AU1" s="24"/>
     </row>
-    <row r="2" spans="1:101" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:100" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="195" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
@@ -10088,15 +10101,15 @@
       <c r="AT2" s="24"/>
       <c r="AU2" s="24"/>
     </row>
-    <row r="3" spans="1:101" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:100" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
-      <c r="B3" s="215" t="s">
+      <c r="B3" s="216" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="214"/>
-      <c r="D3" s="214"/>
-      <c r="E3" s="214"/>
-      <c r="F3" s="214"/>
+      <c r="C3" s="215"/>
+      <c r="D3" s="215"/>
+      <c r="E3" s="215"/>
+      <c r="F3" s="215"/>
       <c r="G3" s="30"/>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
@@ -10147,17 +10160,16 @@
       <c r="BC3" s="109"/>
       <c r="BD3" s="109"/>
       <c r="BE3" s="109"/>
-      <c r="BF3" s="109"/>
-    </row>
-    <row r="4" spans="1:101" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:100" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
-      <c r="B4" s="216" t="s">
+      <c r="B4" s="217" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="217"/>
-      <c r="D4" s="217"/>
-      <c r="E4" s="217"/>
-      <c r="F4" s="217"/>
+      <c r="C4" s="218"/>
+      <c r="D4" s="218"/>
+      <c r="E4" s="218"/>
+      <c r="F4" s="218"/>
       <c r="G4" s="66"/>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
@@ -10199,7 +10211,7 @@
       <c r="AT4" s="24"/>
       <c r="AU4" s="24"/>
     </row>
-    <row r="5" spans="1:101" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:100" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="29"/>
       <c r="C5" s="24"/>
@@ -10247,7 +10259,7 @@
       <c r="AT5" s="24"/>
       <c r="AU5" s="24"/>
     </row>
-    <row r="6" spans="1:101" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:100" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="29"/>
       <c r="C6" s="24"/>
@@ -10295,6 +10307,7 @@
       <c r="AT6" s="24"/>
       <c r="AU6" s="24"/>
       <c r="AV6"/>
+      <c r="BF6"/>
       <c r="BG6"/>
       <c r="BH6"/>
       <c r="BI6"/>
@@ -10337,9 +10350,8 @@
       <c r="CT6"/>
       <c r="CU6"/>
       <c r="CV6"/>
-      <c r="CW6"/>
-    </row>
-    <row r="7" spans="1:101" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:100" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
@@ -10378,7 +10390,7 @@
       <c r="BC7" s="109"/>
       <c r="BD7" s="109"/>
       <c r="BE7" s="109"/>
-      <c r="BF7" s="109"/>
+      <c r="BF7" s="9"/>
       <c r="BG7" s="9"/>
       <c r="BH7" s="9"/>
       <c r="BI7" s="9"/>
@@ -10421,9 +10433,8 @@
       <c r="CT7" s="9"/>
       <c r="CU7" s="9"/>
       <c r="CV7" s="9"/>
-      <c r="CW7" s="9"/>
-    </row>
-    <row r="8" spans="1:101" s="45" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:100" s="45" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
         <v>16</v>
       </c>
@@ -10530,10 +10541,10 @@
         <v>10</v>
       </c>
       <c r="AJ8" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AK8" s="45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AL8" s="45" t="s">
         <v>47</v>
@@ -10545,7 +10556,7 @@
         <v>60</v>
       </c>
       <c r="AO8" s="127" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AP8" s="126" t="s">
         <v>48</v>
@@ -10569,13 +10580,13 @@
         <v>64</v>
       </c>
       <c r="AW8" s="127" t="s">
-        <v>88</v>
-      </c>
-      <c r="AX8" s="127" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="AX8" s="222" t="s">
+        <v>265</v>
       </c>
       <c r="AY8" s="200" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="AZ8" s="10"/>
       <c r="BA8" s="10"/>
@@ -10626,161 +10637,160 @@
       <c r="CT8" s="10"/>
       <c r="CU8" s="10"/>
       <c r="CV8" s="10"/>
-      <c r="CW8" s="10"/>
-    </row>
-    <row r="9" spans="1:101" s="78" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:100" s="78" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="49" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E9" s="49" t="s">
         <v>216</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="G9" s="49" t="s">
         <v>218</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="I9" s="49" t="s">
         <v>220</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="G9" s="49" t="s">
+      <c r="K9" s="49" t="s">
         <v>222</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="I9" s="49" t="s">
+      <c r="M9" s="49" t="s">
         <v>224</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="N9" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="K9" s="49" t="s">
+      <c r="O9" s="49" t="s">
         <v>226</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="P9" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="M9" s="49" t="s">
+      <c r="Q9" s="49" t="s">
         <v>228</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="R9" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="O9" s="49" t="s">
+      <c r="S9" s="49" t="s">
         <v>230</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="T9" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="Q9" s="49" t="s">
+      <c r="U9" s="49" t="s">
         <v>232</v>
       </c>
-      <c r="R9" s="5" t="s">
+      <c r="V9" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="S9" s="49" t="s">
+      <c r="W9" s="49" t="s">
         <v>234</v>
       </c>
-      <c r="T9" s="5" t="s">
+      <c r="X9" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="U9" s="49" t="s">
+      <c r="Y9" s="49" t="s">
         <v>236</v>
       </c>
-      <c r="V9" s="5" t="s">
+      <c r="Z9" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="W9" s="49" t="s">
+      <c r="AA9" s="49" t="s">
         <v>238</v>
       </c>
-      <c r="X9" s="5" t="s">
+      <c r="AB9" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="Y9" s="49" t="s">
+      <c r="AC9" s="49" t="s">
         <v>240</v>
       </c>
-      <c r="Z9" s="5" t="s">
+      <c r="AD9" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="AA9" s="49" t="s">
+      <c r="AE9" s="49" t="s">
         <v>242</v>
       </c>
-      <c r="AB9" s="5" t="s">
+      <c r="AF9" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="AC9" s="49" t="s">
+      <c r="AG9" s="49" t="s">
         <v>244</v>
       </c>
-      <c r="AD9" s="5" t="s">
+      <c r="AH9" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="AE9" s="49" t="s">
+      <c r="AI9" s="49" t="s">
         <v>246</v>
       </c>
-      <c r="AF9" s="5" t="s">
+      <c r="AJ9" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="AG9" s="49" t="s">
+      <c r="AK9" s="49" t="s">
         <v>248</v>
       </c>
-      <c r="AH9" s="5" t="s">
+      <c r="AL9" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="AI9" s="49" t="s">
+      <c r="AM9" s="49" t="s">
         <v>250</v>
       </c>
-      <c r="AJ9" s="5" t="s">
+      <c r="AN9" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="AK9" s="49" t="s">
+      <c r="AO9" s="49" t="s">
         <v>252</v>
       </c>
-      <c r="AL9" s="5" t="s">
+      <c r="AP9" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="AM9" s="49" t="s">
+      <c r="AQ9" s="49" t="s">
         <v>254</v>
       </c>
-      <c r="AN9" s="5" t="s">
+      <c r="AR9" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="AO9" s="49" t="s">
+      <c r="AS9" s="49" t="s">
         <v>256</v>
       </c>
-      <c r="AP9" s="5" t="s">
+      <c r="AT9" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="AQ9" s="49" t="s">
+      <c r="AU9" s="49" t="s">
         <v>258</v>
       </c>
-      <c r="AR9" s="5" t="s">
+      <c r="AV9" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="AS9" s="49" t="s">
+      <c r="AW9" s="49" t="s">
         <v>260</v>
       </c>
-      <c r="AT9" s="5" t="s">
+      <c r="AX9" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="AU9" s="49" t="s">
-        <v>262</v>
-      </c>
-      <c r="AV9" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="AW9" s="49" t="s">
-        <v>264</v>
-      </c>
-      <c r="AX9" s="5" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="10" spans="1:101" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:100" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="49"/>
       <c r="B10" s="5"/>
       <c r="C10" s="62"/>
@@ -10825,7 +10835,7 @@
       <c r="AU10" s="48"/>
       <c r="AV10" s="53"/>
     </row>
-    <row r="11" spans="1:101" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:100" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="49"/>
       <c r="B11" s="5"/>
       <c r="C11" s="62"/>
@@ -10872,9 +10882,8 @@
       <c r="AW11" s="48"/>
       <c r="AX11" s="48"/>
       <c r="AY11" s="48"/>
-      <c r="AZ11" s="48"/>
-    </row>
-    <row r="12" spans="1:101" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:100" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
       <c r="B12" s="5"/>
       <c r="C12" s="62"/>
@@ -10921,9 +10930,8 @@
       <c r="AW12" s="48"/>
       <c r="AX12" s="48"/>
       <c r="AY12" s="48"/>
-      <c r="AZ12" s="48"/>
-    </row>
-    <row r="13" spans="1:101" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:100" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="5"/>
       <c r="C13" s="62"/>
@@ -10970,9 +10978,8 @@
       <c r="AW13" s="48"/>
       <c r="AX13" s="48"/>
       <c r="AY13" s="48"/>
-      <c r="AZ13" s="48"/>
-    </row>
-    <row r="14" spans="1:101" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:100" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="49"/>
       <c r="B14" s="5"/>
       <c r="C14" s="62"/>
@@ -11019,9 +11026,8 @@
       <c r="AW14" s="48"/>
       <c r="AX14" s="48"/>
       <c r="AY14" s="48"/>
-      <c r="AZ14" s="48"/>
-    </row>
-    <row r="15" spans="1:101" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:100" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="49"/>
       <c r="B15" s="5"/>
       <c r="C15" s="62"/>
@@ -11068,9 +11074,8 @@
       <c r="AW15" s="48"/>
       <c r="AX15" s="48"/>
       <c r="AY15" s="48"/>
-      <c r="AZ15" s="48"/>
-    </row>
-    <row r="16" spans="1:101" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:100" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="49"/>
       <c r="B16" s="5"/>
       <c r="C16" s="62"/>
@@ -11117,9 +11122,8 @@
       <c r="AW16" s="48"/>
       <c r="AX16" s="48"/>
       <c r="AY16" s="48"/>
-      <c r="AZ16" s="48"/>
-    </row>
-    <row r="17" spans="1:52" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:51" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="49"/>
       <c r="B17" s="5"/>
       <c r="C17" s="62"/>
@@ -11166,9 +11170,8 @@
       <c r="AW17" s="48"/>
       <c r="AX17" s="48"/>
       <c r="AY17" s="48"/>
-      <c r="AZ17" s="48"/>
-    </row>
-    <row r="18" spans="1:52" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:51" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="49"/>
       <c r="B18" s="5"/>
       <c r="C18" s="62"/>
@@ -11214,9 +11217,8 @@
       <c r="AW18" s="48"/>
       <c r="AX18" s="48"/>
       <c r="AY18" s="48"/>
-      <c r="AZ18" s="48"/>
-    </row>
-    <row r="19" spans="1:52" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:51" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="49"/>
       <c r="B19" s="5"/>
       <c r="C19" s="62"/>
@@ -11261,9 +11263,8 @@
       <c r="AW19" s="48"/>
       <c r="AX19" s="48"/>
       <c r="AY19" s="48"/>
-      <c r="AZ19" s="48"/>
-    </row>
-    <row r="20" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="46"/>
       <c r="B20" s="38"/>
       <c r="C20" s="40"/>
@@ -11315,9 +11316,8 @@
       <c r="AW20" s="48"/>
       <c r="AX20" s="48"/>
       <c r="AY20" s="48"/>
-      <c r="AZ20" s="48"/>
-    </row>
-    <row r="21" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="46"/>
       <c r="B21" s="38"/>
       <c r="C21" s="40"/>
@@ -11368,9 +11368,8 @@
       <c r="AW21" s="48"/>
       <c r="AX21" s="48"/>
       <c r="AY21" s="48"/>
-      <c r="AZ21" s="48"/>
-    </row>
-    <row r="22" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="46"/>
       <c r="B22" s="38"/>
       <c r="C22" s="40"/>
@@ -11421,9 +11420,8 @@
       <c r="AW22" s="48"/>
       <c r="AX22" s="48"/>
       <c r="AY22" s="48"/>
-      <c r="AZ22" s="48"/>
-    </row>
-    <row r="23" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="46"/>
       <c r="B23" s="38"/>
       <c r="C23" s="40"/>
@@ -11474,9 +11472,8 @@
       <c r="AW23" s="48"/>
       <c r="AX23" s="48"/>
       <c r="AY23" s="48"/>
-      <c r="AZ23" s="48"/>
-    </row>
-    <row r="24" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="46"/>
       <c r="B24" s="38"/>
       <c r="C24" s="40"/>
@@ -11527,9 +11524,8 @@
       <c r="AW24" s="48"/>
       <c r="AX24" s="48"/>
       <c r="AY24" s="48"/>
-      <c r="AZ24" s="48"/>
-    </row>
-    <row r="25" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
       <c r="B25" s="38"/>
       <c r="C25" s="40"/>
@@ -11580,9 +11576,8 @@
       <c r="AW25" s="48"/>
       <c r="AX25" s="48"/>
       <c r="AY25" s="48"/>
-      <c r="AZ25" s="48"/>
-    </row>
-    <row r="26" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="46"/>
       <c r="B26" s="38"/>
       <c r="C26" s="40"/>
@@ -11633,9 +11628,8 @@
       <c r="AW26" s="48"/>
       <c r="AX26" s="48"/>
       <c r="AY26" s="48"/>
-      <c r="AZ26" s="48"/>
-    </row>
-    <row r="27" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="46"/>
       <c r="B27" s="38"/>
       <c r="C27" s="40"/>
@@ -11686,9 +11680,8 @@
       <c r="AW27" s="48"/>
       <c r="AX27" s="48"/>
       <c r="AY27" s="48"/>
-      <c r="AZ27" s="48"/>
-    </row>
-    <row r="28" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="46"/>
       <c r="B28" s="38"/>
       <c r="C28" s="40"/>
@@ -11739,9 +11732,8 @@
       <c r="AW28" s="48"/>
       <c r="AX28" s="48"/>
       <c r="AY28" s="48"/>
-      <c r="AZ28" s="48"/>
-    </row>
-    <row r="29" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="46"/>
       <c r="B29" s="38"/>
       <c r="C29" s="40"/>
@@ -11792,9 +11784,8 @@
       <c r="AW29" s="48"/>
       <c r="AX29" s="48"/>
       <c r="AY29" s="48"/>
-      <c r="AZ29" s="48"/>
-    </row>
-    <row r="30" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="46"/>
       <c r="B30" s="38"/>
       <c r="C30" s="40"/>
@@ -11845,9 +11836,8 @@
       <c r="AW30" s="48"/>
       <c r="AX30" s="48"/>
       <c r="AY30" s="48"/>
-      <c r="AZ30" s="48"/>
-    </row>
-    <row r="31" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="39"/>
       <c r="B31" s="38"/>
       <c r="C31" s="40"/>
@@ -11898,9 +11888,8 @@
       <c r="AW31" s="48"/>
       <c r="AX31" s="48"/>
       <c r="AY31" s="48"/>
-      <c r="AZ31" s="48"/>
-    </row>
-    <row r="32" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="39"/>
       <c r="B32" s="38"/>
       <c r="C32" s="40"/>
@@ -11951,9 +11940,8 @@
       <c r="AW32" s="48"/>
       <c r="AX32" s="48"/>
       <c r="AY32" s="48"/>
-      <c r="AZ32" s="48"/>
-    </row>
-    <row r="33" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="39"/>
       <c r="B33" s="38"/>
       <c r="C33" s="40"/>
@@ -12004,9 +11992,8 @@
       <c r="AW33" s="48"/>
       <c r="AX33" s="48"/>
       <c r="AY33" s="48"/>
-      <c r="AZ33" s="48"/>
-    </row>
-    <row r="34" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="39"/>
       <c r="B34" s="38"/>
       <c r="C34" s="40"/>
@@ -12057,9 +12044,8 @@
       <c r="AW34" s="48"/>
       <c r="AX34" s="48"/>
       <c r="AY34" s="48"/>
-      <c r="AZ34" s="48"/>
-    </row>
-    <row r="35" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="35"/>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
@@ -12110,9 +12096,8 @@
       <c r="AW35" s="48"/>
       <c r="AX35" s="48"/>
       <c r="AY35" s="48"/>
-      <c r="AZ35" s="48"/>
-    </row>
-    <row r="36" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
       <c r="B36" s="24"/>
       <c r="C36" s="36"/>
@@ -12163,9 +12148,8 @@
       <c r="AW36" s="48"/>
       <c r="AX36" s="48"/>
       <c r="AY36" s="48"/>
-      <c r="AZ36" s="48"/>
-    </row>
-    <row r="37" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
@@ -12216,9 +12200,8 @@
       <c r="AW37" s="48"/>
       <c r="AX37" s="48"/>
       <c r="AY37" s="48"/>
-      <c r="AZ37" s="48"/>
-    </row>
-    <row r="38" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
       <c r="B38" s="24"/>
       <c r="C38" s="24"/>
@@ -12269,9 +12252,8 @@
       <c r="AW38" s="48"/>
       <c r="AX38" s="48"/>
       <c r="AY38" s="48"/>
-      <c r="AZ38" s="48"/>
-    </row>
-    <row r="39" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="39"/>
       <c r="B39" s="38"/>
       <c r="C39" s="40"/>
@@ -12322,9 +12304,8 @@
       <c r="AW39" s="48"/>
       <c r="AX39" s="48"/>
       <c r="AY39" s="48"/>
-      <c r="AZ39" s="48"/>
-    </row>
-    <row r="40" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="39"/>
       <c r="B40" s="38"/>
       <c r="C40" s="40"/>
@@ -12375,9 +12356,8 @@
       <c r="AW40" s="48"/>
       <c r="AX40" s="48"/>
       <c r="AY40" s="48"/>
-      <c r="AZ40" s="48"/>
-    </row>
-    <row r="41" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="35"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
@@ -12428,9 +12408,8 @@
       <c r="AW41" s="48"/>
       <c r="AX41" s="48"/>
       <c r="AY41" s="48"/>
-      <c r="AZ41" s="48"/>
-    </row>
-    <row r="42" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="24"/>
       <c r="C42" s="36"/>
@@ -12481,9 +12460,8 @@
       <c r="AW42" s="48"/>
       <c r="AX42" s="48"/>
       <c r="AY42" s="48"/>
-      <c r="AZ42" s="48"/>
-    </row>
-    <row r="43" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
       <c r="B43" s="21"/>
       <c r="C43" s="22"/>
@@ -12534,9 +12512,8 @@
       <c r="AW43" s="48"/>
       <c r="AX43" s="48"/>
       <c r="AY43" s="48"/>
-      <c r="AZ43" s="48"/>
-    </row>
-    <row r="44" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="31"/>
       <c r="B44" s="24"/>
       <c r="C44" s="24"/>
@@ -12587,9 +12564,8 @@
       <c r="AW44" s="48"/>
       <c r="AX44" s="48"/>
       <c r="AY44" s="48"/>
-      <c r="AZ44" s="48"/>
-    </row>
-    <row r="45" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="39"/>
       <c r="B45" s="38"/>
       <c r="C45" s="40"/>
@@ -12640,9 +12616,8 @@
       <c r="AW45" s="48"/>
       <c r="AX45" s="48"/>
       <c r="AY45" s="48"/>
-      <c r="AZ45" s="48"/>
-    </row>
-    <row r="46" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="39"/>
       <c r="B46" s="38"/>
       <c r="C46" s="40"/>
@@ -12693,9 +12668,8 @@
       <c r="AW46" s="48"/>
       <c r="AX46" s="48"/>
       <c r="AY46" s="48"/>
-      <c r="AZ46" s="48"/>
-    </row>
-    <row r="47" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="35"/>
       <c r="B47" s="30"/>
       <c r="C47" s="30"/>
@@ -12746,9 +12720,8 @@
       <c r="AW47" s="48"/>
       <c r="AX47" s="48"/>
       <c r="AY47" s="48"/>
-      <c r="AZ47" s="48"/>
-    </row>
-    <row r="48" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="24"/>
       <c r="B48" s="24"/>
       <c r="C48" s="36"/>
@@ -12799,9 +12772,8 @@
       <c r="AW48" s="48"/>
       <c r="AX48" s="48"/>
       <c r="AY48" s="48"/>
-      <c r="AZ48" s="48"/>
-    </row>
-    <row r="49" spans="1:52" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:51" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="21"/>
       <c r="B49" s="21"/>
       <c r="C49" s="22"/>
@@ -12852,9 +12824,8 @@
       <c r="AW49" s="48"/>
       <c r="AX49" s="48"/>
       <c r="AY49" s="48"/>
-      <c r="AZ49" s="48"/>
-    </row>
-    <row r="50" spans="1:52" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="31"/>
       <c r="B50" s="24"/>
       <c r="C50" s="24"/>
@@ -12899,9 +12870,8 @@
       <c r="AW50" s="48"/>
       <c r="AX50" s="48"/>
       <c r="AY50" s="48"/>
-      <c r="AZ50" s="48"/>
-    </row>
-    <row r="51" spans="1:52" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A51" s="39"/>
       <c r="B51" s="38"/>
       <c r="C51" s="40"/>
@@ -12946,9 +12916,8 @@
       <c r="AW51" s="48"/>
       <c r="AX51" s="48"/>
       <c r="AY51" s="48"/>
-      <c r="AZ51" s="48"/>
-    </row>
-    <row r="52" spans="1:52" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A52" s="39"/>
       <c r="B52" s="38"/>
       <c r="C52" s="40"/>
@@ -12988,7 +12957,7 @@
       <c r="AM52" s="40"/>
       <c r="AN52" s="40"/>
     </row>
-    <row r="53" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A53" s="35"/>
       <c r="B53" s="30"/>
       <c r="C53" s="30"/>
@@ -13028,7 +12997,7 @@
       <c r="AM53" s="30"/>
       <c r="AN53" s="30"/>
     </row>
-    <row r="54" spans="1:52" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="24"/>
       <c r="B54" s="24"/>
       <c r="C54" s="36"/>
@@ -13068,7 +13037,7 @@
       <c r="AM54" s="36"/>
       <c r="AN54" s="36"/>
     </row>
-    <row r="55" spans="1:52" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="22"/>
@@ -13108,7 +13077,7 @@
       <c r="AM55" s="22"/>
       <c r="AN55" s="22"/>
     </row>
-    <row r="56" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A56" s="34"/>
       <c r="B56" s="30"/>
       <c r="C56" s="30"/>
@@ -13148,7 +13117,7 @@
       <c r="AM56" s="30"/>
       <c r="AN56" s="30"/>
     </row>
-    <row r="57" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A57" s="35"/>
       <c r="B57" s="38"/>
       <c r="C57" s="36"/>
@@ -13188,7 +13157,7 @@
       <c r="AM57" s="36"/>
       <c r="AN57" s="36"/>
     </row>
-    <row r="59" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:51" x14ac:dyDescent="0.2">
       <c r="X59" s="8"/>
       <c r="AE59" s="8"/>
       <c r="AF59" s="8"/>
@@ -13255,10 +13224,10 @@
         <v>8</v>
       </c>
       <c r="H5" s="93" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I5" s="92" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="J5" s="98"/>
       <c r="K5" s="98"/>
@@ -13877,7 +13846,7 @@
         <v>hoja.Cell("T" &amp; sep</v>
       </c>
       <c r="F1" s="183" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G1" s="180" t="str">
         <f>+A1&amp;C4</f>
@@ -13888,507 +13857,507 @@
       <c r="A2" s="189"/>
       <c r="B2" s="189"/>
       <c r="C2" s="185" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E2" s="182" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;" sep + 1"</f>
         <v>hoja.Cell("T" &amp;  sep + 1</v>
       </c>
       <c r="F2" s="183" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="180" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="180" t="str">
         <f>+B1</f>
         <v xml:space="preserve"> leon</v>
       </c>
       <c r="C3" s="185" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E3" s="182" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;"sep + 3"</f>
         <v>hoja.Cell("T" &amp; sep + 3</v>
       </c>
       <c r="F3" s="183" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E4" s="182" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;"sep + 4"</f>
         <v>hoja.Cell("T" &amp; sep + 4</v>
       </c>
       <c r="F4" s="183" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C5" s="184" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E5" s="182" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;"sep + 5"</f>
         <v>hoja.Cell("T" &amp; sep + 5</v>
       </c>
       <c r="F5" s="183" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C6" s="187" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E6" s="182" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;"sep + 6"</f>
         <v>hoja.Cell("T" &amp; sep + 6</v>
       </c>
       <c r="F6" s="183" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G6" s="180" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C7" s="187" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E7" s="181"/>
       <c r="F7" s="183"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C8" s="187" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E8" s="180" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;"sep + 7"</f>
         <v>hoja.Cell("T" &amp; sep + 7</v>
       </c>
       <c r="F8" s="183" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C9" s="187" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E9" s="180" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;"sep + 8"</f>
         <v>hoja.Cell("T" &amp; sep + 8</v>
       </c>
       <c r="F9" s="183" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C10" s="187" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E10" s="180" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C3&amp;C4&amp;C17&amp;"sep + 9"</f>
         <v>hoja.Cell("T" &amp; sep + 9</v>
       </c>
       <c r="F10" s="183" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C11" s="184" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C12" s="184" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" s="180" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C13" s="184" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C14" s="184" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E14" s="180" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C11</f>
         <v xml:space="preserve">hoja.Cell("V" &amp; sep +3 </v>
       </c>
       <c r="F14" s="180" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G14" s="180" t="str">
         <f>C5&amp;B1&amp;C6&amp;B1&amp;C7&amp;B1&amp;C8&amp;B1&amp;C9</f>
         <v>"=V" &amp; leon+1 &amp; " + X" &amp; leon+1 &amp; " + Z"&amp; leon+1 &amp; "+AB" &amp; leon+1</v>
       </c>
       <c r="H14" s="180" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B15" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C15" s="184" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E15" s="180" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C12</f>
         <v>hoja.Cell("V" &amp; sep +4</v>
       </c>
       <c r="F15" s="180" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G15" s="180" t="str">
         <f>+C10&amp;C2&amp;C4&amp;C11&amp;C15</f>
         <v>"=V" &amp; sep +3  &amp; "*16%"</v>
       </c>
       <c r="H15" s="180" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C16" s="184" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E16" s="180" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C13</f>
         <v>hoja.Cell("V" &amp; sep +5</v>
       </c>
       <c r="F16" s="180" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G16" s="180" t="str">
         <f>+C10&amp;C2&amp;C4&amp;C11&amp;C16</f>
         <v>"=V" &amp; sep +3  &amp;" *6%"</v>
       </c>
       <c r="H16" s="180" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C17" s="184" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E17" s="180" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C14</f>
         <v xml:space="preserve">hoja.Cell("V" &amp; sep +6 </v>
       </c>
       <c r="F17" s="180" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G17" s="180" t="str">
         <f>+C10&amp;C2&amp;C4&amp;C11&amp;C17&amp;C4&amp;C18&amp;C2&amp;C4&amp;C12&amp;C17&amp;C4&amp;C19&amp;C2&amp;C4&amp;C13</f>
         <v>"=V" &amp; sep +3  &amp; "+V" &amp; sep +4 &amp; "-V" &amp; sep +5</v>
       </c>
       <c r="H17" s="180" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C18" s="184" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F18" s="180"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C19" s="184" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E19" s="180" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C23</f>
         <v>hoja.Cell("V" &amp; sep +7</v>
       </c>
       <c r="F19" s="180" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G19" s="180" t="str">
         <f>+C20&amp;B1&amp;C21&amp;B1&amp;C22&amp;B1&amp;C9</f>
         <v>"=W" &amp; leon+1 &amp; "+AA" &amp; leon+1 &amp; "+Q" &amp; leon+1</v>
       </c>
       <c r="H19" s="180" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C20" s="184" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E20" s="180" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C24</f>
         <v>hoja.Cell("V" &amp; sep +8</v>
       </c>
       <c r="F20" s="180" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G20" s="180" t="str">
         <f>+C10&amp;C2&amp;C4&amp;C23&amp;C15</f>
         <v>"=V" &amp; sep +7 &amp; "*16%"</v>
       </c>
       <c r="H20" s="180" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C21" s="187" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E21" s="180" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C25</f>
         <v>hoja.Cell("V" &amp; sep +9</v>
       </c>
       <c r="F21" s="180" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G21" s="180" t="str">
         <f>+C10&amp;C2&amp;C4&amp;C23&amp;C17&amp;C4&amp;C18&amp;C2&amp;C4&amp;C24</f>
         <v>"=V" &amp; sep +7 &amp; "+V" &amp; sep +8</v>
       </c>
       <c r="H21" s="180" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C22" s="187" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F22" s="180"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C23" s="184" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E23" s="180" t="str">
         <f>+"hoja.Cell("&amp;C4&amp;C2&amp;C4&amp;C26</f>
         <v>hoja.Cell("V" &amp; sep +10</v>
       </c>
       <c r="F23" s="180" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G23" s="180" t="str">
         <f>+C10&amp;C2&amp;C4&amp;C14&amp;C17&amp;C4&amp;C18&amp;C2&amp;C4&amp;C25</f>
         <v>"=V" &amp; sep +6  &amp; "+V" &amp; sep +9</v>
       </c>
       <c r="H23" s="180" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B24" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C24" s="184" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="180" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B25" s="180" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C25" s="184" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="180" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B26" s="180" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C26" s="184" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="180" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B27" s="180" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="180" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B28" s="180" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C28" s="184" t="s">
-        <v>180</v>
-      </c>
-      <c r="E28" s="218" t="str">
+        <v>177</v>
+      </c>
+      <c r="E28" s="219" t="str">
         <f>+C28&amp;C4&amp;C3&amp;C4&amp;C25&amp;","&amp;C4&amp;C2&amp;C4&amp;C25&amp;")"</f>
         <v>hoja.Range("T" &amp; sep +9,"V" &amp; sep +9)</v>
       </c>
-      <c r="F28" s="218"/>
+      <c r="F28" s="219"/>
       <c r="G28" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C29" s="184" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E29" t="str">
         <f>+C28&amp;C4&amp;C3&amp;C4&amp;C14&amp;","&amp;C4&amp;C2&amp;C4&amp;C14&amp;")"</f>
         <v>hoja.Range("T" &amp; sep +6 ,"V" &amp; sep +6 )</v>
       </c>
       <c r="G29" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -14397,7 +14366,7 @@
         <v>hoja.Cell("T" &amp; sep)</v>
       </c>
       <c r="F30" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -14413,8 +14382,8 @@
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14458,49 +14427,49 @@
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="132"/>
       <c r="B3" s="135" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="219"/>
-      <c r="D3" s="220"/>
+        <v>67</v>
+      </c>
+      <c r="C3" s="220"/>
+      <c r="D3" s="221"/>
       <c r="E3" s="136"/>
       <c r="F3" s="135" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G3" s="137"/>
-      <c r="H3" s="219"/>
-      <c r="I3" s="220"/>
+      <c r="H3" s="220"/>
+      <c r="I3" s="221"/>
       <c r="J3" s="152"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="132"/>
       <c r="B4" s="138" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="139" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="139" t="s">
+      <c r="D4" s="139" t="s">
         <v>70</v>
-      </c>
-      <c r="D4" s="139" t="s">
-        <v>71</v>
       </c>
       <c r="E4" s="140"/>
       <c r="F4" s="138" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="141" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="139" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="141" t="s">
-        <v>90</v>
-      </c>
-      <c r="H4" s="139" t="s">
+      <c r="I4" s="139" t="s">
         <v>70</v>
-      </c>
-      <c r="I4" s="139" t="s">
-        <v>71</v>
       </c>
       <c r="J4" s="152"/>
     </row>
     <row r="5" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="132"/>
       <c r="B5" s="142" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C5" s="143"/>
       <c r="D5" s="143"/>
@@ -14517,7 +14486,7 @@
     <row r="6" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="132"/>
       <c r="B6" s="145" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="146">
         <f>0</f>
@@ -14526,7 +14495,7 @@
       <c r="D6" s="146"/>
       <c r="E6" s="133"/>
       <c r="F6" s="145" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6" s="147"/>
       <c r="H6" s="146"/>
@@ -14536,7 +14505,7 @@
     <row r="7" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="132"/>
       <c r="B7" s="145" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="146">
         <f>0</f>
@@ -14545,7 +14514,7 @@
       <c r="D7" s="146"/>
       <c r="E7" s="148"/>
       <c r="F7" s="145" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" s="147"/>
       <c r="H7" s="146"/>
@@ -14555,7 +14524,7 @@
     <row r="8" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="132"/>
       <c r="B8" s="145" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" s="146">
         <f>0</f>
@@ -14564,7 +14533,7 @@
       <c r="D8" s="146"/>
       <c r="E8" s="149"/>
       <c r="F8" s="145" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G8" s="147"/>
       <c r="H8" s="146"/>
@@ -14574,7 +14543,7 @@
     <row r="9" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="132"/>
       <c r="B9" s="145" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C9" s="146">
         <f>0</f>
@@ -14583,7 +14552,7 @@
       <c r="D9" s="146"/>
       <c r="E9" s="150"/>
       <c r="F9" s="145" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G9" s="147"/>
       <c r="H9" s="146"/>
@@ -14593,7 +14562,7 @@
     <row r="10" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="132"/>
       <c r="B10" s="145" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" s="146">
         <f>0</f>
@@ -14602,7 +14571,7 @@
       <c r="D10" s="146"/>
       <c r="E10" s="148"/>
       <c r="F10" s="145" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G10" s="147"/>
       <c r="H10" s="146"/>
@@ -14612,7 +14581,7 @@
     <row r="11" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="132"/>
       <c r="B11" s="145" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" s="146">
         <f>0</f>
@@ -14621,7 +14590,7 @@
       <c r="D11" s="146"/>
       <c r="E11" s="148"/>
       <c r="F11" s="145" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G11" s="147"/>
       <c r="H11" s="146"/>
@@ -14631,7 +14600,7 @@
     <row r="12" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="132"/>
       <c r="B12" s="145" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="146">
         <f>0</f>
@@ -14640,7 +14609,7 @@
       <c r="D12" s="146"/>
       <c r="E12" s="149"/>
       <c r="F12" s="145" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G12" s="147"/>
       <c r="H12" s="146"/>
@@ -14650,7 +14619,7 @@
     <row r="13" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="132"/>
       <c r="B13" s="145" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" s="146">
         <f>0</f>
@@ -14659,7 +14628,7 @@
       <c r="D13" s="146"/>
       <c r="E13" s="149"/>
       <c r="F13" s="145" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G13" s="147"/>
       <c r="H13" s="146"/>
@@ -14669,7 +14638,7 @@
     <row r="14" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="132"/>
       <c r="B14" s="145" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="149">
         <f>0</f>
@@ -14678,7 +14647,7 @@
       <c r="D14" s="146"/>
       <c r="E14" s="150"/>
       <c r="F14" s="145" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G14" s="147"/>
       <c r="H14" s="146"/>
@@ -14688,7 +14657,7 @@
     <row r="15" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="132"/>
       <c r="B15" s="151" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="146">
         <f>0</f>
@@ -14697,7 +14666,7 @@
       <c r="D15" s="146"/>
       <c r="E15" s="152"/>
       <c r="F15" s="151" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G15" s="147"/>
       <c r="H15" s="146"/>
@@ -14707,7 +14676,7 @@
     <row r="16" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="132"/>
       <c r="B16" s="153" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" s="149">
         <f>0</f>
@@ -14716,7 +14685,7 @@
       <c r="D16" s="154"/>
       <c r="E16" s="152"/>
       <c r="F16" s="153" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G16" s="147"/>
       <c r="H16" s="146"/>
@@ -14726,7 +14695,7 @@
     <row r="17" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="132"/>
       <c r="B17" s="145" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C17" s="146">
         <f>0</f>
@@ -14735,7 +14704,7 @@
       <c r="D17" s="146"/>
       <c r="E17" s="152"/>
       <c r="F17" s="145" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G17" s="147"/>
       <c r="H17" s="146"/>
@@ -14745,7 +14714,7 @@
     <row r="18" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="132"/>
       <c r="B18" s="145" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C18" s="146">
         <f>0</f>
@@ -14754,7 +14723,7 @@
       <c r="D18" s="146"/>
       <c r="E18" s="152"/>
       <c r="F18" s="145" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G18" s="147"/>
       <c r="H18" s="146"/>
@@ -14764,7 +14733,7 @@
     <row r="19" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="132"/>
       <c r="B19" s="145" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" s="146">
         <f>0</f>
@@ -14773,7 +14742,7 @@
       <c r="D19" s="146"/>
       <c r="E19" s="152"/>
       <c r="F19" s="145" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G19" s="147"/>
       <c r="H19" s="146"/>
@@ -14783,7 +14752,7 @@
     <row r="20" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="132"/>
       <c r="B20" s="145" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C20" s="146">
         <f>0</f>
@@ -14792,7 +14761,7 @@
       <c r="D20" s="146"/>
       <c r="E20" s="152"/>
       <c r="F20" s="145" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G20" s="147"/>
       <c r="H20" s="146"/>
@@ -14802,7 +14771,7 @@
     <row r="21" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="132"/>
       <c r="B21" s="145" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" s="146">
         <f>0</f>
@@ -14811,7 +14780,7 @@
       <c r="D21" s="146"/>
       <c r="E21" s="152"/>
       <c r="F21" s="145" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G21" s="147"/>
       <c r="H21" s="144"/>
@@ -14821,7 +14790,7 @@
     <row r="22" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="132"/>
       <c r="B22" s="145" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" s="146">
         <f>0</f>
@@ -14830,7 +14799,7 @@
       <c r="D22" s="146"/>
       <c r="E22" s="152"/>
       <c r="F22" s="145" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G22" s="147"/>
       <c r="H22" s="144"/>
@@ -14840,7 +14809,7 @@
     <row r="23" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="132"/>
       <c r="B23" s="153" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="154">
         <f>0</f>
@@ -14849,7 +14818,7 @@
       <c r="D23" s="146"/>
       <c r="E23" s="152"/>
       <c r="F23" s="153" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G23" s="147"/>
       <c r="H23" s="144"/>
@@ -14859,7 +14828,7 @@
     <row r="24" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="132"/>
       <c r="B24" s="153" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C24" s="154"/>
       <c r="D24" s="146">
@@ -14868,7 +14837,7 @@
       </c>
       <c r="E24" s="152"/>
       <c r="F24" s="153" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G24" s="147"/>
       <c r="H24" s="144"/>
@@ -14878,13 +14847,13 @@
     <row r="25" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="132"/>
       <c r="B25" s="155" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C25" s="155"/>
       <c r="D25" s="146"/>
       <c r="E25" s="152"/>
       <c r="F25" s="155" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G25" s="147"/>
       <c r="H25" s="191"/>
@@ -14894,13 +14863,13 @@
     <row r="26" spans="1:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="132"/>
       <c r="B26" s="155" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C26" s="155"/>
       <c r="D26" s="146"/>
       <c r="E26" s="152"/>
       <c r="F26" s="155" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G26" s="147"/>
       <c r="H26" s="191"/>
@@ -14910,7 +14879,7 @@
     <row r="27" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="132"/>
       <c r="B27" s="155" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C27" s="155"/>
       <c r="D27" s="146">
@@ -14919,7 +14888,7 @@
       </c>
       <c r="E27" s="152"/>
       <c r="F27" s="155" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G27" s="147"/>
       <c r="H27" s="191"/>
@@ -14929,7 +14898,7 @@
     <row r="28" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="132"/>
       <c r="B28" s="190" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C28" s="190"/>
       <c r="D28" s="154">
@@ -14938,17 +14907,17 @@
       </c>
       <c r="E28" s="152"/>
       <c r="F28" s="190" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G28" s="192"/>
       <c r="H28" s="191"/>
       <c r="I28" s="154"/>
       <c r="J28" s="152"/>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="132"/>
       <c r="B29" s="155" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C29" s="155"/>
       <c r="D29" s="146">
@@ -14957,7 +14926,7 @@
       </c>
       <c r="E29" s="152"/>
       <c r="F29" s="155" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G29" s="192"/>
       <c r="H29" s="191"/>
@@ -14967,7 +14936,7 @@
     <row r="30" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="132"/>
       <c r="B30" s="190" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C30" s="190"/>
       <c r="D30" s="154">
@@ -14975,7 +14944,7 @@
       </c>
       <c r="E30" s="152"/>
       <c r="F30" s="190" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G30" s="192"/>
       <c r="H30" s="191"/>
@@ -14985,7 +14954,7 @@
     <row r="31" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="132"/>
       <c r="B31" s="190" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C31" s="190"/>
       <c r="D31" s="154">
@@ -14993,23 +14962,23 @@
       </c>
       <c r="E31" s="152"/>
       <c r="F31" s="190" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G31" s="190"/>
       <c r="H31" s="154"/>
       <c r="I31" s="154"/>
       <c r="J31" s="152"/>
     </row>
-    <row r="32" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="132"/>
       <c r="B32" s="190" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C32" s="190"/>
       <c r="D32" s="154"/>
       <c r="E32" s="152"/>
       <c r="F32" s="190" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G32" s="190"/>
       <c r="H32" s="154"/>
@@ -15019,13 +14988,13 @@
     <row r="33" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="132"/>
       <c r="B33" s="190" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C33" s="190"/>
       <c r="D33" s="154"/>
       <c r="E33" s="152"/>
       <c r="F33" s="190" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G33" s="190"/>
       <c r="H33" s="154"/>
@@ -15035,7 +15004,7 @@
     <row r="34" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="132"/>
       <c r="B34" s="206" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C34" s="206"/>
       <c r="D34" s="207"/>
@@ -15080,7 +15049,7 @@
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="132"/>
       <c r="B36" s="158" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C36" s="146">
         <f>C35*16%</f>
@@ -15092,7 +15061,7 @@
       </c>
       <c r="E36" s="152"/>
       <c r="F36" s="158" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="146">
@@ -15108,7 +15077,7 @@
     <row r="37" spans="1:10" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="132"/>
       <c r="B37" s="158" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C37" s="146">
         <v>0</v>
@@ -15118,7 +15087,7 @@
       </c>
       <c r="E37" s="152"/>
       <c r="F37" s="158" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G37" s="164">
         <f>SUM(G6:G36)</f>
@@ -15167,7 +15136,7 @@
     <row r="39" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="132"/>
       <c r="B39" s="142" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C39" s="144"/>
       <c r="D39" s="144"/>
@@ -15184,7 +15153,7 @@
     <row r="40" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="132"/>
       <c r="B40" s="145" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" s="144">
         <f>0</f>
@@ -15193,7 +15162,7 @@
       <c r="D40" s="144"/>
       <c r="E40" s="152"/>
       <c r="F40" s="145" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G40" s="147"/>
       <c r="H40" s="146"/>
@@ -15203,7 +15172,7 @@
     <row r="41" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="132"/>
       <c r="B41" s="145" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="146">
         <f>0</f>
@@ -15212,7 +15181,7 @@
       <c r="D41" s="143"/>
       <c r="E41" s="152"/>
       <c r="F41" s="145" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G41" s="147"/>
       <c r="H41" s="146"/>
@@ -15222,7 +15191,7 @@
     <row r="42" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="132"/>
       <c r="B42" s="145" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C42" s="146">
         <f>0</f>
@@ -15231,7 +15200,7 @@
       <c r="D42" s="143"/>
       <c r="E42" s="152"/>
       <c r="F42" s="145" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G42" s="147"/>
       <c r="H42" s="146"/>
@@ -15241,7 +15210,7 @@
     <row r="43" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="152"/>
       <c r="B43" s="145" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C43" s="146">
         <f>0</f>
@@ -15250,7 +15219,7 @@
       <c r="D43" s="143"/>
       <c r="E43" s="152"/>
       <c r="F43" s="145" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G43" s="147"/>
       <c r="H43" s="146"/>
@@ -15260,7 +15229,7 @@
     <row r="44" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="152"/>
       <c r="B44" s="145" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C44" s="146">
         <f>0</f>
@@ -15269,7 +15238,7 @@
       <c r="D44" s="143"/>
       <c r="E44" s="152"/>
       <c r="F44" s="145" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G44" s="147"/>
       <c r="H44" s="146"/>
@@ -15279,7 +15248,7 @@
     <row r="45" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="152"/>
       <c r="B45" s="145" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C45" s="146">
         <f>0</f>
@@ -15288,7 +15257,7 @@
       <c r="D45" s="143"/>
       <c r="E45" s="152"/>
       <c r="F45" s="145" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G45" s="147"/>
       <c r="H45" s="146"/>
@@ -15298,7 +15267,7 @@
     <row r="46" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="152"/>
       <c r="B46" s="145" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C46" s="146">
         <f>0</f>
@@ -15307,7 +15276,7 @@
       <c r="D46" s="143"/>
       <c r="E46" s="152"/>
       <c r="F46" s="145" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G46" s="147"/>
       <c r="H46" s="146"/>
@@ -15317,7 +15286,7 @@
     <row r="47" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="152"/>
       <c r="B47" s="145" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C47" s="146">
         <f>0</f>
@@ -15326,7 +15295,7 @@
       <c r="D47" s="143"/>
       <c r="E47" s="152"/>
       <c r="F47" s="145" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G47" s="147"/>
       <c r="H47" s="146"/>
@@ -15336,7 +15305,7 @@
     <row r="48" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="152"/>
       <c r="B48" s="145" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C48" s="146">
         <f>0</f>
@@ -15345,7 +15314,7 @@
       <c r="D48" s="146"/>
       <c r="E48" s="152"/>
       <c r="F48" s="145" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G48" s="147"/>
       <c r="H48" s="146"/>
@@ -15355,7 +15324,7 @@
     <row r="49" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="152"/>
       <c r="B49" s="151" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" s="146">
         <f>0</f>
@@ -15364,7 +15333,7 @@
       <c r="D49" s="143"/>
       <c r="E49" s="152"/>
       <c r="F49" s="151" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G49" s="147"/>
       <c r="H49" s="146"/>
@@ -15374,7 +15343,7 @@
     <row r="50" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="152"/>
       <c r="B50" s="153" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C50" s="146">
         <f>0</f>
@@ -15383,7 +15352,7 @@
       <c r="D50" s="143"/>
       <c r="E50" s="152"/>
       <c r="F50" s="153" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G50" s="147"/>
       <c r="H50" s="146"/>
@@ -15393,7 +15362,7 @@
     <row r="51" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="152"/>
       <c r="B51" s="145" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C51" s="154">
         <f>0</f>
@@ -15402,7 +15371,7 @@
       <c r="D51" s="165"/>
       <c r="E51" s="152"/>
       <c r="F51" s="145" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G51" s="147"/>
       <c r="H51" s="146"/>
@@ -15412,7 +15381,7 @@
     <row r="52" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="152"/>
       <c r="B52" s="145" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C52" s="146">
         <f>0</f>
@@ -15421,7 +15390,7 @@
       <c r="D52" s="146"/>
       <c r="E52" s="152"/>
       <c r="F52" s="145" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G52" s="147"/>
       <c r="H52" s="146"/>
@@ -15431,7 +15400,7 @@
     <row r="53" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="152"/>
       <c r="B53" s="145" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C53" s="154">
         <f>0</f>
@@ -15440,7 +15409,7 @@
       <c r="D53" s="165"/>
       <c r="E53" s="152"/>
       <c r="F53" s="145" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G53" s="147"/>
       <c r="H53" s="146"/>
@@ -15449,7 +15418,7 @@
     </row>
     <row r="54" spans="1:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="145" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C54" s="154">
         <f>0</f>
@@ -15457,7 +15426,7 @@
       </c>
       <c r="D54" s="165"/>
       <c r="F54" s="145" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G54" s="147"/>
       <c r="H54" s="144"/>
@@ -15465,7 +15434,7 @@
     </row>
     <row r="55" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="145" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C55" s="154">
         <f>0</f>
@@ -15473,7 +15442,7 @@
       </c>
       <c r="D55" s="165"/>
       <c r="F55" s="145" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G55" s="147"/>
       <c r="H55" s="144"/>
@@ -15481,7 +15450,7 @@
     </row>
     <row r="56" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="145" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C56" s="154">
         <f>0</f>
@@ -15489,7 +15458,7 @@
       </c>
       <c r="D56" s="165"/>
       <c r="F56" s="145" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G56" s="147"/>
       <c r="H56" s="144"/>
@@ -15497,7 +15466,7 @@
     </row>
     <row r="57" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="153" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C57" s="154">
         <f>0</f>
@@ -15505,7 +15474,7 @@
       </c>
       <c r="D57" s="154"/>
       <c r="F57" s="153" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G57" s="147"/>
       <c r="H57" s="144"/>
@@ -15513,7 +15482,7 @@
     </row>
     <row r="58" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="153" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C58" s="153"/>
       <c r="D58" s="154">
@@ -15521,7 +15490,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="153" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G58" s="192"/>
       <c r="H58" s="191"/>
@@ -15529,12 +15498,12 @@
     </row>
     <row r="59" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="155" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C59" s="155"/>
       <c r="D59" s="154"/>
       <c r="F59" s="155" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G59" s="147"/>
       <c r="H59" s="144"/>
@@ -15542,12 +15511,12 @@
     </row>
     <row r="60" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="155" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C60" s="155"/>
       <c r="D60" s="154"/>
       <c r="F60" s="155" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G60" s="192"/>
       <c r="H60" s="191"/>
@@ -15555,7 +15524,7 @@
     </row>
     <row r="61" spans="1:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="155" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C61" s="155"/>
       <c r="D61" s="154">
@@ -15563,7 +15532,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="155" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G61" s="192"/>
       <c r="H61" s="191"/>
@@ -15587,7 +15556,7 @@
       <c r="H62" s="191"/>
       <c r="I62" s="154"/>
     </row>
-    <row r="63" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="190" t="str">
         <f>+B29</f>
         <v>PROYECTO MAERSK</v>
@@ -15607,14 +15576,14 @@
     </row>
     <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="155" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C64" s="147"/>
       <c r="D64" s="191">
         <v>0</v>
       </c>
       <c r="F64" s="155" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G64" s="192"/>
       <c r="H64" s="191"/>
@@ -15622,20 +15591,20 @@
     </row>
     <row r="65" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="190" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C65" s="190"/>
       <c r="D65" s="154">
         <v>0</v>
       </c>
       <c r="F65" s="190" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G65" s="190"/>
       <c r="H65" s="154"/>
       <c r="I65" s="154"/>
     </row>
-    <row r="66" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="190" t="str">
         <f>+B32</f>
         <v>GANNET</v>
@@ -15643,7 +15612,7 @@
       <c r="C66" s="190"/>
       <c r="D66" s="154"/>
       <c r="F66" s="190" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G66" s="190"/>
       <c r="H66" s="154"/>
@@ -15651,12 +15620,12 @@
     </row>
     <row r="67" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="190" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C67" s="190"/>
       <c r="D67" s="154"/>
       <c r="F67" s="190" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G67" s="190"/>
       <c r="H67" s="154"/>
@@ -15665,13 +15634,13 @@
     <row r="68" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="132"/>
       <c r="B68" s="206" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C68" s="206"/>
       <c r="D68" s="207"/>
       <c r="E68" s="152"/>
       <c r="F68" s="206" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G68" s="206"/>
       <c r="H68" s="207"/>
@@ -15705,7 +15674,7 @@
     </row>
     <row r="70" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B70" s="158" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C70" s="146">
         <f>C69*16%</f>
@@ -15716,7 +15685,7 @@
         <v>0</v>
       </c>
       <c r="F70" s="158" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G70" s="163"/>
       <c r="H70" s="146">
@@ -15800,8 +15769,8 @@
   <sheetPr codeName="Hoja7"/>
   <dimension ref="B1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15810,22 +15779,25 @@
     <col min="2" max="2" width="37" style="166" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" style="166" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="166" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="34" style="166" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="166" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" style="166" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" style="166" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="166"/>
+    <col min="5" max="5" width="22.140625" style="166" customWidth="1"/>
+    <col min="6" max="6" width="18" style="166" customWidth="1"/>
+    <col min="7" max="7" width="34" style="166" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="166" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="166" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="166" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="25" style="166" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="166"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="170" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C1" s="170" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D1" s="172" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E1" s="172" t="s">
         <v>7</v>
@@ -15837,19 +15809,20 @@
         <v>13</v>
       </c>
       <c r="H1" s="170" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="170" t="s">
         <v>102</v>
-      </c>
-      <c r="I1" s="170" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" s="170" t="s">
-        <v>104</v>
       </c>
       <c r="K1" s="170" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="209"/>
       <c r="I2" s="167"/>
       <c r="K2" s="171">
         <f>I2+J2</f>
@@ -15857,93 +15830,115 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H3" s="209"/>
       <c r="I3" s="167"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H4" s="209"/>
       <c r="I4" s="167"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H5" s="209"/>
       <c r="I5" s="167"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H6" s="209"/>
       <c r="I6" s="168"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H7" s="209"/>
       <c r="I7" s="167"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H8" s="209"/>
       <c r="I8" s="167"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H9" s="209"/>
       <c r="I9" s="167"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H10" s="209"/>
       <c r="I10" s="168"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H11" s="209"/>
       <c r="I11" s="167"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H12" s="209"/>
       <c r="I12" s="167"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H13" s="209"/>
       <c r="I13" s="167"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H14" s="209"/>
       <c r="I14" s="168"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H15" s="209"/>
       <c r="I15" s="167"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H16" s="209"/>
       <c r="I16" s="167"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="209"/>
       <c r="I17" s="167"/>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="209"/>
       <c r="I18" s="167"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="209"/>
       <c r="I19" s="167"/>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="209"/>
       <c r="I20" s="168"/>
     </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H21" s="209"/>
       <c r="I21" s="167"/>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="209"/>
       <c r="I22" s="167"/>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="209"/>
       <c r="I23" s="167"/>
     </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H24" s="209"/>
       <c r="I24" s="168"/>
     </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
       <c r="I25" s="167"/>
     </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
       <c r="I26" s="167"/>
     </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
       <c r="I27" s="167"/>
     </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
       <c r="I28" s="168"/>
     </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
       <c r="I29" s="167"/>
     </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
       <c r="I30" s="167"/>
     </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
       <c r="I31" s="167"/>
     </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
       <c r="I32" s="168"/>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.25">
@@ -15986,19 +15981,19 @@
         <v>6</v>
       </c>
       <c r="C1" s="179" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="179" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="179" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="179" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="179" t="s">
+      <c r="G1" s="179" t="s">
         <v>106</v>
-      </c>
-      <c r="E1" s="179" t="s">
-        <v>110</v>
-      </c>
-      <c r="F1" s="179" t="s">
-        <v>111</v>
-      </c>
-      <c r="G1" s="179" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
@@ -16036,19 +16031,19 @@
         <v>6</v>
       </c>
       <c r="C1" s="179" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="179" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="179" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="179" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="179" t="s">
+      <c r="G1" s="179" t="s">
         <v>106</v>
-      </c>
-      <c r="E1" s="179" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" s="179" t="s">
-        <v>111</v>
-      </c>
-      <c r="G1" s="179" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lote de timbrado correcto xd
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="633"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="633" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NOMINA TOTAL" sheetId="27" r:id="rId1"/>
@@ -3467,17 +3467,20 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="33" fillId="0" borderId="0" xfId="1491" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1113" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3498,9 +3501,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1492">
@@ -5725,7 +5725,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="B1:BK15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="W13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A11" sqref="A11"/>
       <selection pane="topRight" activeCell="F11" sqref="F11"/>
@@ -6407,90 +6407,90 @@
       <c r="BK10" s="50"/>
     </row>
     <row r="11" spans="2:63" s="84" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="210" t="s">
+      <c r="B11" s="211" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="210" t="s">
+      <c r="C11" s="211" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="210" t="s">
+      <c r="D11" s="211" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="210" t="s">
+      <c r="E11" s="211" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="210" t="s">
+      <c r="F11" s="211" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="210" t="s">
+      <c r="G11" s="211" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="210" t="s">
+      <c r="H11" s="211" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="210" t="s">
+      <c r="I11" s="211" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="210" t="s">
+      <c r="J11" s="211" t="s">
         <v>54</v>
       </c>
-      <c r="K11" s="210" t="s">
+      <c r="K11" s="211" t="s">
         <v>53</v>
       </c>
-      <c r="L11" s="210" t="s">
+      <c r="L11" s="211" t="s">
         <v>4</v>
       </c>
-      <c r="M11" s="210" t="s">
+      <c r="M11" s="211" t="s">
         <v>56</v>
       </c>
-      <c r="N11" s="212" t="s">
+      <c r="N11" s="214" t="s">
         <v>262</v>
       </c>
-      <c r="O11" s="212" t="s">
+      <c r="O11" s="214" t="s">
         <v>206</v>
       </c>
-      <c r="P11" s="210" t="s">
+      <c r="P11" s="211" t="s">
         <v>66</v>
       </c>
       <c r="Q11" s="128"/>
-      <c r="R11" s="210" t="s">
+      <c r="R11" s="211" t="s">
         <v>47</v>
       </c>
       <c r="S11" s="131"/>
       <c r="T11" s="131"/>
-      <c r="U11" s="210" t="s">
+      <c r="U11" s="211" t="s">
         <v>52</v>
       </c>
-      <c r="V11" s="210" t="s">
+      <c r="V11" s="211" t="s">
         <v>191</v>
       </c>
-      <c r="W11" s="211" t="s">
+      <c r="W11" s="212" t="s">
         <v>194</v>
       </c>
       <c r="X11" s="197"/>
-      <c r="Y11" s="210" t="s">
+      <c r="Y11" s="211" t="s">
         <v>264</v>
       </c>
       <c r="Z11" s="85"/>
-      <c r="AA11" s="210" t="s">
+      <c r="AA11" s="211" t="s">
         <v>263</v>
       </c>
-      <c r="AB11" s="211" t="s">
+      <c r="AB11" s="212" t="s">
         <v>196</v>
       </c>
-      <c r="AC11" s="210" t="s">
+      <c r="AC11" s="211" t="s">
         <v>5</v>
       </c>
-      <c r="AD11" s="210" t="s">
+      <c r="AD11" s="211" t="s">
         <v>0</v>
       </c>
       <c r="AE11" s="213" t="s">
         <v>18</v>
       </c>
-      <c r="AF11" s="210" t="s">
+      <c r="AF11" s="211" t="s">
         <v>110</v>
       </c>
-      <c r="AG11" s="210" t="s">
+      <c r="AG11" s="211" t="s">
         <v>1</v>
       </c>
       <c r="AH11"/>
@@ -6523,25 +6523,25 @@
       <c r="BJ11" s="83"/>
     </row>
     <row r="12" spans="2:63" s="86" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="210"/>
-      <c r="C12" s="210"/>
-      <c r="D12" s="210"/>
-      <c r="E12" s="210"/>
-      <c r="F12" s="210"/>
-      <c r="G12" s="210"/>
-      <c r="H12" s="210"/>
-      <c r="I12" s="210"/>
-      <c r="J12" s="210"/>
-      <c r="K12" s="210"/>
-      <c r="L12" s="210"/>
-      <c r="M12" s="210"/>
-      <c r="N12" s="212"/>
-      <c r="O12" s="212"/>
-      <c r="P12" s="210"/>
+      <c r="B12" s="211"/>
+      <c r="C12" s="211"/>
+      <c r="D12" s="211"/>
+      <c r="E12" s="211"/>
+      <c r="F12" s="211"/>
+      <c r="G12" s="211"/>
+      <c r="H12" s="211"/>
+      <c r="I12" s="211"/>
+      <c r="J12" s="211"/>
+      <c r="K12" s="211"/>
+      <c r="L12" s="211"/>
+      <c r="M12" s="211"/>
+      <c r="N12" s="214"/>
+      <c r="O12" s="214"/>
+      <c r="P12" s="211"/>
       <c r="Q12" s="128" t="s">
         <v>202</v>
       </c>
-      <c r="R12" s="210" t="s">
+      <c r="R12" s="211" t="s">
         <v>57</v>
       </c>
       <c r="S12" s="131" t="s">
@@ -6550,21 +6550,21 @@
       <c r="T12" s="131" t="s">
         <v>97</v>
       </c>
-      <c r="U12" s="210"/>
-      <c r="V12" s="210"/>
-      <c r="W12" s="211"/>
+      <c r="U12" s="211"/>
+      <c r="V12" s="211"/>
+      <c r="W12" s="212"/>
       <c r="X12" s="197" t="s">
         <v>195</v>
       </c>
-      <c r="Y12" s="210"/>
+      <c r="Y12" s="211"/>
       <c r="Z12" s="85"/>
-      <c r="AA12" s="210"/>
-      <c r="AB12" s="211"/>
-      <c r="AC12" s="210"/>
-      <c r="AD12" s="210"/>
+      <c r="AA12" s="211"/>
+      <c r="AB12" s="212"/>
+      <c r="AC12" s="211"/>
+      <c r="AD12" s="211"/>
       <c r="AE12" s="213"/>
-      <c r="AF12" s="210"/>
-      <c r="AG12" s="210"/>
+      <c r="AF12" s="211"/>
+      <c r="AG12" s="211"/>
       <c r="AH12"/>
       <c r="AI12" s="87"/>
       <c r="AJ12" s="88"/>
@@ -6695,13 +6695,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="AA11:AA12"/>
-    <mergeCell ref="AC11:AC12"/>
-    <mergeCell ref="AB11:AB12"/>
-    <mergeCell ref="AF11:AF12"/>
-    <mergeCell ref="AG11:AG12"/>
-    <mergeCell ref="AD11:AD12"/>
-    <mergeCell ref="AE11:AE12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="M11:M12"/>
     <mergeCell ref="Y11:Y12"/>
@@ -6717,11 +6715,13 @@
     <mergeCell ref="V11:V12"/>
     <mergeCell ref="N11:N12"/>
     <mergeCell ref="O11:O12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="AA11:AA12"/>
+    <mergeCell ref="AC11:AC12"/>
+    <mergeCell ref="AB11:AB12"/>
+    <mergeCell ref="AF11:AF12"/>
+    <mergeCell ref="AG11:AG12"/>
+    <mergeCell ref="AD11:AD12"/>
+    <mergeCell ref="AE11:AE12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6732,11 +6732,11 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:KJ51"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="10" ySplit="8" topLeftCell="BE9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <pane xSplit="10" ySplit="8" topLeftCell="K9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="BF1" sqref="BF1"/>
+      <selection pane="bottomRight" activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6748,7 +6748,7 @@
     <col min="5" max="5" width="12.85546875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="72" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" style="72" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
     <col min="9" max="9" width="36.28515625" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
@@ -6781,13 +6781,13 @@
   <sheetData>
     <row r="1" spans="1:296" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="27"/>
-      <c r="B1" s="214" t="s">
+      <c r="B1" s="215" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="215"/>
-      <c r="D1" s="215"/>
-      <c r="E1" s="215"/>
-      <c r="F1" s="215"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
       <c r="G1" s="64"/>
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
@@ -6889,13 +6889,13 @@
     </row>
     <row r="3" spans="1:296" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
-      <c r="B3" s="216" t="s">
+      <c r="B3" s="217" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="215"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="215"/>
-      <c r="F3" s="215"/>
+      <c r="C3" s="216"/>
+      <c r="D3" s="216"/>
+      <c r="E3" s="216"/>
+      <c r="F3" s="216"/>
       <c r="G3" s="66"/>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
@@ -6949,13 +6949,13 @@
     </row>
     <row r="4" spans="1:296" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
-      <c r="B4" s="217" t="s">
+      <c r="B4" s="218" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="218"/>
-      <c r="D4" s="218"/>
-      <c r="E4" s="218"/>
-      <c r="F4" s="218"/>
+      <c r="C4" s="219"/>
+      <c r="D4" s="219"/>
+      <c r="E4" s="219"/>
+      <c r="F4" s="219"/>
       <c r="G4" s="66"/>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
@@ -7437,7 +7437,7 @@
       <c r="BE8" s="174" t="s">
         <v>87</v>
       </c>
-      <c r="BF8" s="222" t="s">
+      <c r="BF8" s="210" t="s">
         <v>265</v>
       </c>
       <c r="BG8" s="200" t="s">
@@ -10003,13 +10003,13 @@
   <sheetData>
     <row r="1" spans="1:100" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="27"/>
-      <c r="B1" s="214" t="s">
+      <c r="B1" s="215" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="215"/>
-      <c r="D1" s="215"/>
-      <c r="E1" s="215"/>
-      <c r="F1" s="215"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
       <c r="G1" s="24"/>
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
@@ -10103,13 +10103,13 @@
     </row>
     <row r="3" spans="1:100" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
-      <c r="B3" s="216" t="s">
+      <c r="B3" s="217" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="215"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="215"/>
-      <c r="F3" s="215"/>
+      <c r="C3" s="216"/>
+      <c r="D3" s="216"/>
+      <c r="E3" s="216"/>
+      <c r="F3" s="216"/>
       <c r="G3" s="30"/>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
@@ -10163,13 +10163,13 @@
     </row>
     <row r="4" spans="1:100" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
-      <c r="B4" s="217" t="s">
+      <c r="B4" s="218" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="218"/>
-      <c r="D4" s="218"/>
-      <c r="E4" s="218"/>
-      <c r="F4" s="218"/>
+      <c r="C4" s="219"/>
+      <c r="D4" s="219"/>
+      <c r="E4" s="219"/>
+      <c r="F4" s="219"/>
       <c r="G4" s="66"/>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
@@ -10582,7 +10582,7 @@
       <c r="AW8" s="127" t="s">
         <v>87</v>
       </c>
-      <c r="AX8" s="222" t="s">
+      <c r="AX8" s="210" t="s">
         <v>265</v>
       </c>
       <c r="AY8" s="200" t="s">
@@ -14339,11 +14339,11 @@
       <c r="C28" s="184" t="s">
         <v>177</v>
       </c>
-      <c r="E28" s="219" t="str">
+      <c r="E28" s="220" t="str">
         <f>+C28&amp;C4&amp;C3&amp;C4&amp;C25&amp;","&amp;C4&amp;C2&amp;C4&amp;C25&amp;")"</f>
         <v>hoja.Range("T" &amp; sep +9,"V" &amp; sep +9)</v>
       </c>
-      <c r="F28" s="219"/>
+      <c r="F28" s="220"/>
       <c r="G28" t="s">
         <v>174</v>
       </c>
@@ -14429,15 +14429,15 @@
       <c r="B3" s="135" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="220"/>
-      <c r="D3" s="221"/>
+      <c r="C3" s="221"/>
+      <c r="D3" s="222"/>
       <c r="E3" s="136"/>
       <c r="F3" s="135" t="s">
         <v>67</v>
       </c>
       <c r="G3" s="137"/>
-      <c r="H3" s="220"/>
-      <c r="I3" s="221"/>
+      <c r="H3" s="221"/>
+      <c r="I3" s="222"/>
       <c r="J3" s="152"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>